<commit_message>
residue cal finished -  solid, liquid, inhalant, patch
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="243">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -833,6 +833,15 @@
   </si>
   <si>
     <t>Actual  L4 Train</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Select Type:</t>
+  </si>
+  <si>
+    <t>P5</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="427">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2542,6 +2551,13 @@
     <xf numFmtId="0" fontId="159" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="160" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="161" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2690,9 +2706,6 @@
     <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5112,15 +5125,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="403" t="s">
+      <c r="F1" s="406" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
-      <c r="J1" s="403"/>
-      <c r="K1" s="403"/>
-      <c r="L1" s="403"/>
+      <c r="G1" s="406"/>
+      <c r="H1" s="406"/>
+      <c r="I1" s="406"/>
+      <c r="J1" s="406"/>
+      <c r="K1" s="406"/>
+      <c r="L1" s="406"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -5209,22 +5222,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="404" t="s">
+      <c r="D6" s="407" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="405"/>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
-      <c r="H6" s="406"/>
+      <c r="E6" s="408"/>
+      <c r="F6" s="408"/>
+      <c r="G6" s="408"/>
+      <c r="H6" s="409"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="404" t="s">
+      <c r="M6" s="407" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="405"/>
-      <c r="O6" s="405"/>
-      <c r="P6" s="405"/>
-      <c r="Q6" s="406"/>
+      <c r="N6" s="408"/>
+      <c r="O6" s="408"/>
+      <c r="P6" s="408"/>
+      <c r="Q6" s="409"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -5242,10 +5255,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="407" t="s">
+      <c r="F7" s="410" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="408"/>
+      <c r="G7" s="411"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -5268,10 +5281,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="407" t="s">
+      <c r="P7" s="410" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="408"/>
+      <c r="Q7" s="411"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -5348,7 +5361,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="395" t="s">
+      <c r="B9" s="398" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5382,33 +5395,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="386">
+      <c r="M9" s="389">
         <v>20</v>
       </c>
-      <c r="N9" s="398" t="s">
+      <c r="N9" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="386">
+      <c r="O9" s="389">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="386">
+      <c r="P9" s="389">
         <v>3</v>
       </c>
-      <c r="Q9" s="386">
+      <c r="Q9" s="389">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="386">
+      <c r="R9" s="389">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="386"/>
-      <c r="T9" s="389">
+      <c r="S9" s="389"/>
+      <c r="T9" s="392">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="386">
+      <c r="U9" s="389">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -5433,7 +5446,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="396"/>
+      <c r="B10" s="399"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -5465,15 +5478,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="387"/>
-      <c r="N10" s="399"/>
-      <c r="O10" s="387"/>
-      <c r="P10" s="387"/>
-      <c r="Q10" s="387"/>
-      <c r="R10" s="387"/>
-      <c r="S10" s="387"/>
-      <c r="T10" s="390"/>
-      <c r="U10" s="387"/>
+      <c r="M10" s="390"/>
+      <c r="N10" s="402"/>
+      <c r="O10" s="390"/>
+      <c r="P10" s="390"/>
+      <c r="Q10" s="390"/>
+      <c r="R10" s="390"/>
+      <c r="S10" s="390"/>
+      <c r="T10" s="393"/>
+      <c r="U10" s="390"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -5481,10 +5494,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="386" t="s">
+      <c r="A11" s="389" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="396"/>
+      <c r="B11" s="399"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -5495,15 +5508,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="387"/>
-      <c r="N11" s="399"/>
-      <c r="O11" s="387"/>
-      <c r="P11" s="387"/>
-      <c r="Q11" s="387"/>
-      <c r="R11" s="387"/>
-      <c r="S11" s="387"/>
-      <c r="T11" s="390"/>
-      <c r="U11" s="387"/>
+      <c r="M11" s="390"/>
+      <c r="N11" s="402"/>
+      <c r="O11" s="390"/>
+      <c r="P11" s="390"/>
+      <c r="Q11" s="390"/>
+      <c r="R11" s="390"/>
+      <c r="S11" s="390"/>
+      <c r="T11" s="393"/>
+      <c r="U11" s="390"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -5522,8 +5535,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="388"/>
-      <c r="B12" s="397"/>
+      <c r="A12" s="391"/>
+      <c r="B12" s="400"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -5534,15 +5547,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="388"/>
-      <c r="N12" s="400"/>
-      <c r="O12" s="388"/>
-      <c r="P12" s="388"/>
-      <c r="Q12" s="388"/>
-      <c r="R12" s="388"/>
-      <c r="S12" s="388"/>
-      <c r="T12" s="391"/>
-      <c r="U12" s="388"/>
+      <c r="M12" s="391"/>
+      <c r="N12" s="403"/>
+      <c r="O12" s="391"/>
+      <c r="P12" s="391"/>
+      <c r="Q12" s="391"/>
+      <c r="R12" s="391"/>
+      <c r="S12" s="391"/>
+      <c r="T12" s="394"/>
+      <c r="U12" s="391"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -5558,7 +5571,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="395" t="s">
+      <c r="B13" s="398" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5592,33 +5605,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="386">
+      <c r="M13" s="389">
         <v>80</v>
       </c>
-      <c r="N13" s="398" t="s">
+      <c r="N13" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="386">
+      <c r="O13" s="389">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="386">
+      <c r="P13" s="389">
         <v>2</v>
       </c>
-      <c r="Q13" s="386">
+      <c r="Q13" s="389">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="386">
+      <c r="R13" s="389">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="386"/>
-      <c r="T13" s="389">
+      <c r="S13" s="389"/>
+      <c r="T13" s="392">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="386">
+      <c r="U13" s="389">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -5641,7 +5654,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="396"/>
+      <c r="B14" s="399"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -5673,15 +5686,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="387"/>
-      <c r="N14" s="399"/>
-      <c r="O14" s="387"/>
-      <c r="P14" s="387"/>
-      <c r="Q14" s="387"/>
-      <c r="R14" s="387"/>
-      <c r="S14" s="387"/>
-      <c r="T14" s="390"/>
-      <c r="U14" s="387"/>
+      <c r="M14" s="390"/>
+      <c r="N14" s="402"/>
+      <c r="O14" s="390"/>
+      <c r="P14" s="390"/>
+      <c r="Q14" s="390"/>
+      <c r="R14" s="390"/>
+      <c r="S14" s="390"/>
+      <c r="T14" s="393"/>
+      <c r="U14" s="390"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -5689,10 +5702,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="401" t="s">
+      <c r="A15" s="404" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="396"/>
+      <c r="B15" s="399"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -5703,15 +5716,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="387"/>
-      <c r="N15" s="399"/>
-      <c r="O15" s="387"/>
-      <c r="P15" s="387"/>
-      <c r="Q15" s="387"/>
-      <c r="R15" s="387"/>
-      <c r="S15" s="387"/>
-      <c r="T15" s="390"/>
-      <c r="U15" s="387"/>
+      <c r="M15" s="390"/>
+      <c r="N15" s="402"/>
+      <c r="O15" s="390"/>
+      <c r="P15" s="390"/>
+      <c r="Q15" s="390"/>
+      <c r="R15" s="390"/>
+      <c r="S15" s="390"/>
+      <c r="T15" s="393"/>
+      <c r="U15" s="390"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -5721,8 +5734,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="402"/>
-      <c r="B16" s="397"/>
+      <c r="A16" s="405"/>
+      <c r="B16" s="400"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -5733,15 +5746,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="388"/>
-      <c r="N16" s="400"/>
-      <c r="O16" s="388"/>
-      <c r="P16" s="388"/>
-      <c r="Q16" s="388"/>
-      <c r="R16" s="388"/>
-      <c r="S16" s="388"/>
-      <c r="T16" s="391"/>
-      <c r="U16" s="388"/>
+      <c r="M16" s="391"/>
+      <c r="N16" s="403"/>
+      <c r="O16" s="391"/>
+      <c r="P16" s="391"/>
+      <c r="Q16" s="391"/>
+      <c r="R16" s="391"/>
+      <c r="S16" s="391"/>
+      <c r="T16" s="394"/>
+      <c r="U16" s="391"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -5752,7 +5765,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="395" t="s">
+      <c r="B17" s="398" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5786,33 +5799,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="386">
+      <c r="M17" s="389">
         <v>70</v>
       </c>
-      <c r="N17" s="398" t="s">
+      <c r="N17" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="386">
+      <c r="O17" s="389">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="386">
+      <c r="P17" s="389">
         <v>2</v>
       </c>
-      <c r="Q17" s="386">
+      <c r="Q17" s="389">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="386">
+      <c r="R17" s="389">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="386"/>
-      <c r="T17" s="389">
+      <c r="S17" s="389"/>
+      <c r="T17" s="392">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="386">
+      <c r="U17" s="389">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -5831,7 +5844,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="396"/>
+      <c r="B18" s="399"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -5863,24 +5876,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="387"/>
-      <c r="N18" s="399"/>
-      <c r="O18" s="387"/>
-      <c r="P18" s="387"/>
-      <c r="Q18" s="387"/>
-      <c r="R18" s="387"/>
-      <c r="S18" s="387"/>
-      <c r="T18" s="390"/>
-      <c r="U18" s="387"/>
+      <c r="M18" s="390"/>
+      <c r="N18" s="402"/>
+      <c r="O18" s="390"/>
+      <c r="P18" s="390"/>
+      <c r="Q18" s="390"/>
+      <c r="R18" s="390"/>
+      <c r="S18" s="390"/>
+      <c r="T18" s="393"/>
+      <c r="U18" s="390"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="386" t="s">
+      <c r="A19" s="389" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="396"/>
+      <c r="B19" s="399"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -5891,22 +5904,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="387"/>
-      <c r="N19" s="399"/>
-      <c r="O19" s="387"/>
-      <c r="P19" s="387"/>
-      <c r="Q19" s="387"/>
-      <c r="R19" s="387"/>
-      <c r="S19" s="387"/>
-      <c r="T19" s="390"/>
-      <c r="U19" s="387"/>
+      <c r="M19" s="390"/>
+      <c r="N19" s="402"/>
+      <c r="O19" s="390"/>
+      <c r="P19" s="390"/>
+      <c r="Q19" s="390"/>
+      <c r="R19" s="390"/>
+      <c r="S19" s="390"/>
+      <c r="T19" s="393"/>
+      <c r="U19" s="390"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="388"/>
-      <c r="B20" s="397"/>
+      <c r="A20" s="391"/>
+      <c r="B20" s="400"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -5917,15 +5930,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="388"/>
-      <c r="N20" s="400"/>
-      <c r="O20" s="388"/>
-      <c r="P20" s="388"/>
-      <c r="Q20" s="388"/>
-      <c r="R20" s="388"/>
-      <c r="S20" s="388"/>
-      <c r="T20" s="391"/>
-      <c r="U20" s="388"/>
+      <c r="M20" s="391"/>
+      <c r="N20" s="403"/>
+      <c r="O20" s="391"/>
+      <c r="P20" s="391"/>
+      <c r="Q20" s="391"/>
+      <c r="R20" s="391"/>
+      <c r="S20" s="391"/>
+      <c r="T20" s="394"/>
+      <c r="U20" s="391"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -5934,7 +5947,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="395" t="s">
+      <c r="B21" s="398" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5968,33 +5981,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="386">
+      <c r="M21" s="389">
         <v>60</v>
       </c>
-      <c r="N21" s="398" t="s">
+      <c r="N21" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="386">
+      <c r="O21" s="389">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="386">
+      <c r="P21" s="389">
         <v>3</v>
       </c>
-      <c r="Q21" s="386">
+      <c r="Q21" s="389">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="386">
+      <c r="R21" s="389">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="386"/>
-      <c r="T21" s="389">
+      <c r="S21" s="389"/>
+      <c r="T21" s="392">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="386">
+      <c r="U21" s="389">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -6011,7 +6024,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="396"/>
+      <c r="B22" s="399"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -6043,24 +6056,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="387"/>
-      <c r="N22" s="399"/>
-      <c r="O22" s="387"/>
-      <c r="P22" s="387"/>
-      <c r="Q22" s="387"/>
-      <c r="R22" s="387"/>
-      <c r="S22" s="387"/>
-      <c r="T22" s="390"/>
-      <c r="U22" s="387"/>
+      <c r="M22" s="390"/>
+      <c r="N22" s="402"/>
+      <c r="O22" s="390"/>
+      <c r="P22" s="390"/>
+      <c r="Q22" s="390"/>
+      <c r="R22" s="390"/>
+      <c r="S22" s="390"/>
+      <c r="T22" s="393"/>
+      <c r="U22" s="390"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="392" t="s">
+      <c r="A23" s="395" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="396"/>
+      <c r="B23" s="399"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -6071,22 +6084,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="387"/>
-      <c r="N23" s="399"/>
-      <c r="O23" s="387"/>
-      <c r="P23" s="387"/>
-      <c r="Q23" s="387"/>
-      <c r="R23" s="387"/>
-      <c r="S23" s="387"/>
-      <c r="T23" s="390"/>
-      <c r="U23" s="387"/>
+      <c r="M23" s="390"/>
+      <c r="N23" s="402"/>
+      <c r="O23" s="390"/>
+      <c r="P23" s="390"/>
+      <c r="Q23" s="390"/>
+      <c r="R23" s="390"/>
+      <c r="S23" s="390"/>
+      <c r="T23" s="393"/>
+      <c r="U23" s="390"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="393"/>
-      <c r="B24" s="397"/>
+      <c r="A24" s="396"/>
+      <c r="B24" s="400"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -6097,15 +6110,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="388"/>
-      <c r="N24" s="400"/>
-      <c r="O24" s="388"/>
-      <c r="P24" s="388"/>
-      <c r="Q24" s="388"/>
-      <c r="R24" s="388"/>
-      <c r="S24" s="388"/>
-      <c r="T24" s="391"/>
-      <c r="U24" s="388"/>
+      <c r="M24" s="391"/>
+      <c r="N24" s="403"/>
+      <c r="O24" s="391"/>
+      <c r="P24" s="391"/>
+      <c r="Q24" s="391"/>
+      <c r="R24" s="391"/>
+      <c r="S24" s="391"/>
+      <c r="T24" s="394"/>
+      <c r="U24" s="391"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -6131,13 +6144,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="394" t="s">
+      <c r="H27" s="397" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="394"/>
-      <c r="J27" s="394"/>
-      <c r="K27" s="394"/>
-      <c r="L27" s="394"/>
+      <c r="I27" s="397"/>
+      <c r="J27" s="397"/>
+      <c r="K27" s="397"/>
+      <c r="L27" s="397"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -6417,19 +6430,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="384" t="s">
+      <c r="D40" s="387" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="384"/>
-      <c r="F40" s="384"/>
-      <c r="G40" s="384"/>
-      <c r="H40" s="384"/>
-      <c r="I40" s="384" t="s">
+      <c r="E40" s="387"/>
+      <c r="F40" s="387"/>
+      <c r="G40" s="387"/>
+      <c r="H40" s="387"/>
+      <c r="I40" s="387" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="384"/>
-      <c r="K40" s="384"/>
-      <c r="L40" s="384"/>
+      <c r="J40" s="387"/>
+      <c r="K40" s="387"/>
+      <c r="L40" s="387"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -6553,7 +6566,7 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="379" t="s">
+      <c r="B42" s="382" t="s">
         <v>226</v>
       </c>
       <c r="C42" s="190"/>
@@ -6561,17 +6574,17 @@
       <c r="E42" s="111"/>
       <c r="F42" s="189"/>
       <c r="G42" s="189"/>
-      <c r="H42" s="380">
+      <c r="H42" s="383">
         <v>3.095975611358881E-3</v>
       </c>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="189"/>
       <c r="L42" s="189"/>
-      <c r="M42" s="380">
+      <c r="M42" s="383">
         <v>1</v>
       </c>
-      <c r="N42" s="385" t="s">
+      <c r="N42" s="388" t="s">
         <v>59</v>
       </c>
       <c r="P42" s="91"/>
@@ -6619,7 +6632,7 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="379"/>
+      <c r="B43" s="382"/>
       <c r="C43" s="190" t="s">
         <v>220</v>
       </c>
@@ -6635,7 +6648,7 @@
       <c r="G43" s="103">
         <v>97.126746422628088</v>
       </c>
-      <c r="H43" s="380"/>
+      <c r="H43" s="383"/>
       <c r="I43" s="111">
         <v>1</v>
       </c>
@@ -6648,8 +6661,8 @@
       <c r="L43" s="103">
         <v>1</v>
       </c>
-      <c r="M43" s="380"/>
-      <c r="N43" s="380"/>
+      <c r="M43" s="383"/>
+      <c r="N43" s="383"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -6695,7 +6708,7 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="379"/>
+      <c r="B44" s="382"/>
       <c r="C44" s="190" t="s">
         <v>218</v>
       </c>
@@ -6711,7 +6724,7 @@
       <c r="G44" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H44" s="380"/>
+      <c r="H44" s="383"/>
       <c r="I44" s="111">
         <v>1</v>
       </c>
@@ -6724,8 +6737,8 @@
       <c r="L44" s="189">
         <v>1</v>
       </c>
-      <c r="M44" s="380"/>
-      <c r="N44" s="380"/>
+      <c r="M44" s="383"/>
+      <c r="N44" s="383"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -6771,7 +6784,7 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="379"/>
+      <c r="B45" s="382"/>
       <c r="C45" s="190" t="s">
         <v>219</v>
       </c>
@@ -6787,7 +6800,7 @@
       <c r="G45" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H45" s="380"/>
+      <c r="H45" s="383"/>
       <c r="I45" s="111">
         <v>1</v>
       </c>
@@ -6800,8 +6813,8 @@
       <c r="L45" s="189">
         <v>1</v>
       </c>
-      <c r="M45" s="380"/>
-      <c r="N45" s="380"/>
+      <c r="M45" s="383"/>
+      <c r="N45" s="383"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -6847,19 +6860,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="379"/>
+      <c r="B46" s="382"/>
       <c r="C46" s="190"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="189"/>
       <c r="G46" s="189"/>
-      <c r="H46" s="380"/>
+      <c r="H46" s="383"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="189"/>
       <c r="L46" s="189"/>
-      <c r="M46" s="380"/>
-      <c r="N46" s="381"/>
+      <c r="M46" s="383"/>
+      <c r="N46" s="384"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -6905,19 +6918,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="379"/>
+      <c r="B47" s="382"/>
       <c r="C47" s="190"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="380"/>
+      <c r="H47" s="383"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="380"/>
-      <c r="N47" s="382"/>
+      <c r="M47" s="383"/>
+      <c r="N47" s="385"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -6965,19 +6978,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="379"/>
+      <c r="B48" s="382"/>
       <c r="C48" s="190"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="380"/>
+      <c r="H48" s="383"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="380"/>
-      <c r="N48" s="382"/>
+      <c r="M48" s="383"/>
+      <c r="N48" s="385"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -7025,19 +7038,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="379"/>
+      <c r="B49" s="382"/>
       <c r="C49" s="190"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="380"/>
+      <c r="H49" s="383"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="380"/>
-      <c r="N49" s="382"/>
+      <c r="M49" s="383"/>
+      <c r="N49" s="385"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -7085,19 +7098,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="374"/>
+      <c r="B50" s="377"/>
       <c r="C50" s="191"/>
       <c r="D50" s="187"/>
       <c r="E50" s="187"/>
       <c r="F50" s="187"/>
       <c r="G50" s="187"/>
-      <c r="H50" s="375"/>
+      <c r="H50" s="378"/>
       <c r="I50" s="187"/>
       <c r="J50" s="187"/>
       <c r="K50" s="187"/>
       <c r="L50" s="187"/>
-      <c r="M50" s="375"/>
-      <c r="N50" s="383"/>
+      <c r="M50" s="378"/>
+      <c r="N50" s="386"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -7118,19 +7131,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="374"/>
+      <c r="B51" s="377"/>
       <c r="C51" s="191"/>
       <c r="D51" s="187"/>
       <c r="E51" s="187"/>
       <c r="F51" s="187"/>
       <c r="G51" s="187"/>
-      <c r="H51" s="375"/>
+      <c r="H51" s="378"/>
       <c r="I51" s="187"/>
       <c r="J51" s="187"/>
       <c r="K51" s="187"/>
       <c r="L51" s="187"/>
-      <c r="M51" s="375"/>
-      <c r="N51" s="377"/>
+      <c r="M51" s="378"/>
+      <c r="N51" s="380"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -7161,19 +7174,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="374"/>
+      <c r="B52" s="377"/>
       <c r="C52" s="191"/>
       <c r="D52" s="187"/>
       <c r="E52" s="187"/>
       <c r="F52" s="187"/>
       <c r="G52" s="187"/>
-      <c r="H52" s="375"/>
+      <c r="H52" s="378"/>
       <c r="I52" s="187"/>
       <c r="J52" s="187"/>
       <c r="K52" s="187"/>
       <c r="L52" s="187"/>
-      <c r="M52" s="375"/>
-      <c r="N52" s="377"/>
+      <c r="M52" s="378"/>
+      <c r="N52" s="380"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -7237,19 +7250,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="374"/>
+      <c r="B53" s="377"/>
       <c r="C53" s="191"/>
       <c r="D53" s="187"/>
       <c r="E53" s="187"/>
       <c r="F53" s="187"/>
       <c r="G53" s="187"/>
-      <c r="H53" s="375"/>
+      <c r="H53" s="378"/>
       <c r="I53" s="187"/>
       <c r="J53" s="187"/>
       <c r="K53" s="187"/>
       <c r="L53" s="187"/>
-      <c r="M53" s="375"/>
-      <c r="N53" s="377"/>
+      <c r="M53" s="378"/>
+      <c r="N53" s="380"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -7298,19 +7311,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="374"/>
+      <c r="B54" s="377"/>
       <c r="C54" s="191"/>
       <c r="D54" s="187"/>
       <c r="E54" s="187"/>
       <c r="F54" s="187"/>
       <c r="G54" s="187"/>
-      <c r="H54" s="375"/>
+      <c r="H54" s="378"/>
       <c r="I54" s="187"/>
       <c r="J54" s="187"/>
       <c r="K54" s="187"/>
       <c r="L54" s="187"/>
-      <c r="M54" s="375"/>
-      <c r="N54" s="376"/>
+      <c r="M54" s="378"/>
+      <c r="N54" s="379"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -7357,19 +7370,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="374"/>
+      <c r="B55" s="377"/>
       <c r="C55" s="191"/>
       <c r="D55" s="187"/>
       <c r="E55" s="187"/>
       <c r="F55" s="187"/>
       <c r="G55" s="187"/>
-      <c r="H55" s="375"/>
+      <c r="H55" s="378"/>
       <c r="I55" s="187"/>
       <c r="J55" s="187"/>
       <c r="K55" s="187"/>
       <c r="L55" s="187"/>
-      <c r="M55" s="375"/>
-      <c r="N55" s="377"/>
+      <c r="M55" s="378"/>
+      <c r="N55" s="380"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -7416,19 +7429,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="374"/>
+      <c r="B56" s="377"/>
       <c r="C56" s="191"/>
       <c r="D56" s="187"/>
       <c r="E56" s="187"/>
       <c r="F56" s="187"/>
       <c r="G56" s="187"/>
-      <c r="H56" s="375"/>
+      <c r="H56" s="378"/>
       <c r="I56" s="187"/>
       <c r="J56" s="187"/>
       <c r="K56" s="187"/>
       <c r="L56" s="187"/>
-      <c r="M56" s="375"/>
-      <c r="N56" s="377"/>
+      <c r="M56" s="378"/>
+      <c r="N56" s="380"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -7475,19 +7488,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="374"/>
+      <c r="B57" s="377"/>
       <c r="C57" s="191"/>
       <c r="D57" s="187"/>
       <c r="E57" s="187"/>
       <c r="F57" s="187"/>
       <c r="G57" s="187"/>
-      <c r="H57" s="375"/>
+      <c r="H57" s="378"/>
       <c r="I57" s="187"/>
       <c r="J57" s="187"/>
       <c r="K57" s="187"/>
       <c r="L57" s="187"/>
-      <c r="M57" s="375"/>
-      <c r="N57" s="377"/>
+      <c r="M57" s="378"/>
+      <c r="N57" s="380"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -7534,19 +7547,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="369"/>
+      <c r="B58" s="372"/>
       <c r="C58" s="185"/>
       <c r="D58" s="192"/>
       <c r="E58" s="192"/>
       <c r="F58" s="192"/>
       <c r="G58" s="192"/>
-      <c r="H58" s="370"/>
+      <c r="H58" s="373"/>
       <c r="I58" s="192"/>
       <c r="J58" s="192"/>
       <c r="K58" s="192"/>
       <c r="L58" s="192"/>
-      <c r="M58" s="370"/>
-      <c r="N58" s="378"/>
+      <c r="M58" s="373"/>
+      <c r="N58" s="381"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -7593,19 +7606,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="369"/>
+      <c r="B59" s="372"/>
       <c r="C59" s="185"/>
       <c r="D59" s="192"/>
       <c r="E59" s="192"/>
       <c r="F59" s="192"/>
       <c r="G59" s="192"/>
-      <c r="H59" s="370"/>
+      <c r="H59" s="373"/>
       <c r="I59" s="192"/>
       <c r="J59" s="192"/>
       <c r="K59" s="192"/>
       <c r="L59" s="192"/>
-      <c r="M59" s="370"/>
-      <c r="N59" s="372"/>
+      <c r="M59" s="373"/>
+      <c r="N59" s="375"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -7652,19 +7665,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="369"/>
+      <c r="B60" s="372"/>
       <c r="C60" s="185"/>
       <c r="D60" s="192"/>
       <c r="E60" s="192"/>
       <c r="F60" s="192"/>
       <c r="G60" s="192"/>
-      <c r="H60" s="370"/>
+      <c r="H60" s="373"/>
       <c r="I60" s="192"/>
       <c r="J60" s="192"/>
       <c r="K60" s="192"/>
       <c r="L60" s="192"/>
-      <c r="M60" s="370"/>
-      <c r="N60" s="372"/>
+      <c r="M60" s="373"/>
+      <c r="N60" s="375"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -7711,247 +7724,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="369"/>
+      <c r="B61" s="372"/>
       <c r="C61" s="185"/>
       <c r="D61" s="192"/>
       <c r="E61" s="192"/>
       <c r="F61" s="192"/>
       <c r="G61" s="192"/>
-      <c r="H61" s="370"/>
+      <c r="H61" s="373"/>
       <c r="I61" s="192"/>
       <c r="J61" s="192"/>
       <c r="K61" s="192"/>
       <c r="L61" s="192"/>
-      <c r="M61" s="370"/>
-      <c r="N61" s="372"/>
+      <c r="M61" s="373"/>
+      <c r="N61" s="375"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="369"/>
+      <c r="B62" s="372"/>
       <c r="C62" s="185"/>
       <c r="D62" s="192"/>
       <c r="E62" s="192"/>
       <c r="F62" s="192"/>
       <c r="G62" s="192"/>
-      <c r="H62" s="370"/>
+      <c r="H62" s="373"/>
       <c r="I62" s="192"/>
       <c r="J62" s="192"/>
       <c r="K62" s="192"/>
       <c r="L62" s="192"/>
-      <c r="M62" s="370"/>
-      <c r="N62" s="371"/>
+      <c r="M62" s="373"/>
+      <c r="N62" s="374"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="369"/>
+      <c r="B63" s="372"/>
       <c r="C63" s="185"/>
       <c r="D63" s="192"/>
       <c r="E63" s="192"/>
       <c r="F63" s="192"/>
       <c r="G63" s="192"/>
-      <c r="H63" s="370"/>
+      <c r="H63" s="373"/>
       <c r="I63" s="192"/>
       <c r="J63" s="192"/>
       <c r="K63" s="192"/>
       <c r="L63" s="192"/>
-      <c r="M63" s="370"/>
-      <c r="N63" s="372"/>
+      <c r="M63" s="373"/>
+      <c r="N63" s="375"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="369"/>
+      <c r="B64" s="372"/>
       <c r="C64" s="185"/>
       <c r="D64" s="192"/>
       <c r="E64" s="192"/>
       <c r="F64" s="192"/>
       <c r="G64" s="192"/>
-      <c r="H64" s="370"/>
+      <c r="H64" s="373"/>
       <c r="I64" s="192"/>
       <c r="J64" s="192"/>
       <c r="K64" s="192"/>
       <c r="L64" s="192"/>
-      <c r="M64" s="370"/>
-      <c r="N64" s="372"/>
+      <c r="M64" s="373"/>
+      <c r="N64" s="375"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="369"/>
+      <c r="B65" s="372"/>
       <c r="C65" s="185"/>
       <c r="D65" s="192"/>
       <c r="E65" s="192"/>
       <c r="F65" s="192"/>
       <c r="G65" s="192"/>
-      <c r="H65" s="370"/>
+      <c r="H65" s="373"/>
       <c r="I65" s="192"/>
       <c r="J65" s="192"/>
       <c r="K65" s="192"/>
       <c r="L65" s="192"/>
-      <c r="M65" s="370"/>
-      <c r="N65" s="372"/>
+      <c r="M65" s="373"/>
+      <c r="N65" s="375"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="365"/>
+      <c r="B66" s="368"/>
       <c r="C66" s="186"/>
       <c r="D66" s="188"/>
       <c r="E66" s="188"/>
       <c r="F66" s="188"/>
       <c r="G66" s="188"/>
-      <c r="H66" s="366"/>
+      <c r="H66" s="369"/>
       <c r="I66" s="188"/>
       <c r="J66" s="188"/>
       <c r="K66" s="188"/>
       <c r="L66" s="188"/>
-      <c r="M66" s="366"/>
-      <c r="N66" s="373"/>
+      <c r="M66" s="369"/>
+      <c r="N66" s="376"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="365"/>
+      <c r="B67" s="368"/>
       <c r="C67" s="186"/>
       <c r="D67" s="188"/>
       <c r="E67" s="188"/>
       <c r="F67" s="188"/>
       <c r="G67" s="188"/>
-      <c r="H67" s="366"/>
+      <c r="H67" s="369"/>
       <c r="I67" s="188"/>
       <c r="J67" s="188"/>
       <c r="K67" s="188"/>
       <c r="L67" s="188"/>
-      <c r="M67" s="366"/>
-      <c r="N67" s="368"/>
+      <c r="M67" s="369"/>
+      <c r="N67" s="371"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="365"/>
+      <c r="B68" s="368"/>
       <c r="C68" s="186"/>
       <c r="D68" s="188"/>
       <c r="E68" s="188"/>
       <c r="F68" s="188"/>
       <c r="G68" s="188"/>
-      <c r="H68" s="366"/>
+      <c r="H68" s="369"/>
       <c r="I68" s="188"/>
       <c r="J68" s="188"/>
       <c r="K68" s="188"/>
       <c r="L68" s="188"/>
-      <c r="M68" s="366"/>
-      <c r="N68" s="368"/>
+      <c r="M68" s="369"/>
+      <c r="N68" s="371"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="365"/>
+      <c r="B69" s="368"/>
       <c r="C69" s="186"/>
       <c r="D69" s="188"/>
       <c r="E69" s="188"/>
       <c r="F69" s="188"/>
       <c r="G69" s="188"/>
-      <c r="H69" s="366"/>
+      <c r="H69" s="369"/>
       <c r="I69" s="188"/>
       <c r="J69" s="188"/>
       <c r="K69" s="188"/>
       <c r="L69" s="188"/>
-      <c r="M69" s="366"/>
-      <c r="N69" s="368"/>
+      <c r="M69" s="369"/>
+      <c r="N69" s="371"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="365"/>
+      <c r="B70" s="368"/>
       <c r="C70" s="186"/>
       <c r="D70" s="188"/>
       <c r="E70" s="188"/>
       <c r="F70" s="188"/>
       <c r="G70" s="188"/>
-      <c r="H70" s="366"/>
+      <c r="H70" s="369"/>
       <c r="I70" s="188"/>
       <c r="J70" s="188"/>
       <c r="K70" s="188"/>
       <c r="L70" s="188"/>
-      <c r="M70" s="366"/>
-      <c r="N70" s="367"/>
+      <c r="M70" s="369"/>
+      <c r="N70" s="370"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="365"/>
+      <c r="B71" s="368"/>
       <c r="C71" s="186"/>
       <c r="D71" s="188"/>
       <c r="E71" s="188"/>
       <c r="F71" s="188"/>
       <c r="G71" s="188"/>
-      <c r="H71" s="366"/>
+      <c r="H71" s="369"/>
       <c r="I71" s="188"/>
       <c r="J71" s="188"/>
       <c r="K71" s="188"/>
       <c r="L71" s="188"/>
-      <c r="M71" s="366"/>
-      <c r="N71" s="368"/>
+      <c r="M71" s="369"/>
+      <c r="N71" s="371"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="365"/>
+      <c r="B72" s="368"/>
       <c r="C72" s="186"/>
       <c r="D72" s="188"/>
       <c r="E72" s="188"/>
       <c r="F72" s="188"/>
       <c r="G72" s="188"/>
-      <c r="H72" s="366"/>
+      <c r="H72" s="369"/>
       <c r="I72" s="188"/>
       <c r="J72" s="188"/>
       <c r="K72" s="188"/>
       <c r="L72" s="188"/>
-      <c r="M72" s="366"/>
-      <c r="N72" s="368"/>
+      <c r="M72" s="369"/>
+      <c r="N72" s="371"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="365"/>
+      <c r="B73" s="368"/>
       <c r="C73" s="186"/>
       <c r="D73" s="188"/>
       <c r="E73" s="188"/>
       <c r="F73" s="188"/>
       <c r="G73" s="188"/>
-      <c r="H73" s="366"/>
+      <c r="H73" s="369"/>
       <c r="I73" s="188"/>
       <c r="J73" s="188"/>
       <c r="K73" s="188"/>
       <c r="L73" s="188"/>
-      <c r="M73" s="366"/>
-      <c r="N73" s="368"/>
+      <c r="M73" s="369"/>
+      <c r="N73" s="371"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>
@@ -9605,12 +9618,12 @@
   <dimension ref="A1:AU434"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27" style="22" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="33.5703125" style="22" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.85546875" style="22" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="36.140625" style="22" customWidth="1" collapsed="1"/>
@@ -9653,15 +9666,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="403" t="s">
+      <c r="F1" s="406" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
-      <c r="J1" s="403"/>
-      <c r="K1" s="403"/>
-      <c r="L1" s="403"/>
+      <c r="G1" s="406"/>
+      <c r="H1" s="406"/>
+      <c r="I1" s="406"/>
+      <c r="J1" s="406"/>
+      <c r="K1" s="406"/>
+      <c r="L1" s="406"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -9710,22 +9723,22 @@
       <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="404" t="s">
+      <c r="D6" s="407" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="405"/>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
-      <c r="H6" s="406"/>
+      <c r="E6" s="408"/>
+      <c r="F6" s="408"/>
+      <c r="G6" s="408"/>
+      <c r="H6" s="409"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="404" t="s">
+      <c r="M6" s="407" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="405"/>
-      <c r="O6" s="405"/>
-      <c r="P6" s="405"/>
-      <c r="Q6" s="406"/>
+      <c r="N6" s="408"/>
+      <c r="O6" s="408"/>
+      <c r="P6" s="408"/>
+      <c r="Q6" s="409"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -9743,10 +9756,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="407" t="s">
+      <c r="F7" s="410" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="408"/>
+      <c r="G7" s="411"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -9769,10 +9782,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="407" t="s">
+      <c r="P7" s="410" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="408"/>
+      <c r="Q7" s="411"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -9840,7 +9853,7 @@
     </row>
     <row r="9" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="39"/>
-      <c r="B9" s="395"/>
+      <c r="B9" s="398"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
       <c r="E9" s="40"/>
@@ -9851,15 +9864,15 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="42"/>
-      <c r="M9" s="386"/>
-      <c r="N9" s="398"/>
-      <c r="O9" s="386"/>
-      <c r="P9" s="386"/>
-      <c r="Q9" s="386"/>
-      <c r="R9" s="386"/>
-      <c r="S9" s="386"/>
-      <c r="T9" s="389"/>
-      <c r="U9" s="386"/>
+      <c r="M9" s="389"/>
+      <c r="N9" s="401"/>
+      <c r="O9" s="389"/>
+      <c r="P9" s="389"/>
+      <c r="Q9" s="389"/>
+      <c r="R9" s="389"/>
+      <c r="S9" s="389"/>
+      <c r="T9" s="392"/>
+      <c r="U9" s="389"/>
       <c r="V9" s="41"/>
       <c r="W9" s="36"/>
       <c r="X9" s="36"/>
@@ -9869,7 +9882,7 @@
     </row>
     <row r="10" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
-      <c r="B10" s="396"/>
+      <c r="B10" s="399"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
@@ -9880,15 +9893,15 @@
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="42"/>
-      <c r="M10" s="387"/>
-      <c r="N10" s="399"/>
-      <c r="O10" s="387"/>
-      <c r="P10" s="387"/>
-      <c r="Q10" s="387"/>
-      <c r="R10" s="387"/>
-      <c r="S10" s="387"/>
-      <c r="T10" s="390"/>
-      <c r="U10" s="387"/>
+      <c r="M10" s="390"/>
+      <c r="N10" s="402"/>
+      <c r="O10" s="390"/>
+      <c r="P10" s="390"/>
+      <c r="Q10" s="390"/>
+      <c r="R10" s="390"/>
+      <c r="S10" s="390"/>
+      <c r="T10" s="393"/>
+      <c r="U10" s="390"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -9896,8 +9909,8 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="386"/>
-      <c r="B11" s="396"/>
+      <c r="A11" s="389"/>
+      <c r="B11" s="399"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -9908,15 +9921,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="387"/>
-      <c r="N11" s="399"/>
-      <c r="O11" s="387"/>
-      <c r="P11" s="387"/>
-      <c r="Q11" s="387"/>
-      <c r="R11" s="387"/>
-      <c r="S11" s="387"/>
-      <c r="T11" s="390"/>
-      <c r="U11" s="387"/>
+      <c r="M11" s="390"/>
+      <c r="N11" s="402"/>
+      <c r="O11" s="390"/>
+      <c r="P11" s="390"/>
+      <c r="Q11" s="390"/>
+      <c r="R11" s="390"/>
+      <c r="S11" s="390"/>
+      <c r="T11" s="393"/>
+      <c r="U11" s="390"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -9926,8 +9939,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="388"/>
-      <c r="B12" s="397"/>
+      <c r="A12" s="391"/>
+      <c r="B12" s="400"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -9938,15 +9951,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="388"/>
-      <c r="N12" s="400"/>
-      <c r="O12" s="388"/>
-      <c r="P12" s="388"/>
-      <c r="Q12" s="388"/>
-      <c r="R12" s="388"/>
-      <c r="S12" s="388"/>
-      <c r="T12" s="391"/>
-      <c r="U12" s="388"/>
+      <c r="M12" s="391"/>
+      <c r="N12" s="403"/>
+      <c r="O12" s="391"/>
+      <c r="P12" s="391"/>
+      <c r="Q12" s="391"/>
+      <c r="R12" s="391"/>
+      <c r="S12" s="391"/>
+      <c r="T12" s="394"/>
+      <c r="U12" s="391"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -9955,7 +9968,7 @@
     </row>
     <row r="13" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43"/>
-      <c r="B13" s="395"/>
+      <c r="B13" s="398"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
@@ -9966,15 +9979,15 @@
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="386"/>
-      <c r="N13" s="398"/>
-      <c r="O13" s="386"/>
-      <c r="P13" s="386"/>
-      <c r="Q13" s="386"/>
-      <c r="R13" s="386"/>
-      <c r="S13" s="386"/>
-      <c r="T13" s="389"/>
-      <c r="U13" s="386"/>
+      <c r="M13" s="389"/>
+      <c r="N13" s="401"/>
+      <c r="O13" s="389"/>
+      <c r="P13" s="389"/>
+      <c r="Q13" s="389"/>
+      <c r="R13" s="389"/>
+      <c r="S13" s="389"/>
+      <c r="T13" s="392"/>
+      <c r="U13" s="389"/>
       <c r="V13" s="41"/>
       <c r="W13" s="36"/>
       <c r="X13" s="36"/>
@@ -9983,7 +9996,7 @@
     </row>
     <row r="14" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44"/>
-      <c r="B14" s="396"/>
+      <c r="B14" s="399"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
@@ -9994,15 +10007,15 @@
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
       <c r="L14" s="42"/>
-      <c r="M14" s="387"/>
-      <c r="N14" s="399"/>
-      <c r="O14" s="387"/>
-      <c r="P14" s="387"/>
-      <c r="Q14" s="387"/>
-      <c r="R14" s="387"/>
-      <c r="S14" s="387"/>
-      <c r="T14" s="390"/>
-      <c r="U14" s="387"/>
+      <c r="M14" s="390"/>
+      <c r="N14" s="402"/>
+      <c r="O14" s="390"/>
+      <c r="P14" s="390"/>
+      <c r="Q14" s="390"/>
+      <c r="R14" s="390"/>
+      <c r="S14" s="390"/>
+      <c r="T14" s="393"/>
+      <c r="U14" s="390"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -10010,8 +10023,8 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="401"/>
-      <c r="B15" s="396"/>
+      <c r="A15" s="404"/>
+      <c r="B15" s="399"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -10022,15 +10035,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="387"/>
-      <c r="N15" s="399"/>
-      <c r="O15" s="387"/>
-      <c r="P15" s="387"/>
-      <c r="Q15" s="387"/>
-      <c r="R15" s="387"/>
-      <c r="S15" s="387"/>
-      <c r="T15" s="390"/>
-      <c r="U15" s="387"/>
+      <c r="M15" s="390"/>
+      <c r="N15" s="402"/>
+      <c r="O15" s="390"/>
+      <c r="P15" s="390"/>
+      <c r="Q15" s="390"/>
+      <c r="R15" s="390"/>
+      <c r="S15" s="390"/>
+      <c r="T15" s="393"/>
+      <c r="U15" s="390"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -10038,8 +10051,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="402"/>
-      <c r="B16" s="397"/>
+      <c r="A16" s="405"/>
+      <c r="B16" s="400"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -10050,15 +10063,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="388"/>
-      <c r="N16" s="400"/>
-      <c r="O16" s="388"/>
-      <c r="P16" s="388"/>
-      <c r="Q16" s="388"/>
-      <c r="R16" s="388"/>
-      <c r="S16" s="388"/>
-      <c r="T16" s="391"/>
-      <c r="U16" s="388"/>
+      <c r="M16" s="391"/>
+      <c r="N16" s="403"/>
+      <c r="O16" s="391"/>
+      <c r="P16" s="391"/>
+      <c r="Q16" s="391"/>
+      <c r="R16" s="391"/>
+      <c r="S16" s="391"/>
+      <c r="T16" s="394"/>
+      <c r="U16" s="391"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -10067,7 +10080,7 @@
     </row>
     <row r="17" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
-      <c r="B17" s="395"/>
+      <c r="B17" s="398"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="40"/>
@@ -10078,15 +10091,15 @@
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="386"/>
-      <c r="N17" s="398"/>
-      <c r="O17" s="386"/>
-      <c r="P17" s="386"/>
-      <c r="Q17" s="386"/>
-      <c r="R17" s="386"/>
-      <c r="S17" s="386"/>
-      <c r="T17" s="389"/>
-      <c r="U17" s="386"/>
+      <c r="M17" s="389"/>
+      <c r="N17" s="401"/>
+      <c r="O17" s="389"/>
+      <c r="P17" s="389"/>
+      <c r="Q17" s="389"/>
+      <c r="R17" s="389"/>
+      <c r="S17" s="389"/>
+      <c r="T17" s="392"/>
+      <c r="U17" s="389"/>
       <c r="V17" s="41"/>
       <c r="W17" s="36"/>
       <c r="X17" s="36"/>
@@ -10095,7 +10108,7 @@
     </row>
     <row r="18" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40"/>
-      <c r="B18" s="396"/>
+      <c r="B18" s="399"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
       <c r="E18" s="40"/>
@@ -10106,22 +10119,22 @@
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="387"/>
-      <c r="N18" s="399"/>
-      <c r="O18" s="387"/>
-      <c r="P18" s="387"/>
-      <c r="Q18" s="387"/>
-      <c r="R18" s="387"/>
-      <c r="S18" s="387"/>
-      <c r="T18" s="390"/>
-      <c r="U18" s="387"/>
+      <c r="M18" s="390"/>
+      <c r="N18" s="402"/>
+      <c r="O18" s="390"/>
+      <c r="P18" s="390"/>
+      <c r="Q18" s="390"/>
+      <c r="R18" s="390"/>
+      <c r="S18" s="390"/>
+      <c r="T18" s="393"/>
+      <c r="U18" s="390"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="386"/>
-      <c r="B19" s="396"/>
+      <c r="A19" s="389"/>
+      <c r="B19" s="399"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -10132,22 +10145,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="387"/>
-      <c r="N19" s="399"/>
-      <c r="O19" s="387"/>
-      <c r="P19" s="387"/>
-      <c r="Q19" s="387"/>
-      <c r="R19" s="387"/>
-      <c r="S19" s="387"/>
-      <c r="T19" s="390"/>
-      <c r="U19" s="387"/>
+      <c r="M19" s="390"/>
+      <c r="N19" s="402"/>
+      <c r="O19" s="390"/>
+      <c r="P19" s="390"/>
+      <c r="Q19" s="390"/>
+      <c r="R19" s="390"/>
+      <c r="S19" s="390"/>
+      <c r="T19" s="393"/>
+      <c r="U19" s="390"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="388"/>
-      <c r="B20" s="397"/>
+      <c r="A20" s="391"/>
+      <c r="B20" s="400"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -10158,22 +10171,22 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="388"/>
-      <c r="N20" s="400"/>
-      <c r="O20" s="388"/>
-      <c r="P20" s="388"/>
-      <c r="Q20" s="388"/>
-      <c r="R20" s="388"/>
-      <c r="S20" s="388"/>
-      <c r="T20" s="391"/>
-      <c r="U20" s="388"/>
+      <c r="M20" s="391"/>
+      <c r="N20" s="403"/>
+      <c r="O20" s="391"/>
+      <c r="P20" s="391"/>
+      <c r="Q20" s="391"/>
+      <c r="R20" s="391"/>
+      <c r="S20" s="391"/>
+      <c r="T20" s="394"/>
+      <c r="U20" s="391"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
     </row>
     <row r="21" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="39"/>
-      <c r="B21" s="395"/>
+      <c r="B21" s="398"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
@@ -10184,22 +10197,22 @@
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
       <c r="L21" s="42"/>
-      <c r="M21" s="386"/>
-      <c r="N21" s="398"/>
-      <c r="O21" s="386"/>
-      <c r="P21" s="386"/>
-      <c r="Q21" s="386"/>
-      <c r="R21" s="386"/>
-      <c r="S21" s="386"/>
-      <c r="T21" s="389"/>
-      <c r="U21" s="386"/>
+      <c r="M21" s="389"/>
+      <c r="N21" s="401"/>
+      <c r="O21" s="389"/>
+      <c r="P21" s="389"/>
+      <c r="Q21" s="389"/>
+      <c r="R21" s="389"/>
+      <c r="S21" s="389"/>
+      <c r="T21" s="392"/>
+      <c r="U21" s="389"/>
       <c r="V21" s="41"/>
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
     </row>
     <row r="22" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
-      <c r="B22" s="396"/>
+      <c r="B22" s="399"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
@@ -10210,22 +10223,22 @@
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
       <c r="L22" s="42"/>
-      <c r="M22" s="387"/>
-      <c r="N22" s="399"/>
-      <c r="O22" s="387"/>
-      <c r="P22" s="387"/>
-      <c r="Q22" s="387"/>
-      <c r="R22" s="387"/>
-      <c r="S22" s="387"/>
-      <c r="T22" s="390"/>
-      <c r="U22" s="387"/>
+      <c r="M22" s="390"/>
+      <c r="N22" s="402"/>
+      <c r="O22" s="390"/>
+      <c r="P22" s="390"/>
+      <c r="Q22" s="390"/>
+      <c r="R22" s="390"/>
+      <c r="S22" s="390"/>
+      <c r="T22" s="393"/>
+      <c r="U22" s="390"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="392"/>
-      <c r="B23" s="396"/>
+      <c r="A23" s="395"/>
+      <c r="B23" s="399"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -10236,22 +10249,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="387"/>
-      <c r="N23" s="399"/>
-      <c r="O23" s="387"/>
-      <c r="P23" s="387"/>
-      <c r="Q23" s="387"/>
-      <c r="R23" s="387"/>
-      <c r="S23" s="387"/>
-      <c r="T23" s="390"/>
-      <c r="U23" s="387"/>
+      <c r="M23" s="390"/>
+      <c r="N23" s="402"/>
+      <c r="O23" s="390"/>
+      <c r="P23" s="390"/>
+      <c r="Q23" s="390"/>
+      <c r="R23" s="390"/>
+      <c r="S23" s="390"/>
+      <c r="T23" s="393"/>
+      <c r="U23" s="390"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="393"/>
-      <c r="B24" s="397"/>
+      <c r="A24" s="396"/>
+      <c r="B24" s="400"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -10262,15 +10275,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="388"/>
-      <c r="N24" s="400"/>
-      <c r="O24" s="388"/>
-      <c r="P24" s="388"/>
-      <c r="Q24" s="388"/>
-      <c r="R24" s="388"/>
-      <c r="S24" s="388"/>
-      <c r="T24" s="391"/>
-      <c r="U24" s="388"/>
+      <c r="M24" s="391"/>
+      <c r="N24" s="403"/>
+      <c r="O24" s="391"/>
+      <c r="P24" s="391"/>
+      <c r="Q24" s="391"/>
+      <c r="R24" s="391"/>
+      <c r="S24" s="391"/>
+      <c r="T24" s="394"/>
+      <c r="U24" s="391"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -10576,36 +10589,42 @@
       <c r="AN39" s="23"/>
       <c r="AO39" s="23"/>
     </row>
-    <row r="40" spans="1:41" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:41" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="366" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40" s="367" t="s">
+        <v>240</v>
+      </c>
       <c r="D40" s="104"/>
       <c r="E40" s="105"/>
-      <c r="F40" s="410" t="s">
+      <c r="F40" s="413" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="411"/>
-      <c r="H40" s="411"/>
-      <c r="I40" s="412"/>
-      <c r="J40" s="413" t="s">
+      <c r="G40" s="414"/>
+      <c r="H40" s="414"/>
+      <c r="I40" s="415"/>
+      <c r="J40" s="416" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="414"/>
-      <c r="L40" s="414"/>
-      <c r="M40" s="415"/>
+      <c r="K40" s="417"/>
+      <c r="L40" s="417"/>
+      <c r="M40" s="418"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
       </c>
       <c r="P40" s="227"/>
-      <c r="Q40" s="409" t="s">
+      <c r="Q40" s="412" t="s">
         <v>234</v>
       </c>
-      <c r="R40" s="409"/>
-      <c r="S40" s="409"/>
-      <c r="T40" s="409"/>
-      <c r="U40" s="409"/>
-      <c r="V40" s="409"/>
-      <c r="W40" s="409"/>
-      <c r="X40" s="409"/>
-      <c r="Y40" s="409"/>
+      <c r="R40" s="412"/>
+      <c r="S40" s="412"/>
+      <c r="T40" s="412"/>
+      <c r="U40" s="412"/>
+      <c r="V40" s="412"/>
+      <c r="W40" s="412"/>
+      <c r="X40" s="412"/>
+      <c r="Y40" s="412"/>
       <c r="Z40" s="46"/>
       <c r="AA40" s="46"/>
       <c r="AB40" s="46"/>
@@ -10624,10 +10643,10 @@
       <c r="AO40" s="23"/>
     </row>
     <row r="41" spans="1:41" ht="75.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="424" t="s">
+      <c r="A41" s="365" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="424" t="s">
+      <c r="B41" s="365" t="s">
         <v>217</v>
       </c>
       <c r="D41" s="253" t="s">
@@ -10914,7 +10933,9 @@
     </row>
     <row r="46" spans="1:41" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="310"/>
-      <c r="B46" s="310"/>
+      <c r="B46" s="310" t="s">
+        <v>242</v>
+      </c>
       <c r="D46" s="34"/>
       <c r="E46" s="34"/>
       <c r="F46" s="286"/>
@@ -18338,9 +18359,12 @@
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">
       <formula1>"daily,week,month"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
+      <formula1>"Solid,Liquid,Inhalant,Patch,Topical"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18392,15 +18416,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="403" t="s">
+      <c r="F1" s="406" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
-      <c r="J1" s="403"/>
-      <c r="K1" s="403"/>
-      <c r="L1" s="403"/>
+      <c r="G1" s="406"/>
+      <c r="H1" s="406"/>
+      <c r="I1" s="406"/>
+      <c r="J1" s="406"/>
+      <c r="K1" s="406"/>
+      <c r="L1" s="406"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -18489,22 +18513,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="404" t="s">
+      <c r="D6" s="407" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="405"/>
-      <c r="F6" s="405"/>
-      <c r="G6" s="405"/>
-      <c r="H6" s="406"/>
+      <c r="E6" s="408"/>
+      <c r="F6" s="408"/>
+      <c r="G6" s="408"/>
+      <c r="H6" s="409"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="404" t="s">
+      <c r="M6" s="407" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="405"/>
-      <c r="O6" s="405"/>
-      <c r="P6" s="405"/>
-      <c r="Q6" s="406"/>
+      <c r="N6" s="408"/>
+      <c r="O6" s="408"/>
+      <c r="P6" s="408"/>
+      <c r="Q6" s="409"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -18522,10 +18546,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="407" t="s">
+      <c r="F7" s="410" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="408"/>
+      <c r="G7" s="411"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -18548,10 +18572,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="407" t="s">
+      <c r="P7" s="410" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="408"/>
+      <c r="Q7" s="411"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -18628,7 +18652,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="395" t="s">
+      <c r="B9" s="398" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -18662,33 +18686,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="386">
+      <c r="M9" s="389">
         <v>20</v>
       </c>
-      <c r="N9" s="398" t="s">
+      <c r="N9" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="386">
+      <c r="O9" s="389">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="386">
+      <c r="P9" s="389">
         <v>3</v>
       </c>
-      <c r="Q9" s="386">
+      <c r="Q9" s="389">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="386">
+      <c r="R9" s="389">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="386"/>
-      <c r="T9" s="389">
+      <c r="S9" s="389"/>
+      <c r="T9" s="392">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="386">
+      <c r="U9" s="389">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -18713,7 +18737,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="396"/>
+      <c r="B10" s="399"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -18745,15 +18769,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="387"/>
-      <c r="N10" s="399"/>
-      <c r="O10" s="387"/>
-      <c r="P10" s="387"/>
-      <c r="Q10" s="387"/>
-      <c r="R10" s="387"/>
-      <c r="S10" s="387"/>
-      <c r="T10" s="390"/>
-      <c r="U10" s="387"/>
+      <c r="M10" s="390"/>
+      <c r="N10" s="402"/>
+      <c r="O10" s="390"/>
+      <c r="P10" s="390"/>
+      <c r="Q10" s="390"/>
+      <c r="R10" s="390"/>
+      <c r="S10" s="390"/>
+      <c r="T10" s="393"/>
+      <c r="U10" s="390"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -18761,10 +18785,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="386" t="s">
+      <c r="A11" s="389" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="396"/>
+      <c r="B11" s="399"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -18775,15 +18799,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="387"/>
-      <c r="N11" s="399"/>
-      <c r="O11" s="387"/>
-      <c r="P11" s="387"/>
-      <c r="Q11" s="387"/>
-      <c r="R11" s="387"/>
-      <c r="S11" s="387"/>
-      <c r="T11" s="390"/>
-      <c r="U11" s="387"/>
+      <c r="M11" s="390"/>
+      <c r="N11" s="402"/>
+      <c r="O11" s="390"/>
+      <c r="P11" s="390"/>
+      <c r="Q11" s="390"/>
+      <c r="R11" s="390"/>
+      <c r="S11" s="390"/>
+      <c r="T11" s="393"/>
+      <c r="U11" s="390"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -18802,8 +18826,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="388"/>
-      <c r="B12" s="397"/>
+      <c r="A12" s="391"/>
+      <c r="B12" s="400"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -18814,15 +18838,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="388"/>
-      <c r="N12" s="400"/>
-      <c r="O12" s="388"/>
-      <c r="P12" s="388"/>
-      <c r="Q12" s="388"/>
-      <c r="R12" s="388"/>
-      <c r="S12" s="388"/>
-      <c r="T12" s="391"/>
-      <c r="U12" s="388"/>
+      <c r="M12" s="391"/>
+      <c r="N12" s="403"/>
+      <c r="O12" s="391"/>
+      <c r="P12" s="391"/>
+      <c r="Q12" s="391"/>
+      <c r="R12" s="391"/>
+      <c r="S12" s="391"/>
+      <c r="T12" s="394"/>
+      <c r="U12" s="391"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -18838,7 +18862,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="395" t="s">
+      <c r="B13" s="398" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -18872,33 +18896,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="386">
+      <c r="M13" s="389">
         <v>80</v>
       </c>
-      <c r="N13" s="398" t="s">
+      <c r="N13" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="386">
+      <c r="O13" s="389">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="386">
+      <c r="P13" s="389">
         <v>2</v>
       </c>
-      <c r="Q13" s="386">
+      <c r="Q13" s="389">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="386">
+      <c r="R13" s="389">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="386"/>
-      <c r="T13" s="389">
+      <c r="S13" s="389"/>
+      <c r="T13" s="392">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="386">
+      <c r="U13" s="389">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -18921,7 +18945,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="396"/>
+      <c r="B14" s="399"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -18953,15 +18977,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="387"/>
-      <c r="N14" s="399"/>
-      <c r="O14" s="387"/>
-      <c r="P14" s="387"/>
-      <c r="Q14" s="387"/>
-      <c r="R14" s="387"/>
-      <c r="S14" s="387"/>
-      <c r="T14" s="390"/>
-      <c r="U14" s="387"/>
+      <c r="M14" s="390"/>
+      <c r="N14" s="402"/>
+      <c r="O14" s="390"/>
+      <c r="P14" s="390"/>
+      <c r="Q14" s="390"/>
+      <c r="R14" s="390"/>
+      <c r="S14" s="390"/>
+      <c r="T14" s="393"/>
+      <c r="U14" s="390"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -18969,10 +18993,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="401" t="s">
+      <c r="A15" s="404" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="396"/>
+      <c r="B15" s="399"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -18983,15 +19007,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="387"/>
-      <c r="N15" s="399"/>
-      <c r="O15" s="387"/>
-      <c r="P15" s="387"/>
-      <c r="Q15" s="387"/>
-      <c r="R15" s="387"/>
-      <c r="S15" s="387"/>
-      <c r="T15" s="390"/>
-      <c r="U15" s="387"/>
+      <c r="M15" s="390"/>
+      <c r="N15" s="402"/>
+      <c r="O15" s="390"/>
+      <c r="P15" s="390"/>
+      <c r="Q15" s="390"/>
+      <c r="R15" s="390"/>
+      <c r="S15" s="390"/>
+      <c r="T15" s="393"/>
+      <c r="U15" s="390"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -19001,8 +19025,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="402"/>
-      <c r="B16" s="397"/>
+      <c r="A16" s="405"/>
+      <c r="B16" s="400"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -19013,15 +19037,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="388"/>
-      <c r="N16" s="400"/>
-      <c r="O16" s="388"/>
-      <c r="P16" s="388"/>
-      <c r="Q16" s="388"/>
-      <c r="R16" s="388"/>
-      <c r="S16" s="388"/>
-      <c r="T16" s="391"/>
-      <c r="U16" s="388"/>
+      <c r="M16" s="391"/>
+      <c r="N16" s="403"/>
+      <c r="O16" s="391"/>
+      <c r="P16" s="391"/>
+      <c r="Q16" s="391"/>
+      <c r="R16" s="391"/>
+      <c r="S16" s="391"/>
+      <c r="T16" s="394"/>
+      <c r="U16" s="391"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -19032,7 +19056,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="395" t="s">
+      <c r="B17" s="398" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -19066,33 +19090,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="386">
+      <c r="M17" s="389">
         <v>70</v>
       </c>
-      <c r="N17" s="398" t="s">
+      <c r="N17" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="386">
+      <c r="O17" s="389">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="386">
+      <c r="P17" s="389">
         <v>2</v>
       </c>
-      <c r="Q17" s="386">
+      <c r="Q17" s="389">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="386">
+      <c r="R17" s="389">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="386"/>
-      <c r="T17" s="389">
+      <c r="S17" s="389"/>
+      <c r="T17" s="392">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="386">
+      <c r="U17" s="389">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -19111,7 +19135,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="396"/>
+      <c r="B18" s="399"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -19143,24 +19167,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="387"/>
-      <c r="N18" s="399"/>
-      <c r="O18" s="387"/>
-      <c r="P18" s="387"/>
-      <c r="Q18" s="387"/>
-      <c r="R18" s="387"/>
-      <c r="S18" s="387"/>
-      <c r="T18" s="390"/>
-      <c r="U18" s="387"/>
+      <c r="M18" s="390"/>
+      <c r="N18" s="402"/>
+      <c r="O18" s="390"/>
+      <c r="P18" s="390"/>
+      <c r="Q18" s="390"/>
+      <c r="R18" s="390"/>
+      <c r="S18" s="390"/>
+      <c r="T18" s="393"/>
+      <c r="U18" s="390"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="386" t="s">
+      <c r="A19" s="389" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="396"/>
+      <c r="B19" s="399"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -19171,22 +19195,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="387"/>
-      <c r="N19" s="399"/>
-      <c r="O19" s="387"/>
-      <c r="P19" s="387"/>
-      <c r="Q19" s="387"/>
-      <c r="R19" s="387"/>
-      <c r="S19" s="387"/>
-      <c r="T19" s="390"/>
-      <c r="U19" s="387"/>
+      <c r="M19" s="390"/>
+      <c r="N19" s="402"/>
+      <c r="O19" s="390"/>
+      <c r="P19" s="390"/>
+      <c r="Q19" s="390"/>
+      <c r="R19" s="390"/>
+      <c r="S19" s="390"/>
+      <c r="T19" s="393"/>
+      <c r="U19" s="390"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="388"/>
-      <c r="B20" s="397"/>
+      <c r="A20" s="391"/>
+      <c r="B20" s="400"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -19197,15 +19221,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="388"/>
-      <c r="N20" s="400"/>
-      <c r="O20" s="388"/>
-      <c r="P20" s="388"/>
-      <c r="Q20" s="388"/>
-      <c r="R20" s="388"/>
-      <c r="S20" s="388"/>
-      <c r="T20" s="391"/>
-      <c r="U20" s="388"/>
+      <c r="M20" s="391"/>
+      <c r="N20" s="403"/>
+      <c r="O20" s="391"/>
+      <c r="P20" s="391"/>
+      <c r="Q20" s="391"/>
+      <c r="R20" s="391"/>
+      <c r="S20" s="391"/>
+      <c r="T20" s="394"/>
+      <c r="U20" s="391"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -19214,7 +19238,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="395" t="s">
+      <c r="B21" s="398" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -19248,33 +19272,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="386">
+      <c r="M21" s="389">
         <v>60</v>
       </c>
-      <c r="N21" s="398" t="s">
+      <c r="N21" s="401" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="386">
+      <c r="O21" s="389">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="386">
+      <c r="P21" s="389">
         <v>3</v>
       </c>
-      <c r="Q21" s="386">
+      <c r="Q21" s="389">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="386">
+      <c r="R21" s="389">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="386"/>
-      <c r="T21" s="389">
+      <c r="S21" s="389"/>
+      <c r="T21" s="392">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="386">
+      <c r="U21" s="389">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -19291,7 +19315,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="396"/>
+      <c r="B22" s="399"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -19323,24 +19347,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="387"/>
-      <c r="N22" s="399"/>
-      <c r="O22" s="387"/>
-      <c r="P22" s="387"/>
-      <c r="Q22" s="387"/>
-      <c r="R22" s="387"/>
-      <c r="S22" s="387"/>
-      <c r="T22" s="390"/>
-      <c r="U22" s="387"/>
+      <c r="M22" s="390"/>
+      <c r="N22" s="402"/>
+      <c r="O22" s="390"/>
+      <c r="P22" s="390"/>
+      <c r="Q22" s="390"/>
+      <c r="R22" s="390"/>
+      <c r="S22" s="390"/>
+      <c r="T22" s="393"/>
+      <c r="U22" s="390"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="392" t="s">
+      <c r="A23" s="395" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="396"/>
+      <c r="B23" s="399"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -19351,22 +19375,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="387"/>
-      <c r="N23" s="399"/>
-      <c r="O23" s="387"/>
-      <c r="P23" s="387"/>
-      <c r="Q23" s="387"/>
-      <c r="R23" s="387"/>
-      <c r="S23" s="387"/>
-      <c r="T23" s="390"/>
-      <c r="U23" s="387"/>
+      <c r="M23" s="390"/>
+      <c r="N23" s="402"/>
+      <c r="O23" s="390"/>
+      <c r="P23" s="390"/>
+      <c r="Q23" s="390"/>
+      <c r="R23" s="390"/>
+      <c r="S23" s="390"/>
+      <c r="T23" s="393"/>
+      <c r="U23" s="390"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="393"/>
-      <c r="B24" s="397"/>
+      <c r="A24" s="396"/>
+      <c r="B24" s="400"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -19377,15 +19401,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="388"/>
-      <c r="N24" s="400"/>
-      <c r="O24" s="388"/>
-      <c r="P24" s="388"/>
-      <c r="Q24" s="388"/>
-      <c r="R24" s="388"/>
-      <c r="S24" s="388"/>
-      <c r="T24" s="391"/>
-      <c r="U24" s="388"/>
+      <c r="M24" s="391"/>
+      <c r="N24" s="403"/>
+      <c r="O24" s="391"/>
+      <c r="P24" s="391"/>
+      <c r="Q24" s="391"/>
+      <c r="R24" s="391"/>
+      <c r="S24" s="391"/>
+      <c r="T24" s="394"/>
+      <c r="U24" s="391"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -19411,13 +19435,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="394" t="s">
+      <c r="H27" s="397" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="394"/>
-      <c r="J27" s="394"/>
-      <c r="K27" s="394"/>
-      <c r="L27" s="394"/>
+      <c r="I27" s="397"/>
+      <c r="J27" s="397"/>
+      <c r="K27" s="397"/>
+      <c r="L27" s="397"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -19697,19 +19721,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="384" t="s">
+      <c r="D40" s="387" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="384"/>
-      <c r="F40" s="384"/>
-      <c r="G40" s="384"/>
-      <c r="H40" s="384"/>
-      <c r="I40" s="384" t="s">
+      <c r="E40" s="387"/>
+      <c r="F40" s="387"/>
+      <c r="G40" s="387"/>
+      <c r="H40" s="387"/>
+      <c r="I40" s="387" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="384"/>
-      <c r="K40" s="384"/>
-      <c r="L40" s="384"/>
+      <c r="J40" s="387"/>
+      <c r="K40" s="387"/>
+      <c r="L40" s="387"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -19833,19 +19857,19 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="379"/>
+      <c r="B42" s="382"/>
       <c r="C42" s="110"/>
       <c r="D42" s="111"/>
       <c r="E42" s="111"/>
       <c r="F42" s="125"/>
       <c r="G42" s="125"/>
-      <c r="H42" s="380"/>
+      <c r="H42" s="383"/>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="125"/>
       <c r="L42" s="125"/>
-      <c r="M42" s="380"/>
-      <c r="N42" s="421"/>
+      <c r="M42" s="383"/>
+      <c r="N42" s="424"/>
       <c r="P42" s="91"/>
       <c r="Q42" s="91"/>
       <c r="U42" s="64"/>
@@ -19891,19 +19915,19 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="379"/>
+      <c r="B43" s="382"/>
       <c r="C43" s="110"/>
       <c r="D43" s="125"/>
       <c r="E43" s="111"/>
       <c r="F43" s="125"/>
       <c r="G43" s="103"/>
-      <c r="H43" s="380"/>
+      <c r="H43" s="383"/>
       <c r="I43" s="111"/>
       <c r="J43" s="111"/>
       <c r="K43" s="103"/>
       <c r="L43" s="103"/>
-      <c r="M43" s="380"/>
-      <c r="N43" s="380"/>
+      <c r="M43" s="383"/>
+      <c r="N43" s="383"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -19949,19 +19973,19 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="379"/>
+      <c r="B44" s="382"/>
       <c r="C44" s="110"/>
       <c r="D44" s="111"/>
       <c r="E44" s="111"/>
       <c r="F44" s="125"/>
       <c r="G44" s="125"/>
-      <c r="H44" s="380"/>
+      <c r="H44" s="383"/>
       <c r="I44" s="111"/>
       <c r="J44" s="111"/>
       <c r="K44" s="125"/>
       <c r="L44" s="125"/>
-      <c r="M44" s="380"/>
-      <c r="N44" s="380"/>
+      <c r="M44" s="383"/>
+      <c r="N44" s="383"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -20007,19 +20031,19 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="379"/>
+      <c r="B45" s="382"/>
       <c r="C45" s="110"/>
       <c r="D45" s="111"/>
       <c r="E45" s="111"/>
       <c r="F45" s="125"/>
       <c r="G45" s="125"/>
-      <c r="H45" s="380"/>
+      <c r="H45" s="383"/>
       <c r="I45" s="111"/>
       <c r="J45" s="111"/>
       <c r="K45" s="125"/>
       <c r="L45" s="125"/>
-      <c r="M45" s="380"/>
-      <c r="N45" s="380"/>
+      <c r="M45" s="383"/>
+      <c r="N45" s="383"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -20065,19 +20089,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="379"/>
+      <c r="B46" s="382"/>
       <c r="C46" s="110"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="125"/>
       <c r="G46" s="125"/>
-      <c r="H46" s="380"/>
+      <c r="H46" s="383"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="125"/>
       <c r="L46" s="125"/>
-      <c r="M46" s="380"/>
-      <c r="N46" s="422"/>
+      <c r="M46" s="383"/>
+      <c r="N46" s="425"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -20123,19 +20147,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="379"/>
+      <c r="B47" s="382"/>
       <c r="C47" s="110"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="380"/>
+      <c r="H47" s="383"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="380"/>
-      <c r="N47" s="382"/>
+      <c r="M47" s="383"/>
+      <c r="N47" s="385"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -20183,19 +20207,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="379"/>
+      <c r="B48" s="382"/>
       <c r="C48" s="110"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="380"/>
+      <c r="H48" s="383"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="380"/>
-      <c r="N48" s="382"/>
+      <c r="M48" s="383"/>
+      <c r="N48" s="385"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -20243,19 +20267,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="379"/>
+      <c r="B49" s="382"/>
       <c r="C49" s="110"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="380"/>
+      <c r="H49" s="383"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="380"/>
-      <c r="N49" s="382"/>
+      <c r="M49" s="383"/>
+      <c r="N49" s="385"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -20303,19 +20327,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="374"/>
+      <c r="B50" s="377"/>
       <c r="C50" s="112"/>
       <c r="D50" s="113"/>
       <c r="E50" s="113"/>
       <c r="F50" s="113"/>
       <c r="G50" s="113"/>
-      <c r="H50" s="375"/>
+      <c r="H50" s="378"/>
       <c r="I50" s="113"/>
       <c r="J50" s="113"/>
       <c r="K50" s="113"/>
       <c r="L50" s="113"/>
-      <c r="M50" s="375"/>
-      <c r="N50" s="423"/>
+      <c r="M50" s="378"/>
+      <c r="N50" s="426"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -20336,19 +20360,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="374"/>
+      <c r="B51" s="377"/>
       <c r="C51" s="112"/>
       <c r="D51" s="113"/>
       <c r="E51" s="113"/>
       <c r="F51" s="113"/>
       <c r="G51" s="113"/>
-      <c r="H51" s="375"/>
+      <c r="H51" s="378"/>
       <c r="I51" s="113"/>
       <c r="J51" s="113"/>
       <c r="K51" s="113"/>
       <c r="L51" s="113"/>
-      <c r="M51" s="375"/>
-      <c r="N51" s="377"/>
+      <c r="M51" s="378"/>
+      <c r="N51" s="380"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -20379,19 +20403,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="374"/>
+      <c r="B52" s="377"/>
       <c r="C52" s="112"/>
       <c r="D52" s="113"/>
       <c r="E52" s="113"/>
       <c r="F52" s="113"/>
       <c r="G52" s="113"/>
-      <c r="H52" s="375"/>
+      <c r="H52" s="378"/>
       <c r="I52" s="113"/>
       <c r="J52" s="113"/>
       <c r="K52" s="113"/>
       <c r="L52" s="113"/>
-      <c r="M52" s="375"/>
-      <c r="N52" s="377"/>
+      <c r="M52" s="378"/>
+      <c r="N52" s="380"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -20455,19 +20479,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="374"/>
+      <c r="B53" s="377"/>
       <c r="C53" s="112"/>
       <c r="D53" s="113"/>
       <c r="E53" s="113"/>
       <c r="F53" s="113"/>
       <c r="G53" s="113"/>
-      <c r="H53" s="375"/>
+      <c r="H53" s="378"/>
       <c r="I53" s="113"/>
       <c r="J53" s="113"/>
       <c r="K53" s="113"/>
       <c r="L53" s="113"/>
-      <c r="M53" s="375"/>
-      <c r="N53" s="377"/>
+      <c r="M53" s="378"/>
+      <c r="N53" s="380"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -20516,19 +20540,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="374"/>
+      <c r="B54" s="377"/>
       <c r="C54" s="112"/>
       <c r="D54" s="113"/>
       <c r="E54" s="113"/>
       <c r="F54" s="113"/>
       <c r="G54" s="113"/>
-      <c r="H54" s="375"/>
+      <c r="H54" s="378"/>
       <c r="I54" s="113"/>
       <c r="J54" s="113"/>
       <c r="K54" s="113"/>
       <c r="L54" s="113"/>
-      <c r="M54" s="375"/>
-      <c r="N54" s="416"/>
+      <c r="M54" s="378"/>
+      <c r="N54" s="419"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -20575,19 +20599,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="374"/>
+      <c r="B55" s="377"/>
       <c r="C55" s="112"/>
       <c r="D55" s="113"/>
       <c r="E55" s="113"/>
       <c r="F55" s="113"/>
       <c r="G55" s="113"/>
-      <c r="H55" s="375"/>
+      <c r="H55" s="378"/>
       <c r="I55" s="113"/>
       <c r="J55" s="113"/>
       <c r="K55" s="113"/>
       <c r="L55" s="113"/>
-      <c r="M55" s="375"/>
-      <c r="N55" s="377"/>
+      <c r="M55" s="378"/>
+      <c r="N55" s="380"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -20634,19 +20658,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="374"/>
+      <c r="B56" s="377"/>
       <c r="C56" s="112"/>
       <c r="D56" s="113"/>
       <c r="E56" s="113"/>
       <c r="F56" s="113"/>
       <c r="G56" s="113"/>
-      <c r="H56" s="375"/>
+      <c r="H56" s="378"/>
       <c r="I56" s="113"/>
       <c r="J56" s="113"/>
       <c r="K56" s="113"/>
       <c r="L56" s="113"/>
-      <c r="M56" s="375"/>
-      <c r="N56" s="377"/>
+      <c r="M56" s="378"/>
+      <c r="N56" s="380"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -20693,19 +20717,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="374"/>
+      <c r="B57" s="377"/>
       <c r="C57" s="112"/>
       <c r="D57" s="113"/>
       <c r="E57" s="113"/>
       <c r="F57" s="113"/>
       <c r="G57" s="113"/>
-      <c r="H57" s="375"/>
+      <c r="H57" s="378"/>
       <c r="I57" s="113"/>
       <c r="J57" s="113"/>
       <c r="K57" s="113"/>
       <c r="L57" s="113"/>
-      <c r="M57" s="375"/>
-      <c r="N57" s="377"/>
+      <c r="M57" s="378"/>
+      <c r="N57" s="380"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -20752,19 +20776,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="369"/>
+      <c r="B58" s="372"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
       <c r="E58" s="115"/>
       <c r="F58" s="115"/>
       <c r="G58" s="115"/>
-      <c r="H58" s="370"/>
+      <c r="H58" s="373"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115"/>
       <c r="K58" s="115"/>
       <c r="L58" s="115"/>
-      <c r="M58" s="370"/>
-      <c r="N58" s="417"/>
+      <c r="M58" s="373"/>
+      <c r="N58" s="420"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -20811,19 +20835,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="369"/>
+      <c r="B59" s="372"/>
       <c r="C59" s="114"/>
       <c r="D59" s="115"/>
       <c r="E59" s="115"/>
       <c r="F59" s="115"/>
       <c r="G59" s="115"/>
-      <c r="H59" s="370"/>
+      <c r="H59" s="373"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115"/>
       <c r="K59" s="115"/>
       <c r="L59" s="115"/>
-      <c r="M59" s="370"/>
-      <c r="N59" s="372"/>
+      <c r="M59" s="373"/>
+      <c r="N59" s="375"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -20870,19 +20894,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="369"/>
+      <c r="B60" s="372"/>
       <c r="C60" s="114"/>
       <c r="D60" s="115"/>
       <c r="E60" s="115"/>
       <c r="F60" s="115"/>
       <c r="G60" s="115"/>
-      <c r="H60" s="370"/>
+      <c r="H60" s="373"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115"/>
       <c r="K60" s="115"/>
       <c r="L60" s="115"/>
-      <c r="M60" s="370"/>
-      <c r="N60" s="372"/>
+      <c r="M60" s="373"/>
+      <c r="N60" s="375"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -20929,247 +20953,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="369"/>
+      <c r="B61" s="372"/>
       <c r="C61" s="114"/>
       <c r="D61" s="115"/>
       <c r="E61" s="115"/>
       <c r="F61" s="115"/>
       <c r="G61" s="115"/>
-      <c r="H61" s="370"/>
+      <c r="H61" s="373"/>
       <c r="I61" s="115"/>
       <c r="J61" s="115"/>
       <c r="K61" s="115"/>
       <c r="L61" s="115"/>
-      <c r="M61" s="370"/>
-      <c r="N61" s="372"/>
+      <c r="M61" s="373"/>
+      <c r="N61" s="375"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="369"/>
+      <c r="B62" s="372"/>
       <c r="C62" s="114"/>
       <c r="D62" s="115"/>
       <c r="E62" s="115"/>
       <c r="F62" s="115"/>
       <c r="G62" s="115"/>
-      <c r="H62" s="370"/>
+      <c r="H62" s="373"/>
       <c r="I62" s="115"/>
       <c r="J62" s="115"/>
       <c r="K62" s="115"/>
       <c r="L62" s="115"/>
-      <c r="M62" s="370"/>
-      <c r="N62" s="418"/>
+      <c r="M62" s="373"/>
+      <c r="N62" s="421"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="369"/>
+      <c r="B63" s="372"/>
       <c r="C63" s="114"/>
       <c r="D63" s="115"/>
       <c r="E63" s="115"/>
       <c r="F63" s="115"/>
       <c r="G63" s="115"/>
-      <c r="H63" s="370"/>
+      <c r="H63" s="373"/>
       <c r="I63" s="115"/>
       <c r="J63" s="115"/>
       <c r="K63" s="115"/>
       <c r="L63" s="115"/>
-      <c r="M63" s="370"/>
-      <c r="N63" s="372"/>
+      <c r="M63" s="373"/>
+      <c r="N63" s="375"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="369"/>
+      <c r="B64" s="372"/>
       <c r="C64" s="114"/>
       <c r="D64" s="115"/>
       <c r="E64" s="115"/>
       <c r="F64" s="115"/>
       <c r="G64" s="115"/>
-      <c r="H64" s="370"/>
+      <c r="H64" s="373"/>
       <c r="I64" s="115"/>
       <c r="J64" s="115"/>
       <c r="K64" s="115"/>
       <c r="L64" s="115"/>
-      <c r="M64" s="370"/>
-      <c r="N64" s="372"/>
+      <c r="M64" s="373"/>
+      <c r="N64" s="375"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="369"/>
+      <c r="B65" s="372"/>
       <c r="C65" s="114"/>
       <c r="D65" s="115"/>
       <c r="E65" s="115"/>
       <c r="F65" s="115"/>
       <c r="G65" s="115"/>
-      <c r="H65" s="370"/>
+      <c r="H65" s="373"/>
       <c r="I65" s="115"/>
       <c r="J65" s="115"/>
       <c r="K65" s="115"/>
       <c r="L65" s="115"/>
-      <c r="M65" s="370"/>
-      <c r="N65" s="372"/>
+      <c r="M65" s="373"/>
+      <c r="N65" s="375"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="365"/>
+      <c r="B66" s="368"/>
       <c r="C66" s="128"/>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
       <c r="F66" s="116"/>
       <c r="G66" s="116"/>
-      <c r="H66" s="366"/>
+      <c r="H66" s="369"/>
       <c r="I66" s="116"/>
       <c r="J66" s="116"/>
       <c r="K66" s="116"/>
       <c r="L66" s="116"/>
-      <c r="M66" s="366"/>
-      <c r="N66" s="419"/>
+      <c r="M66" s="369"/>
+      <c r="N66" s="422"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="365"/>
+      <c r="B67" s="368"/>
       <c r="C67" s="128"/>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
       <c r="F67" s="116"/>
       <c r="G67" s="116"/>
-      <c r="H67" s="366"/>
+      <c r="H67" s="369"/>
       <c r="I67" s="116"/>
       <c r="J67" s="116"/>
       <c r="K67" s="116"/>
       <c r="L67" s="116"/>
-      <c r="M67" s="366"/>
-      <c r="N67" s="368"/>
+      <c r="M67" s="369"/>
+      <c r="N67" s="371"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="365"/>
+      <c r="B68" s="368"/>
       <c r="C68" s="128"/>
       <c r="D68" s="116"/>
       <c r="E68" s="116"/>
       <c r="F68" s="116"/>
       <c r="G68" s="116"/>
-      <c r="H68" s="366"/>
+      <c r="H68" s="369"/>
       <c r="I68" s="116"/>
       <c r="J68" s="116"/>
       <c r="K68" s="116"/>
       <c r="L68" s="116"/>
-      <c r="M68" s="366"/>
-      <c r="N68" s="368"/>
+      <c r="M68" s="369"/>
+      <c r="N68" s="371"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="365"/>
+      <c r="B69" s="368"/>
       <c r="C69" s="128"/>
       <c r="D69" s="116"/>
       <c r="E69" s="116"/>
       <c r="F69" s="116"/>
       <c r="G69" s="116"/>
-      <c r="H69" s="366"/>
+      <c r="H69" s="369"/>
       <c r="I69" s="116"/>
       <c r="J69" s="116"/>
       <c r="K69" s="116"/>
       <c r="L69" s="116"/>
-      <c r="M69" s="366"/>
-      <c r="N69" s="368"/>
+      <c r="M69" s="369"/>
+      <c r="N69" s="371"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="365"/>
+      <c r="B70" s="368"/>
       <c r="C70" s="128"/>
       <c r="D70" s="116"/>
       <c r="E70" s="116"/>
       <c r="F70" s="116"/>
       <c r="G70" s="116"/>
-      <c r="H70" s="366"/>
+      <c r="H70" s="369"/>
       <c r="I70" s="116"/>
       <c r="J70" s="116"/>
       <c r="K70" s="116"/>
       <c r="L70" s="116"/>
-      <c r="M70" s="366"/>
-      <c r="N70" s="420"/>
+      <c r="M70" s="369"/>
+      <c r="N70" s="423"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="365"/>
+      <c r="B71" s="368"/>
       <c r="C71" s="128"/>
       <c r="D71" s="116"/>
       <c r="E71" s="116"/>
       <c r="F71" s="116"/>
       <c r="G71" s="116"/>
-      <c r="H71" s="366"/>
+      <c r="H71" s="369"/>
       <c r="I71" s="116"/>
       <c r="J71" s="116"/>
       <c r="K71" s="116"/>
       <c r="L71" s="116"/>
-      <c r="M71" s="366"/>
-      <c r="N71" s="368"/>
+      <c r="M71" s="369"/>
+      <c r="N71" s="371"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="365"/>
+      <c r="B72" s="368"/>
       <c r="C72" s="128"/>
       <c r="D72" s="116"/>
       <c r="E72" s="116"/>
       <c r="F72" s="116"/>
       <c r="G72" s="116"/>
-      <c r="H72" s="366"/>
+      <c r="H72" s="369"/>
       <c r="I72" s="116"/>
       <c r="J72" s="116"/>
       <c r="K72" s="116"/>
       <c r="L72" s="116"/>
-      <c r="M72" s="366"/>
-      <c r="N72" s="368"/>
+      <c r="M72" s="369"/>
+      <c r="N72" s="371"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="365"/>
+      <c r="B73" s="368"/>
       <c r="C73" s="128"/>
       <c r="D73" s="116"/>
       <c r="E73" s="116"/>
       <c r="F73" s="116"/>
       <c r="G73" s="116"/>
-      <c r="H73" s="366"/>
+      <c r="H73" s="369"/>
       <c r="I73" s="116"/>
       <c r="J73" s="116"/>
       <c r="K73" s="116"/>
       <c r="L73" s="116"/>
-      <c r="M73" s="366"/>
-      <c r="N73" s="368"/>
+      <c r="M73" s="369"/>
+      <c r="N73" s="371"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>

</xml_diff>

<commit_message>
calculation tenant id update
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="247">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -838,13 +838,22 @@
     <t>Solid</t>
   </si>
   <si>
-    <t>Select Type:</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
+    <t>Select Product Type</t>
+  </si>
+  <si>
+    <t>Limit Selection Type</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Test Product5</t>
+  </si>
+  <si>
+    <t>Test Product6</t>
+  </si>
+  <si>
+    <t>Tenant ID:</t>
   </si>
 </sst>
 </file>
@@ -1940,7 +1949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="427">
+  <cellXfs count="429">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2561,6 +2570,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2709,6 +2721,7 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5128,15 +5141,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="371" t="s">
+      <c r="F1" s="372" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="371"/>
-      <c r="H1" s="371"/>
-      <c r="I1" s="371"/>
-      <c r="J1" s="371"/>
-      <c r="K1" s="371"/>
-      <c r="L1" s="371"/>
+      <c r="G1" s="372"/>
+      <c r="H1" s="372"/>
+      <c r="I1" s="372"/>
+      <c r="J1" s="372"/>
+      <c r="K1" s="372"/>
+      <c r="L1" s="372"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -5225,22 +5238,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="372" t="s">
+      <c r="D6" s="373" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="373"/>
-      <c r="F6" s="373"/>
-      <c r="G6" s="373"/>
-      <c r="H6" s="374"/>
+      <c r="E6" s="374"/>
+      <c r="F6" s="374"/>
+      <c r="G6" s="374"/>
+      <c r="H6" s="375"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="372" t="s">
+      <c r="M6" s="373" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="373"/>
-      <c r="O6" s="373"/>
-      <c r="P6" s="373"/>
-      <c r="Q6" s="374"/>
+      <c r="N6" s="374"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="374"/>
+      <c r="Q6" s="375"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -5258,10 +5271,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="375" t="s">
+      <c r="F7" s="376" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="376"/>
+      <c r="G7" s="377"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -5284,10 +5297,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="375" t="s">
+      <c r="P7" s="376" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="376"/>
+      <c r="Q7" s="377"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -5364,7 +5377,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="377" t="s">
+      <c r="B9" s="378" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5398,33 +5411,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="368">
+      <c r="M9" s="369">
         <v>20</v>
       </c>
-      <c r="N9" s="380" t="s">
+      <c r="N9" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="368">
+      <c r="O9" s="369">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="368">
+      <c r="P9" s="369">
         <v>3</v>
       </c>
-      <c r="Q9" s="368">
+      <c r="Q9" s="369">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="368">
+      <c r="R9" s="369">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="368"/>
-      <c r="T9" s="383">
+      <c r="S9" s="369"/>
+      <c r="T9" s="384">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="368">
+      <c r="U9" s="369">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -5449,7 +5462,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="378"/>
+      <c r="B10" s="379"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -5481,15 +5494,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="369"/>
-      <c r="N10" s="381"/>
-      <c r="O10" s="369"/>
-      <c r="P10" s="369"/>
-      <c r="Q10" s="369"/>
-      <c r="R10" s="369"/>
-      <c r="S10" s="369"/>
-      <c r="T10" s="384"/>
-      <c r="U10" s="369"/>
+      <c r="M10" s="370"/>
+      <c r="N10" s="382"/>
+      <c r="O10" s="370"/>
+      <c r="P10" s="370"/>
+      <c r="Q10" s="370"/>
+      <c r="R10" s="370"/>
+      <c r="S10" s="370"/>
+      <c r="T10" s="385"/>
+      <c r="U10" s="370"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -5497,10 +5510,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="368" t="s">
+      <c r="A11" s="369" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="378"/>
+      <c r="B11" s="379"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -5511,15 +5524,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="369"/>
-      <c r="N11" s="381"/>
-      <c r="O11" s="369"/>
-      <c r="P11" s="369"/>
-      <c r="Q11" s="369"/>
-      <c r="R11" s="369"/>
-      <c r="S11" s="369"/>
-      <c r="T11" s="384"/>
-      <c r="U11" s="369"/>
+      <c r="M11" s="370"/>
+      <c r="N11" s="382"/>
+      <c r="O11" s="370"/>
+      <c r="P11" s="370"/>
+      <c r="Q11" s="370"/>
+      <c r="R11" s="370"/>
+      <c r="S11" s="370"/>
+      <c r="T11" s="385"/>
+      <c r="U11" s="370"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -5538,8 +5551,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="370"/>
-      <c r="B12" s="379"/>
+      <c r="A12" s="371"/>
+      <c r="B12" s="380"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -5550,15 +5563,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="370"/>
-      <c r="N12" s="382"/>
-      <c r="O12" s="370"/>
-      <c r="P12" s="370"/>
-      <c r="Q12" s="370"/>
-      <c r="R12" s="370"/>
-      <c r="S12" s="370"/>
-      <c r="T12" s="385"/>
-      <c r="U12" s="370"/>
+      <c r="M12" s="371"/>
+      <c r="N12" s="383"/>
+      <c r="O12" s="371"/>
+      <c r="P12" s="371"/>
+      <c r="Q12" s="371"/>
+      <c r="R12" s="371"/>
+      <c r="S12" s="371"/>
+      <c r="T12" s="386"/>
+      <c r="U12" s="371"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -5574,7 +5587,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="377" t="s">
+      <c r="B13" s="378" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5608,33 +5621,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="368">
+      <c r="M13" s="369">
         <v>80</v>
       </c>
-      <c r="N13" s="380" t="s">
+      <c r="N13" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="368">
+      <c r="O13" s="369">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="368">
+      <c r="P13" s="369">
         <v>2</v>
       </c>
-      <c r="Q13" s="368">
+      <c r="Q13" s="369">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="368">
+      <c r="R13" s="369">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="368"/>
-      <c r="T13" s="383">
+      <c r="S13" s="369"/>
+      <c r="T13" s="384">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="368">
+      <c r="U13" s="369">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -5657,7 +5670,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="378"/>
+      <c r="B14" s="379"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -5689,15 +5702,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="369"/>
-      <c r="N14" s="381"/>
-      <c r="O14" s="369"/>
-      <c r="P14" s="369"/>
-      <c r="Q14" s="369"/>
-      <c r="R14" s="369"/>
-      <c r="S14" s="369"/>
-      <c r="T14" s="384"/>
-      <c r="U14" s="369"/>
+      <c r="M14" s="370"/>
+      <c r="N14" s="382"/>
+      <c r="O14" s="370"/>
+      <c r="P14" s="370"/>
+      <c r="Q14" s="370"/>
+      <c r="R14" s="370"/>
+      <c r="S14" s="370"/>
+      <c r="T14" s="385"/>
+      <c r="U14" s="370"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -5705,10 +5718,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="386" t="s">
+      <c r="A15" s="387" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="378"/>
+      <c r="B15" s="379"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -5719,15 +5732,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="369"/>
-      <c r="N15" s="381"/>
-      <c r="O15" s="369"/>
-      <c r="P15" s="369"/>
-      <c r="Q15" s="369"/>
-      <c r="R15" s="369"/>
-      <c r="S15" s="369"/>
-      <c r="T15" s="384"/>
-      <c r="U15" s="369"/>
+      <c r="M15" s="370"/>
+      <c r="N15" s="382"/>
+      <c r="O15" s="370"/>
+      <c r="P15" s="370"/>
+      <c r="Q15" s="370"/>
+      <c r="R15" s="370"/>
+      <c r="S15" s="370"/>
+      <c r="T15" s="385"/>
+      <c r="U15" s="370"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -5737,8 +5750,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="387"/>
-      <c r="B16" s="379"/>
+      <c r="A16" s="388"/>
+      <c r="B16" s="380"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -5749,15 +5762,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="370"/>
-      <c r="N16" s="382"/>
-      <c r="O16" s="370"/>
-      <c r="P16" s="370"/>
-      <c r="Q16" s="370"/>
-      <c r="R16" s="370"/>
-      <c r="S16" s="370"/>
-      <c r="T16" s="385"/>
-      <c r="U16" s="370"/>
+      <c r="M16" s="371"/>
+      <c r="N16" s="383"/>
+      <c r="O16" s="371"/>
+      <c r="P16" s="371"/>
+      <c r="Q16" s="371"/>
+      <c r="R16" s="371"/>
+      <c r="S16" s="371"/>
+      <c r="T16" s="386"/>
+      <c r="U16" s="371"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -5768,7 +5781,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="377" t="s">
+      <c r="B17" s="378" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5802,33 +5815,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="368">
+      <c r="M17" s="369">
         <v>70</v>
       </c>
-      <c r="N17" s="380" t="s">
+      <c r="N17" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="368">
+      <c r="O17" s="369">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="368">
+      <c r="P17" s="369">
         <v>2</v>
       </c>
-      <c r="Q17" s="368">
+      <c r="Q17" s="369">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="368">
+      <c r="R17" s="369">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="368"/>
-      <c r="T17" s="383">
+      <c r="S17" s="369"/>
+      <c r="T17" s="384">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="368">
+      <c r="U17" s="369">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -5847,7 +5860,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="378"/>
+      <c r="B18" s="379"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -5879,24 +5892,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="369"/>
-      <c r="N18" s="381"/>
-      <c r="O18" s="369"/>
-      <c r="P18" s="369"/>
-      <c r="Q18" s="369"/>
-      <c r="R18" s="369"/>
-      <c r="S18" s="369"/>
-      <c r="T18" s="384"/>
-      <c r="U18" s="369"/>
+      <c r="M18" s="370"/>
+      <c r="N18" s="382"/>
+      <c r="O18" s="370"/>
+      <c r="P18" s="370"/>
+      <c r="Q18" s="370"/>
+      <c r="R18" s="370"/>
+      <c r="S18" s="370"/>
+      <c r="T18" s="385"/>
+      <c r="U18" s="370"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="368" t="s">
+      <c r="A19" s="369" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="378"/>
+      <c r="B19" s="379"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -5907,22 +5920,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="369"/>
-      <c r="N19" s="381"/>
-      <c r="O19" s="369"/>
-      <c r="P19" s="369"/>
-      <c r="Q19" s="369"/>
-      <c r="R19" s="369"/>
-      <c r="S19" s="369"/>
-      <c r="T19" s="384"/>
-      <c r="U19" s="369"/>
+      <c r="M19" s="370"/>
+      <c r="N19" s="382"/>
+      <c r="O19" s="370"/>
+      <c r="P19" s="370"/>
+      <c r="Q19" s="370"/>
+      <c r="R19" s="370"/>
+      <c r="S19" s="370"/>
+      <c r="T19" s="385"/>
+      <c r="U19" s="370"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="370"/>
-      <c r="B20" s="379"/>
+      <c r="A20" s="371"/>
+      <c r="B20" s="380"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -5933,15 +5946,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="370"/>
-      <c r="N20" s="382"/>
-      <c r="O20" s="370"/>
-      <c r="P20" s="370"/>
-      <c r="Q20" s="370"/>
-      <c r="R20" s="370"/>
-      <c r="S20" s="370"/>
-      <c r="T20" s="385"/>
-      <c r="U20" s="370"/>
+      <c r="M20" s="371"/>
+      <c r="N20" s="383"/>
+      <c r="O20" s="371"/>
+      <c r="P20" s="371"/>
+      <c r="Q20" s="371"/>
+      <c r="R20" s="371"/>
+      <c r="S20" s="371"/>
+      <c r="T20" s="386"/>
+      <c r="U20" s="371"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -5950,7 +5963,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="377" t="s">
+      <c r="B21" s="378" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5984,33 +5997,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="368">
+      <c r="M21" s="369">
         <v>60</v>
       </c>
-      <c r="N21" s="380" t="s">
+      <c r="N21" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="368">
+      <c r="O21" s="369">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="368">
+      <c r="P21" s="369">
         <v>3</v>
       </c>
-      <c r="Q21" s="368">
+      <c r="Q21" s="369">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="368">
+      <c r="R21" s="369">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="368"/>
-      <c r="T21" s="383">
+      <c r="S21" s="369"/>
+      <c r="T21" s="384">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="368">
+      <c r="U21" s="369">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -6027,7 +6040,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="378"/>
+      <c r="B22" s="379"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -6059,24 +6072,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="369"/>
-      <c r="N22" s="381"/>
-      <c r="O22" s="369"/>
-      <c r="P22" s="369"/>
-      <c r="Q22" s="369"/>
-      <c r="R22" s="369"/>
-      <c r="S22" s="369"/>
-      <c r="T22" s="384"/>
-      <c r="U22" s="369"/>
+      <c r="M22" s="370"/>
+      <c r="N22" s="382"/>
+      <c r="O22" s="370"/>
+      <c r="P22" s="370"/>
+      <c r="Q22" s="370"/>
+      <c r="R22" s="370"/>
+      <c r="S22" s="370"/>
+      <c r="T22" s="385"/>
+      <c r="U22" s="370"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="388" t="s">
+      <c r="A23" s="389" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="378"/>
+      <c r="B23" s="379"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -6087,22 +6100,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="369"/>
-      <c r="N23" s="381"/>
-      <c r="O23" s="369"/>
-      <c r="P23" s="369"/>
-      <c r="Q23" s="369"/>
-      <c r="R23" s="369"/>
-      <c r="S23" s="369"/>
-      <c r="T23" s="384"/>
-      <c r="U23" s="369"/>
+      <c r="M23" s="370"/>
+      <c r="N23" s="382"/>
+      <c r="O23" s="370"/>
+      <c r="P23" s="370"/>
+      <c r="Q23" s="370"/>
+      <c r="R23" s="370"/>
+      <c r="S23" s="370"/>
+      <c r="T23" s="385"/>
+      <c r="U23" s="370"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="389"/>
-      <c r="B24" s="379"/>
+      <c r="A24" s="390"/>
+      <c r="B24" s="380"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -6113,15 +6126,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="370"/>
-      <c r="N24" s="382"/>
-      <c r="O24" s="370"/>
-      <c r="P24" s="370"/>
-      <c r="Q24" s="370"/>
-      <c r="R24" s="370"/>
-      <c r="S24" s="370"/>
-      <c r="T24" s="385"/>
-      <c r="U24" s="370"/>
+      <c r="M24" s="371"/>
+      <c r="N24" s="383"/>
+      <c r="O24" s="371"/>
+      <c r="P24" s="371"/>
+      <c r="Q24" s="371"/>
+      <c r="R24" s="371"/>
+      <c r="S24" s="371"/>
+      <c r="T24" s="386"/>
+      <c r="U24" s="371"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -6147,13 +6160,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="390" t="s">
+      <c r="H27" s="391" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="390"/>
-      <c r="J27" s="390"/>
-      <c r="K27" s="390"/>
-      <c r="L27" s="390"/>
+      <c r="I27" s="391"/>
+      <c r="J27" s="391"/>
+      <c r="K27" s="391"/>
+      <c r="L27" s="391"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -6433,19 +6446,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="393" t="s">
+      <c r="D40" s="394" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="393"/>
-      <c r="F40" s="393"/>
-      <c r="G40" s="393"/>
-      <c r="H40" s="393"/>
-      <c r="I40" s="393" t="s">
+      <c r="E40" s="394"/>
+      <c r="F40" s="394"/>
+      <c r="G40" s="394"/>
+      <c r="H40" s="394"/>
+      <c r="I40" s="394" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="393"/>
-      <c r="K40" s="393"/>
-      <c r="L40" s="393"/>
+      <c r="J40" s="394"/>
+      <c r="K40" s="394"/>
+      <c r="L40" s="394"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -6569,7 +6582,7 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="394" t="s">
+      <c r="B42" s="395" t="s">
         <v>226</v>
       </c>
       <c r="C42" s="190"/>
@@ -6577,17 +6590,17 @@
       <c r="E42" s="111"/>
       <c r="F42" s="189"/>
       <c r="G42" s="189"/>
-      <c r="H42" s="392">
+      <c r="H42" s="393">
         <v>3.095975611358881E-3</v>
       </c>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="189"/>
       <c r="L42" s="189"/>
-      <c r="M42" s="392">
+      <c r="M42" s="393">
         <v>1</v>
       </c>
-      <c r="N42" s="391" t="s">
+      <c r="N42" s="392" t="s">
         <v>59</v>
       </c>
       <c r="P42" s="91"/>
@@ -6635,7 +6648,7 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="394"/>
+      <c r="B43" s="395"/>
       <c r="C43" s="190" t="s">
         <v>220</v>
       </c>
@@ -6651,7 +6664,7 @@
       <c r="G43" s="103">
         <v>97.126746422628088</v>
       </c>
-      <c r="H43" s="392"/>
+      <c r="H43" s="393"/>
       <c r="I43" s="111">
         <v>1</v>
       </c>
@@ -6664,8 +6677,8 @@
       <c r="L43" s="103">
         <v>1</v>
       </c>
-      <c r="M43" s="392"/>
-      <c r="N43" s="392"/>
+      <c r="M43" s="393"/>
+      <c r="N43" s="393"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -6711,7 +6724,7 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="394"/>
+      <c r="B44" s="395"/>
       <c r="C44" s="190" t="s">
         <v>218</v>
       </c>
@@ -6727,7 +6740,7 @@
       <c r="G44" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H44" s="392"/>
+      <c r="H44" s="393"/>
       <c r="I44" s="111">
         <v>1</v>
       </c>
@@ -6740,8 +6753,8 @@
       <c r="L44" s="189">
         <v>1</v>
       </c>
-      <c r="M44" s="392"/>
-      <c r="N44" s="392"/>
+      <c r="M44" s="393"/>
+      <c r="N44" s="393"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -6787,7 +6800,7 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="394"/>
+      <c r="B45" s="395"/>
       <c r="C45" s="190" t="s">
         <v>219</v>
       </c>
@@ -6803,7 +6816,7 @@
       <c r="G45" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H45" s="392"/>
+      <c r="H45" s="393"/>
       <c r="I45" s="111">
         <v>1</v>
       </c>
@@ -6816,8 +6829,8 @@
       <c r="L45" s="189">
         <v>1</v>
       </c>
-      <c r="M45" s="392"/>
-      <c r="N45" s="392"/>
+      <c r="M45" s="393"/>
+      <c r="N45" s="393"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -6863,19 +6876,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="394"/>
+      <c r="B46" s="395"/>
       <c r="C46" s="190"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="189"/>
       <c r="G46" s="189"/>
-      <c r="H46" s="392"/>
+      <c r="H46" s="393"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="189"/>
       <c r="L46" s="189"/>
-      <c r="M46" s="392"/>
-      <c r="N46" s="395"/>
+      <c r="M46" s="393"/>
+      <c r="N46" s="396"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -6921,19 +6934,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="394"/>
+      <c r="B47" s="395"/>
       <c r="C47" s="190"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="392"/>
+      <c r="H47" s="393"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="392"/>
-      <c r="N47" s="396"/>
+      <c r="M47" s="393"/>
+      <c r="N47" s="397"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -6981,19 +6994,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="394"/>
+      <c r="B48" s="395"/>
       <c r="C48" s="190"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="392"/>
+      <c r="H48" s="393"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="392"/>
-      <c r="N48" s="396"/>
+      <c r="M48" s="393"/>
+      <c r="N48" s="397"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -7041,19 +7054,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="394"/>
+      <c r="B49" s="395"/>
       <c r="C49" s="190"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="392"/>
+      <c r="H49" s="393"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="392"/>
-      <c r="N49" s="396"/>
+      <c r="M49" s="393"/>
+      <c r="N49" s="397"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -7101,19 +7114,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="397"/>
+      <c r="B50" s="398"/>
       <c r="C50" s="191"/>
       <c r="D50" s="187"/>
       <c r="E50" s="187"/>
       <c r="F50" s="187"/>
       <c r="G50" s="187"/>
-      <c r="H50" s="398"/>
+      <c r="H50" s="399"/>
       <c r="I50" s="187"/>
       <c r="J50" s="187"/>
       <c r="K50" s="187"/>
       <c r="L50" s="187"/>
-      <c r="M50" s="398"/>
-      <c r="N50" s="399"/>
+      <c r="M50" s="399"/>
+      <c r="N50" s="400"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -7134,19 +7147,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="397"/>
+      <c r="B51" s="398"/>
       <c r="C51" s="191"/>
       <c r="D51" s="187"/>
       <c r="E51" s="187"/>
       <c r="F51" s="187"/>
       <c r="G51" s="187"/>
-      <c r="H51" s="398"/>
+      <c r="H51" s="399"/>
       <c r="I51" s="187"/>
       <c r="J51" s="187"/>
       <c r="K51" s="187"/>
       <c r="L51" s="187"/>
-      <c r="M51" s="398"/>
-      <c r="N51" s="400"/>
+      <c r="M51" s="399"/>
+      <c r="N51" s="401"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -7177,19 +7190,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="397"/>
+      <c r="B52" s="398"/>
       <c r="C52" s="191"/>
       <c r="D52" s="187"/>
       <c r="E52" s="187"/>
       <c r="F52" s="187"/>
       <c r="G52" s="187"/>
-      <c r="H52" s="398"/>
+      <c r="H52" s="399"/>
       <c r="I52" s="187"/>
       <c r="J52" s="187"/>
       <c r="K52" s="187"/>
       <c r="L52" s="187"/>
-      <c r="M52" s="398"/>
-      <c r="N52" s="400"/>
+      <c r="M52" s="399"/>
+      <c r="N52" s="401"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -7253,19 +7266,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="397"/>
+      <c r="B53" s="398"/>
       <c r="C53" s="191"/>
       <c r="D53" s="187"/>
       <c r="E53" s="187"/>
       <c r="F53" s="187"/>
       <c r="G53" s="187"/>
-      <c r="H53" s="398"/>
+      <c r="H53" s="399"/>
       <c r="I53" s="187"/>
       <c r="J53" s="187"/>
       <c r="K53" s="187"/>
       <c r="L53" s="187"/>
-      <c r="M53" s="398"/>
-      <c r="N53" s="400"/>
+      <c r="M53" s="399"/>
+      <c r="N53" s="401"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -7314,19 +7327,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="397"/>
+      <c r="B54" s="398"/>
       <c r="C54" s="191"/>
       <c r="D54" s="187"/>
       <c r="E54" s="187"/>
       <c r="F54" s="187"/>
       <c r="G54" s="187"/>
-      <c r="H54" s="398"/>
+      <c r="H54" s="399"/>
       <c r="I54" s="187"/>
       <c r="J54" s="187"/>
       <c r="K54" s="187"/>
       <c r="L54" s="187"/>
-      <c r="M54" s="398"/>
-      <c r="N54" s="401"/>
+      <c r="M54" s="399"/>
+      <c r="N54" s="402"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -7373,19 +7386,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="397"/>
+      <c r="B55" s="398"/>
       <c r="C55" s="191"/>
       <c r="D55" s="187"/>
       <c r="E55" s="187"/>
       <c r="F55" s="187"/>
       <c r="G55" s="187"/>
-      <c r="H55" s="398"/>
+      <c r="H55" s="399"/>
       <c r="I55" s="187"/>
       <c r="J55" s="187"/>
       <c r="K55" s="187"/>
       <c r="L55" s="187"/>
-      <c r="M55" s="398"/>
-      <c r="N55" s="400"/>
+      <c r="M55" s="399"/>
+      <c r="N55" s="401"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -7432,19 +7445,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="397"/>
+      <c r="B56" s="398"/>
       <c r="C56" s="191"/>
       <c r="D56" s="187"/>
       <c r="E56" s="187"/>
       <c r="F56" s="187"/>
       <c r="G56" s="187"/>
-      <c r="H56" s="398"/>
+      <c r="H56" s="399"/>
       <c r="I56" s="187"/>
       <c r="J56" s="187"/>
       <c r="K56" s="187"/>
       <c r="L56" s="187"/>
-      <c r="M56" s="398"/>
-      <c r="N56" s="400"/>
+      <c r="M56" s="399"/>
+      <c r="N56" s="401"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -7491,19 +7504,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="397"/>
+      <c r="B57" s="398"/>
       <c r="C57" s="191"/>
       <c r="D57" s="187"/>
       <c r="E57" s="187"/>
       <c r="F57" s="187"/>
       <c r="G57" s="187"/>
-      <c r="H57" s="398"/>
+      <c r="H57" s="399"/>
       <c r="I57" s="187"/>
       <c r="J57" s="187"/>
       <c r="K57" s="187"/>
       <c r="L57" s="187"/>
-      <c r="M57" s="398"/>
-      <c r="N57" s="400"/>
+      <c r="M57" s="399"/>
+      <c r="N57" s="401"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -7550,19 +7563,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="402"/>
+      <c r="B58" s="403"/>
       <c r="C58" s="185"/>
       <c r="D58" s="192"/>
       <c r="E58" s="192"/>
       <c r="F58" s="192"/>
       <c r="G58" s="192"/>
-      <c r="H58" s="403"/>
+      <c r="H58" s="404"/>
       <c r="I58" s="192"/>
       <c r="J58" s="192"/>
       <c r="K58" s="192"/>
       <c r="L58" s="192"/>
-      <c r="M58" s="403"/>
-      <c r="N58" s="404"/>
+      <c r="M58" s="404"/>
+      <c r="N58" s="405"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -7609,19 +7622,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="402"/>
+      <c r="B59" s="403"/>
       <c r="C59" s="185"/>
       <c r="D59" s="192"/>
       <c r="E59" s="192"/>
       <c r="F59" s="192"/>
       <c r="G59" s="192"/>
-      <c r="H59" s="403"/>
+      <c r="H59" s="404"/>
       <c r="I59" s="192"/>
       <c r="J59" s="192"/>
       <c r="K59" s="192"/>
       <c r="L59" s="192"/>
-      <c r="M59" s="403"/>
-      <c r="N59" s="405"/>
+      <c r="M59" s="404"/>
+      <c r="N59" s="406"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -7668,19 +7681,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="402"/>
+      <c r="B60" s="403"/>
       <c r="C60" s="185"/>
       <c r="D60" s="192"/>
       <c r="E60" s="192"/>
       <c r="F60" s="192"/>
       <c r="G60" s="192"/>
-      <c r="H60" s="403"/>
+      <c r="H60" s="404"/>
       <c r="I60" s="192"/>
       <c r="J60" s="192"/>
       <c r="K60" s="192"/>
       <c r="L60" s="192"/>
-      <c r="M60" s="403"/>
-      <c r="N60" s="405"/>
+      <c r="M60" s="404"/>
+      <c r="N60" s="406"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -7727,247 +7740,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="402"/>
+      <c r="B61" s="403"/>
       <c r="C61" s="185"/>
       <c r="D61" s="192"/>
       <c r="E61" s="192"/>
       <c r="F61" s="192"/>
       <c r="G61" s="192"/>
-      <c r="H61" s="403"/>
+      <c r="H61" s="404"/>
       <c r="I61" s="192"/>
       <c r="J61" s="192"/>
       <c r="K61" s="192"/>
       <c r="L61" s="192"/>
-      <c r="M61" s="403"/>
-      <c r="N61" s="405"/>
+      <c r="M61" s="404"/>
+      <c r="N61" s="406"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="402"/>
+      <c r="B62" s="403"/>
       <c r="C62" s="185"/>
       <c r="D62" s="192"/>
       <c r="E62" s="192"/>
       <c r="F62" s="192"/>
       <c r="G62" s="192"/>
-      <c r="H62" s="403"/>
+      <c r="H62" s="404"/>
       <c r="I62" s="192"/>
       <c r="J62" s="192"/>
       <c r="K62" s="192"/>
       <c r="L62" s="192"/>
-      <c r="M62" s="403"/>
-      <c r="N62" s="410"/>
+      <c r="M62" s="404"/>
+      <c r="N62" s="411"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="402"/>
+      <c r="B63" s="403"/>
       <c r="C63" s="185"/>
       <c r="D63" s="192"/>
       <c r="E63" s="192"/>
       <c r="F63" s="192"/>
       <c r="G63" s="192"/>
-      <c r="H63" s="403"/>
+      <c r="H63" s="404"/>
       <c r="I63" s="192"/>
       <c r="J63" s="192"/>
       <c r="K63" s="192"/>
       <c r="L63" s="192"/>
-      <c r="M63" s="403"/>
-      <c r="N63" s="405"/>
+      <c r="M63" s="404"/>
+      <c r="N63" s="406"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="402"/>
+      <c r="B64" s="403"/>
       <c r="C64" s="185"/>
       <c r="D64" s="192"/>
       <c r="E64" s="192"/>
       <c r="F64" s="192"/>
       <c r="G64" s="192"/>
-      <c r="H64" s="403"/>
+      <c r="H64" s="404"/>
       <c r="I64" s="192"/>
       <c r="J64" s="192"/>
       <c r="K64" s="192"/>
       <c r="L64" s="192"/>
-      <c r="M64" s="403"/>
-      <c r="N64" s="405"/>
+      <c r="M64" s="404"/>
+      <c r="N64" s="406"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="402"/>
+      <c r="B65" s="403"/>
       <c r="C65" s="185"/>
       <c r="D65" s="192"/>
       <c r="E65" s="192"/>
       <c r="F65" s="192"/>
       <c r="G65" s="192"/>
-      <c r="H65" s="403"/>
+      <c r="H65" s="404"/>
       <c r="I65" s="192"/>
       <c r="J65" s="192"/>
       <c r="K65" s="192"/>
       <c r="L65" s="192"/>
-      <c r="M65" s="403"/>
-      <c r="N65" s="405"/>
+      <c r="M65" s="404"/>
+      <c r="N65" s="406"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="406"/>
+      <c r="B66" s="407"/>
       <c r="C66" s="186"/>
       <c r="D66" s="188"/>
       <c r="E66" s="188"/>
       <c r="F66" s="188"/>
       <c r="G66" s="188"/>
-      <c r="H66" s="407"/>
+      <c r="H66" s="408"/>
       <c r="I66" s="188"/>
       <c r="J66" s="188"/>
       <c r="K66" s="188"/>
       <c r="L66" s="188"/>
-      <c r="M66" s="407"/>
-      <c r="N66" s="411"/>
+      <c r="M66" s="408"/>
+      <c r="N66" s="412"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="406"/>
+      <c r="B67" s="407"/>
       <c r="C67" s="186"/>
       <c r="D67" s="188"/>
       <c r="E67" s="188"/>
       <c r="F67" s="188"/>
       <c r="G67" s="188"/>
-      <c r="H67" s="407"/>
+      <c r="H67" s="408"/>
       <c r="I67" s="188"/>
       <c r="J67" s="188"/>
       <c r="K67" s="188"/>
       <c r="L67" s="188"/>
-      <c r="M67" s="407"/>
-      <c r="N67" s="409"/>
+      <c r="M67" s="408"/>
+      <c r="N67" s="410"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="406"/>
+      <c r="B68" s="407"/>
       <c r="C68" s="186"/>
       <c r="D68" s="188"/>
       <c r="E68" s="188"/>
       <c r="F68" s="188"/>
       <c r="G68" s="188"/>
-      <c r="H68" s="407"/>
+      <c r="H68" s="408"/>
       <c r="I68" s="188"/>
       <c r="J68" s="188"/>
       <c r="K68" s="188"/>
       <c r="L68" s="188"/>
-      <c r="M68" s="407"/>
-      <c r="N68" s="409"/>
+      <c r="M68" s="408"/>
+      <c r="N68" s="410"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="406"/>
+      <c r="B69" s="407"/>
       <c r="C69" s="186"/>
       <c r="D69" s="188"/>
       <c r="E69" s="188"/>
       <c r="F69" s="188"/>
       <c r="G69" s="188"/>
-      <c r="H69" s="407"/>
+      <c r="H69" s="408"/>
       <c r="I69" s="188"/>
       <c r="J69" s="188"/>
       <c r="K69" s="188"/>
       <c r="L69" s="188"/>
-      <c r="M69" s="407"/>
-      <c r="N69" s="409"/>
+      <c r="M69" s="408"/>
+      <c r="N69" s="410"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="406"/>
+      <c r="B70" s="407"/>
       <c r="C70" s="186"/>
       <c r="D70" s="188"/>
       <c r="E70" s="188"/>
       <c r="F70" s="188"/>
       <c r="G70" s="188"/>
-      <c r="H70" s="407"/>
+      <c r="H70" s="408"/>
       <c r="I70" s="188"/>
       <c r="J70" s="188"/>
       <c r="K70" s="188"/>
       <c r="L70" s="188"/>
-      <c r="M70" s="407"/>
-      <c r="N70" s="408"/>
+      <c r="M70" s="408"/>
+      <c r="N70" s="409"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="406"/>
+      <c r="B71" s="407"/>
       <c r="C71" s="186"/>
       <c r="D71" s="188"/>
       <c r="E71" s="188"/>
       <c r="F71" s="188"/>
       <c r="G71" s="188"/>
-      <c r="H71" s="407"/>
+      <c r="H71" s="408"/>
       <c r="I71" s="188"/>
       <c r="J71" s="188"/>
       <c r="K71" s="188"/>
       <c r="L71" s="188"/>
-      <c r="M71" s="407"/>
-      <c r="N71" s="409"/>
+      <c r="M71" s="408"/>
+      <c r="N71" s="410"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="406"/>
+      <c r="B72" s="407"/>
       <c r="C72" s="186"/>
       <c r="D72" s="188"/>
       <c r="E72" s="188"/>
       <c r="F72" s="188"/>
       <c r="G72" s="188"/>
-      <c r="H72" s="407"/>
+      <c r="H72" s="408"/>
       <c r="I72" s="188"/>
       <c r="J72" s="188"/>
       <c r="K72" s="188"/>
       <c r="L72" s="188"/>
-      <c r="M72" s="407"/>
-      <c r="N72" s="409"/>
+      <c r="M72" s="408"/>
+      <c r="N72" s="410"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="406"/>
+      <c r="B73" s="407"/>
       <c r="C73" s="186"/>
       <c r="D73" s="188"/>
       <c r="E73" s="188"/>
       <c r="F73" s="188"/>
       <c r="G73" s="188"/>
-      <c r="H73" s="407"/>
+      <c r="H73" s="408"/>
       <c r="I73" s="188"/>
       <c r="J73" s="188"/>
       <c r="K73" s="188"/>
       <c r="L73" s="188"/>
-      <c r="M73" s="407"/>
-      <c r="N73" s="409"/>
+      <c r="M73" s="408"/>
+      <c r="N73" s="410"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>
@@ -9621,14 +9634,14 @@
   <dimension ref="A1:AU434"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B45"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27" style="22" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.5703125" style="22" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="33.5703125" style="22" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" style="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25" style="22" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="36.140625" style="22" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="30.5703125" style="22" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="21.42578125" style="22" customWidth="1" collapsed="1"/>
@@ -9669,15 +9682,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="371" t="s">
+      <c r="F1" s="372" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="371"/>
-      <c r="H1" s="371"/>
-      <c r="I1" s="371"/>
-      <c r="J1" s="371"/>
-      <c r="K1" s="371"/>
-      <c r="L1" s="371"/>
+      <c r="G1" s="372"/>
+      <c r="H1" s="372"/>
+      <c r="I1" s="372"/>
+      <c r="J1" s="372"/>
+      <c r="K1" s="372"/>
+      <c r="L1" s="372"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -9726,22 +9739,22 @@
       <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="372" t="s">
+      <c r="D6" s="373" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="373"/>
-      <c r="F6" s="373"/>
-      <c r="G6" s="373"/>
-      <c r="H6" s="374"/>
+      <c r="E6" s="374"/>
+      <c r="F6" s="374"/>
+      <c r="G6" s="374"/>
+      <c r="H6" s="375"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="372" t="s">
+      <c r="M6" s="373" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="373"/>
-      <c r="O6" s="373"/>
-      <c r="P6" s="373"/>
-      <c r="Q6" s="374"/>
+      <c r="N6" s="374"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="374"/>
+      <c r="Q6" s="375"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -9759,10 +9772,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="375" t="s">
+      <c r="F7" s="376" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="376"/>
+      <c r="G7" s="377"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -9785,10 +9798,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="375" t="s">
+      <c r="P7" s="376" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="376"/>
+      <c r="Q7" s="377"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -9856,7 +9869,7 @@
     </row>
     <row r="9" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="39"/>
-      <c r="B9" s="377"/>
+      <c r="B9" s="378"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
       <c r="E9" s="40"/>
@@ -9867,15 +9880,15 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="42"/>
-      <c r="M9" s="368"/>
-      <c r="N9" s="380"/>
-      <c r="O9" s="368"/>
-      <c r="P9" s="368"/>
-      <c r="Q9" s="368"/>
-      <c r="R9" s="368"/>
-      <c r="S9" s="368"/>
-      <c r="T9" s="383"/>
-      <c r="U9" s="368"/>
+      <c r="M9" s="369"/>
+      <c r="N9" s="381"/>
+      <c r="O9" s="369"/>
+      <c r="P9" s="369"/>
+      <c r="Q9" s="369"/>
+      <c r="R9" s="369"/>
+      <c r="S9" s="369"/>
+      <c r="T9" s="384"/>
+      <c r="U9" s="369"/>
       <c r="V9" s="41"/>
       <c r="W9" s="36"/>
       <c r="X9" s="36"/>
@@ -9885,7 +9898,7 @@
     </row>
     <row r="10" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
-      <c r="B10" s="378"/>
+      <c r="B10" s="379"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
@@ -9896,15 +9909,15 @@
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="42"/>
-      <c r="M10" s="369"/>
-      <c r="N10" s="381"/>
-      <c r="O10" s="369"/>
-      <c r="P10" s="369"/>
-      <c r="Q10" s="369"/>
-      <c r="R10" s="369"/>
-      <c r="S10" s="369"/>
-      <c r="T10" s="384"/>
-      <c r="U10" s="369"/>
+      <c r="M10" s="370"/>
+      <c r="N10" s="382"/>
+      <c r="O10" s="370"/>
+      <c r="P10" s="370"/>
+      <c r="Q10" s="370"/>
+      <c r="R10" s="370"/>
+      <c r="S10" s="370"/>
+      <c r="T10" s="385"/>
+      <c r="U10" s="370"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -9912,8 +9925,8 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="368"/>
-      <c r="B11" s="378"/>
+      <c r="A11" s="369"/>
+      <c r="B11" s="379"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -9924,15 +9937,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="369"/>
-      <c r="N11" s="381"/>
-      <c r="O11" s="369"/>
-      <c r="P11" s="369"/>
-      <c r="Q11" s="369"/>
-      <c r="R11" s="369"/>
-      <c r="S11" s="369"/>
-      <c r="T11" s="384"/>
-      <c r="U11" s="369"/>
+      <c r="M11" s="370"/>
+      <c r="N11" s="382"/>
+      <c r="O11" s="370"/>
+      <c r="P11" s="370"/>
+      <c r="Q11" s="370"/>
+      <c r="R11" s="370"/>
+      <c r="S11" s="370"/>
+      <c r="T11" s="385"/>
+      <c r="U11" s="370"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -9942,8 +9955,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="370"/>
-      <c r="B12" s="379"/>
+      <c r="A12" s="371"/>
+      <c r="B12" s="380"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -9954,15 +9967,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="370"/>
-      <c r="N12" s="382"/>
-      <c r="O12" s="370"/>
-      <c r="P12" s="370"/>
-      <c r="Q12" s="370"/>
-      <c r="R12" s="370"/>
-      <c r="S12" s="370"/>
-      <c r="T12" s="385"/>
-      <c r="U12" s="370"/>
+      <c r="M12" s="371"/>
+      <c r="N12" s="383"/>
+      <c r="O12" s="371"/>
+      <c r="P12" s="371"/>
+      <c r="Q12" s="371"/>
+      <c r="R12" s="371"/>
+      <c r="S12" s="371"/>
+      <c r="T12" s="386"/>
+      <c r="U12" s="371"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -9971,7 +9984,7 @@
     </row>
     <row r="13" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43"/>
-      <c r="B13" s="377"/>
+      <c r="B13" s="378"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
@@ -9982,15 +9995,15 @@
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="368"/>
-      <c r="N13" s="380"/>
-      <c r="O13" s="368"/>
-      <c r="P13" s="368"/>
-      <c r="Q13" s="368"/>
-      <c r="R13" s="368"/>
-      <c r="S13" s="368"/>
-      <c r="T13" s="383"/>
-      <c r="U13" s="368"/>
+      <c r="M13" s="369"/>
+      <c r="N13" s="381"/>
+      <c r="O13" s="369"/>
+      <c r="P13" s="369"/>
+      <c r="Q13" s="369"/>
+      <c r="R13" s="369"/>
+      <c r="S13" s="369"/>
+      <c r="T13" s="384"/>
+      <c r="U13" s="369"/>
       <c r="V13" s="41"/>
       <c r="W13" s="36"/>
       <c r="X13" s="36"/>
@@ -9999,7 +10012,7 @@
     </row>
     <row r="14" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44"/>
-      <c r="B14" s="378"/>
+      <c r="B14" s="379"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
@@ -10010,15 +10023,15 @@
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
       <c r="L14" s="42"/>
-      <c r="M14" s="369"/>
-      <c r="N14" s="381"/>
-      <c r="O14" s="369"/>
-      <c r="P14" s="369"/>
-      <c r="Q14" s="369"/>
-      <c r="R14" s="369"/>
-      <c r="S14" s="369"/>
-      <c r="T14" s="384"/>
-      <c r="U14" s="369"/>
+      <c r="M14" s="370"/>
+      <c r="N14" s="382"/>
+      <c r="O14" s="370"/>
+      <c r="P14" s="370"/>
+      <c r="Q14" s="370"/>
+      <c r="R14" s="370"/>
+      <c r="S14" s="370"/>
+      <c r="T14" s="385"/>
+      <c r="U14" s="370"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -10026,8 +10039,8 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="386"/>
-      <c r="B15" s="378"/>
+      <c r="A15" s="387"/>
+      <c r="B15" s="379"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -10038,15 +10051,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="369"/>
-      <c r="N15" s="381"/>
-      <c r="O15" s="369"/>
-      <c r="P15" s="369"/>
-      <c r="Q15" s="369"/>
-      <c r="R15" s="369"/>
-      <c r="S15" s="369"/>
-      <c r="T15" s="384"/>
-      <c r="U15" s="369"/>
+      <c r="M15" s="370"/>
+      <c r="N15" s="382"/>
+      <c r="O15" s="370"/>
+      <c r="P15" s="370"/>
+      <c r="Q15" s="370"/>
+      <c r="R15" s="370"/>
+      <c r="S15" s="370"/>
+      <c r="T15" s="385"/>
+      <c r="U15" s="370"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -10054,8 +10067,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="387"/>
-      <c r="B16" s="379"/>
+      <c r="A16" s="388"/>
+      <c r="B16" s="380"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -10066,15 +10079,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="370"/>
-      <c r="N16" s="382"/>
-      <c r="O16" s="370"/>
-      <c r="P16" s="370"/>
-      <c r="Q16" s="370"/>
-      <c r="R16" s="370"/>
-      <c r="S16" s="370"/>
-      <c r="T16" s="385"/>
-      <c r="U16" s="370"/>
+      <c r="M16" s="371"/>
+      <c r="N16" s="383"/>
+      <c r="O16" s="371"/>
+      <c r="P16" s="371"/>
+      <c r="Q16" s="371"/>
+      <c r="R16" s="371"/>
+      <c r="S16" s="371"/>
+      <c r="T16" s="386"/>
+      <c r="U16" s="371"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -10083,7 +10096,7 @@
     </row>
     <row r="17" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
-      <c r="B17" s="377"/>
+      <c r="B17" s="378"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="40"/>
@@ -10094,15 +10107,15 @@
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="368"/>
-      <c r="N17" s="380"/>
-      <c r="O17" s="368"/>
-      <c r="P17" s="368"/>
-      <c r="Q17" s="368"/>
-      <c r="R17" s="368"/>
-      <c r="S17" s="368"/>
-      <c r="T17" s="383"/>
-      <c r="U17" s="368"/>
+      <c r="M17" s="369"/>
+      <c r="N17" s="381"/>
+      <c r="O17" s="369"/>
+      <c r="P17" s="369"/>
+      <c r="Q17" s="369"/>
+      <c r="R17" s="369"/>
+      <c r="S17" s="369"/>
+      <c r="T17" s="384"/>
+      <c r="U17" s="369"/>
       <c r="V17" s="41"/>
       <c r="W17" s="36"/>
       <c r="X17" s="36"/>
@@ -10111,7 +10124,7 @@
     </row>
     <row r="18" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40"/>
-      <c r="B18" s="378"/>
+      <c r="B18" s="379"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
       <c r="E18" s="40"/>
@@ -10122,22 +10135,22 @@
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="369"/>
-      <c r="N18" s="381"/>
-      <c r="O18" s="369"/>
-      <c r="P18" s="369"/>
-      <c r="Q18" s="369"/>
-      <c r="R18" s="369"/>
-      <c r="S18" s="369"/>
-      <c r="T18" s="384"/>
-      <c r="U18" s="369"/>
+      <c r="M18" s="370"/>
+      <c r="N18" s="382"/>
+      <c r="O18" s="370"/>
+      <c r="P18" s="370"/>
+      <c r="Q18" s="370"/>
+      <c r="R18" s="370"/>
+      <c r="S18" s="370"/>
+      <c r="T18" s="385"/>
+      <c r="U18" s="370"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="368"/>
-      <c r="B19" s="378"/>
+      <c r="A19" s="369"/>
+      <c r="B19" s="379"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -10148,22 +10161,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="369"/>
-      <c r="N19" s="381"/>
-      <c r="O19" s="369"/>
-      <c r="P19" s="369"/>
-      <c r="Q19" s="369"/>
-      <c r="R19" s="369"/>
-      <c r="S19" s="369"/>
-      <c r="T19" s="384"/>
-      <c r="U19" s="369"/>
+      <c r="M19" s="370"/>
+      <c r="N19" s="382"/>
+      <c r="O19" s="370"/>
+      <c r="P19" s="370"/>
+      <c r="Q19" s="370"/>
+      <c r="R19" s="370"/>
+      <c r="S19" s="370"/>
+      <c r="T19" s="385"/>
+      <c r="U19" s="370"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="370"/>
-      <c r="B20" s="379"/>
+      <c r="A20" s="371"/>
+      <c r="B20" s="380"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -10174,22 +10187,22 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="370"/>
-      <c r="N20" s="382"/>
-      <c r="O20" s="370"/>
-      <c r="P20" s="370"/>
-      <c r="Q20" s="370"/>
-      <c r="R20" s="370"/>
-      <c r="S20" s="370"/>
-      <c r="T20" s="385"/>
-      <c r="U20" s="370"/>
+      <c r="M20" s="371"/>
+      <c r="N20" s="383"/>
+      <c r="O20" s="371"/>
+      <c r="P20" s="371"/>
+      <c r="Q20" s="371"/>
+      <c r="R20" s="371"/>
+      <c r="S20" s="371"/>
+      <c r="T20" s="386"/>
+      <c r="U20" s="371"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
     </row>
     <row r="21" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="39"/>
-      <c r="B21" s="377"/>
+      <c r="B21" s="378"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
@@ -10200,22 +10213,22 @@
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
       <c r="L21" s="42"/>
-      <c r="M21" s="368"/>
-      <c r="N21" s="380"/>
-      <c r="O21" s="368"/>
-      <c r="P21" s="368"/>
-      <c r="Q21" s="368"/>
-      <c r="R21" s="368"/>
-      <c r="S21" s="368"/>
-      <c r="T21" s="383"/>
-      <c r="U21" s="368"/>
+      <c r="M21" s="369"/>
+      <c r="N21" s="381"/>
+      <c r="O21" s="369"/>
+      <c r="P21" s="369"/>
+      <c r="Q21" s="369"/>
+      <c r="R21" s="369"/>
+      <c r="S21" s="369"/>
+      <c r="T21" s="384"/>
+      <c r="U21" s="369"/>
       <c r="V21" s="41"/>
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
     </row>
     <row r="22" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
-      <c r="B22" s="378"/>
+      <c r="B22" s="379"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
@@ -10226,22 +10239,22 @@
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
       <c r="L22" s="42"/>
-      <c r="M22" s="369"/>
-      <c r="N22" s="381"/>
-      <c r="O22" s="369"/>
-      <c r="P22" s="369"/>
-      <c r="Q22" s="369"/>
-      <c r="R22" s="369"/>
-      <c r="S22" s="369"/>
-      <c r="T22" s="384"/>
-      <c r="U22" s="369"/>
+      <c r="M22" s="370"/>
+      <c r="N22" s="382"/>
+      <c r="O22" s="370"/>
+      <c r="P22" s="370"/>
+      <c r="Q22" s="370"/>
+      <c r="R22" s="370"/>
+      <c r="S22" s="370"/>
+      <c r="T22" s="385"/>
+      <c r="U22" s="370"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="388"/>
-      <c r="B23" s="378"/>
+      <c r="A23" s="389"/>
+      <c r="B23" s="379"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -10252,22 +10265,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="369"/>
-      <c r="N23" s="381"/>
-      <c r="O23" s="369"/>
-      <c r="P23" s="369"/>
-      <c r="Q23" s="369"/>
-      <c r="R23" s="369"/>
-      <c r="S23" s="369"/>
-      <c r="T23" s="384"/>
-      <c r="U23" s="369"/>
+      <c r="M23" s="370"/>
+      <c r="N23" s="382"/>
+      <c r="O23" s="370"/>
+      <c r="P23" s="370"/>
+      <c r="Q23" s="370"/>
+      <c r="R23" s="370"/>
+      <c r="S23" s="370"/>
+      <c r="T23" s="385"/>
+      <c r="U23" s="370"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="389"/>
-      <c r="B24" s="379"/>
+      <c r="A24" s="390"/>
+      <c r="B24" s="380"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -10278,15 +10291,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="370"/>
-      <c r="N24" s="382"/>
-      <c r="O24" s="370"/>
-      <c r="P24" s="370"/>
-      <c r="Q24" s="370"/>
-      <c r="R24" s="370"/>
-      <c r="S24" s="370"/>
-      <c r="T24" s="385"/>
-      <c r="U24" s="370"/>
+      <c r="M24" s="371"/>
+      <c r="N24" s="383"/>
+      <c r="O24" s="371"/>
+      <c r="P24" s="371"/>
+      <c r="Q24" s="371"/>
+      <c r="R24" s="371"/>
+      <c r="S24" s="371"/>
+      <c r="T24" s="386"/>
+      <c r="U24" s="371"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -10476,13 +10489,17 @@
       <c r="J37" s="46"/>
       <c r="K37" s="46"/>
     </row>
-    <row r="38" spans="1:41" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A39" s="22">
-        <v>0</v>
-      </c>
-      <c r="B39" s="22">
-        <v>1</v>
+    <row r="38" spans="1:41" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="428" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="368" t="s">
+        <v>242</v>
+      </c>
+      <c r="B39" s="368" t="s">
+        <v>241</v>
       </c>
       <c r="C39" s="22">
         <v>2</v>
@@ -10594,40 +10611,40 @@
     </row>
     <row r="40" spans="1:41" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="366" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B40" s="367" t="s">
         <v>240</v>
       </c>
       <c r="D40" s="104"/>
       <c r="E40" s="105"/>
-      <c r="F40" s="413" t="s">
+      <c r="F40" s="414" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="414"/>
-      <c r="H40" s="414"/>
-      <c r="I40" s="415"/>
-      <c r="J40" s="416" t="s">
+      <c r="G40" s="415"/>
+      <c r="H40" s="415"/>
+      <c r="I40" s="416"/>
+      <c r="J40" s="417" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="417"/>
-      <c r="L40" s="417"/>
-      <c r="M40" s="418"/>
+      <c r="K40" s="418"/>
+      <c r="L40" s="418"/>
+      <c r="M40" s="419"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
       </c>
       <c r="P40" s="227"/>
-      <c r="Q40" s="412" t="s">
+      <c r="Q40" s="413" t="s">
         <v>234</v>
       </c>
-      <c r="R40" s="412"/>
-      <c r="S40" s="412"/>
-      <c r="T40" s="412"/>
-      <c r="U40" s="412"/>
-      <c r="V40" s="412"/>
-      <c r="W40" s="412"/>
-      <c r="X40" s="412"/>
-      <c r="Y40" s="412"/>
+      <c r="R40" s="413"/>
+      <c r="S40" s="413"/>
+      <c r="T40" s="413"/>
+      <c r="U40" s="413"/>
+      <c r="V40" s="413"/>
+      <c r="W40" s="413"/>
+      <c r="X40" s="413"/>
+      <c r="Y40" s="413"/>
       <c r="Z40" s="46"/>
       <c r="AA40" s="46"/>
       <c r="AB40" s="46"/>
@@ -10755,7 +10772,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="310" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34"/>
@@ -10801,7 +10818,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="310" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
@@ -18356,12 +18373,15 @@
     <mergeCell ref="P9:P12"/>
     <mergeCell ref="Q9:Q12"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">
       <formula1>"daily,week,month"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
       <formula1>"Solid,Liquid,Inhalant,Patch,Topical"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A40">
+      <formula1>"Manual,Campaign"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18413,15 +18433,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="371" t="s">
+      <c r="F1" s="372" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="371"/>
-      <c r="H1" s="371"/>
-      <c r="I1" s="371"/>
-      <c r="J1" s="371"/>
-      <c r="K1" s="371"/>
-      <c r="L1" s="371"/>
+      <c r="G1" s="372"/>
+      <c r="H1" s="372"/>
+      <c r="I1" s="372"/>
+      <c r="J1" s="372"/>
+      <c r="K1" s="372"/>
+      <c r="L1" s="372"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -18510,22 +18530,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="372" t="s">
+      <c r="D6" s="373" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="373"/>
-      <c r="F6" s="373"/>
-      <c r="G6" s="373"/>
-      <c r="H6" s="374"/>
+      <c r="E6" s="374"/>
+      <c r="F6" s="374"/>
+      <c r="G6" s="374"/>
+      <c r="H6" s="375"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="372" t="s">
+      <c r="M6" s="373" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="373"/>
-      <c r="O6" s="373"/>
-      <c r="P6" s="373"/>
-      <c r="Q6" s="374"/>
+      <c r="N6" s="374"/>
+      <c r="O6" s="374"/>
+      <c r="P6" s="374"/>
+      <c r="Q6" s="375"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -18543,10 +18563,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="375" t="s">
+      <c r="F7" s="376" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="376"/>
+      <c r="G7" s="377"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -18569,10 +18589,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="375" t="s">
+      <c r="P7" s="376" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="376"/>
+      <c r="Q7" s="377"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -18649,7 +18669,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="377" t="s">
+      <c r="B9" s="378" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -18683,33 +18703,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="368">
+      <c r="M9" s="369">
         <v>20</v>
       </c>
-      <c r="N9" s="380" t="s">
+      <c r="N9" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="368">
+      <c r="O9" s="369">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="368">
+      <c r="P9" s="369">
         <v>3</v>
       </c>
-      <c r="Q9" s="368">
+      <c r="Q9" s="369">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="368">
+      <c r="R9" s="369">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="368"/>
-      <c r="T9" s="383">
+      <c r="S9" s="369"/>
+      <c r="T9" s="384">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="368">
+      <c r="U9" s="369">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -18734,7 +18754,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="378"/>
+      <c r="B10" s="379"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -18766,15 +18786,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="369"/>
-      <c r="N10" s="381"/>
-      <c r="O10" s="369"/>
-      <c r="P10" s="369"/>
-      <c r="Q10" s="369"/>
-      <c r="R10" s="369"/>
-      <c r="S10" s="369"/>
-      <c r="T10" s="384"/>
-      <c r="U10" s="369"/>
+      <c r="M10" s="370"/>
+      <c r="N10" s="382"/>
+      <c r="O10" s="370"/>
+      <c r="P10" s="370"/>
+      <c r="Q10" s="370"/>
+      <c r="R10" s="370"/>
+      <c r="S10" s="370"/>
+      <c r="T10" s="385"/>
+      <c r="U10" s="370"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -18782,10 +18802,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="368" t="s">
+      <c r="A11" s="369" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="378"/>
+      <c r="B11" s="379"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -18796,15 +18816,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="369"/>
-      <c r="N11" s="381"/>
-      <c r="O11" s="369"/>
-      <c r="P11" s="369"/>
-      <c r="Q11" s="369"/>
-      <c r="R11" s="369"/>
-      <c r="S11" s="369"/>
-      <c r="T11" s="384"/>
-      <c r="U11" s="369"/>
+      <c r="M11" s="370"/>
+      <c r="N11" s="382"/>
+      <c r="O11" s="370"/>
+      <c r="P11" s="370"/>
+      <c r="Q11" s="370"/>
+      <c r="R11" s="370"/>
+      <c r="S11" s="370"/>
+      <c r="T11" s="385"/>
+      <c r="U11" s="370"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -18823,8 +18843,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="370"/>
-      <c r="B12" s="379"/>
+      <c r="A12" s="371"/>
+      <c r="B12" s="380"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -18835,15 +18855,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="370"/>
-      <c r="N12" s="382"/>
-      <c r="O12" s="370"/>
-      <c r="P12" s="370"/>
-      <c r="Q12" s="370"/>
-      <c r="R12" s="370"/>
-      <c r="S12" s="370"/>
-      <c r="T12" s="385"/>
-      <c r="U12" s="370"/>
+      <c r="M12" s="371"/>
+      <c r="N12" s="383"/>
+      <c r="O12" s="371"/>
+      <c r="P12" s="371"/>
+      <c r="Q12" s="371"/>
+      <c r="R12" s="371"/>
+      <c r="S12" s="371"/>
+      <c r="T12" s="386"/>
+      <c r="U12" s="371"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -18859,7 +18879,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="377" t="s">
+      <c r="B13" s="378" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -18893,33 +18913,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="368">
+      <c r="M13" s="369">
         <v>80</v>
       </c>
-      <c r="N13" s="380" t="s">
+      <c r="N13" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="368">
+      <c r="O13" s="369">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="368">
+      <c r="P13" s="369">
         <v>2</v>
       </c>
-      <c r="Q13" s="368">
+      <c r="Q13" s="369">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="368">
+      <c r="R13" s="369">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="368"/>
-      <c r="T13" s="383">
+      <c r="S13" s="369"/>
+      <c r="T13" s="384">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="368">
+      <c r="U13" s="369">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -18942,7 +18962,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="378"/>
+      <c r="B14" s="379"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -18974,15 +18994,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="369"/>
-      <c r="N14" s="381"/>
-      <c r="O14" s="369"/>
-      <c r="P14" s="369"/>
-      <c r="Q14" s="369"/>
-      <c r="R14" s="369"/>
-      <c r="S14" s="369"/>
-      <c r="T14" s="384"/>
-      <c r="U14" s="369"/>
+      <c r="M14" s="370"/>
+      <c r="N14" s="382"/>
+      <c r="O14" s="370"/>
+      <c r="P14" s="370"/>
+      <c r="Q14" s="370"/>
+      <c r="R14" s="370"/>
+      <c r="S14" s="370"/>
+      <c r="T14" s="385"/>
+      <c r="U14" s="370"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -18990,10 +19010,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="386" t="s">
+      <c r="A15" s="387" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="378"/>
+      <c r="B15" s="379"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -19004,15 +19024,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="369"/>
-      <c r="N15" s="381"/>
-      <c r="O15" s="369"/>
-      <c r="P15" s="369"/>
-      <c r="Q15" s="369"/>
-      <c r="R15" s="369"/>
-      <c r="S15" s="369"/>
-      <c r="T15" s="384"/>
-      <c r="U15" s="369"/>
+      <c r="M15" s="370"/>
+      <c r="N15" s="382"/>
+      <c r="O15" s="370"/>
+      <c r="P15" s="370"/>
+      <c r="Q15" s="370"/>
+      <c r="R15" s="370"/>
+      <c r="S15" s="370"/>
+      <c r="T15" s="385"/>
+      <c r="U15" s="370"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -19022,8 +19042,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="387"/>
-      <c r="B16" s="379"/>
+      <c r="A16" s="388"/>
+      <c r="B16" s="380"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -19034,15 +19054,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="370"/>
-      <c r="N16" s="382"/>
-      <c r="O16" s="370"/>
-      <c r="P16" s="370"/>
-      <c r="Q16" s="370"/>
-      <c r="R16" s="370"/>
-      <c r="S16" s="370"/>
-      <c r="T16" s="385"/>
-      <c r="U16" s="370"/>
+      <c r="M16" s="371"/>
+      <c r="N16" s="383"/>
+      <c r="O16" s="371"/>
+      <c r="P16" s="371"/>
+      <c r="Q16" s="371"/>
+      <c r="R16" s="371"/>
+      <c r="S16" s="371"/>
+      <c r="T16" s="386"/>
+      <c r="U16" s="371"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -19053,7 +19073,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="377" t="s">
+      <c r="B17" s="378" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -19087,33 +19107,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="368">
+      <c r="M17" s="369">
         <v>70</v>
       </c>
-      <c r="N17" s="380" t="s">
+      <c r="N17" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="368">
+      <c r="O17" s="369">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="368">
+      <c r="P17" s="369">
         <v>2</v>
       </c>
-      <c r="Q17" s="368">
+      <c r="Q17" s="369">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="368">
+      <c r="R17" s="369">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="368"/>
-      <c r="T17" s="383">
+      <c r="S17" s="369"/>
+      <c r="T17" s="384">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="368">
+      <c r="U17" s="369">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -19132,7 +19152,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="378"/>
+      <c r="B18" s="379"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -19164,24 +19184,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="369"/>
-      <c r="N18" s="381"/>
-      <c r="O18" s="369"/>
-      <c r="P18" s="369"/>
-      <c r="Q18" s="369"/>
-      <c r="R18" s="369"/>
-      <c r="S18" s="369"/>
-      <c r="T18" s="384"/>
-      <c r="U18" s="369"/>
+      <c r="M18" s="370"/>
+      <c r="N18" s="382"/>
+      <c r="O18" s="370"/>
+      <c r="P18" s="370"/>
+      <c r="Q18" s="370"/>
+      <c r="R18" s="370"/>
+      <c r="S18" s="370"/>
+      <c r="T18" s="385"/>
+      <c r="U18" s="370"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="368" t="s">
+      <c r="A19" s="369" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="378"/>
+      <c r="B19" s="379"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -19192,22 +19212,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="369"/>
-      <c r="N19" s="381"/>
-      <c r="O19" s="369"/>
-      <c r="P19" s="369"/>
-      <c r="Q19" s="369"/>
-      <c r="R19" s="369"/>
-      <c r="S19" s="369"/>
-      <c r="T19" s="384"/>
-      <c r="U19" s="369"/>
+      <c r="M19" s="370"/>
+      <c r="N19" s="382"/>
+      <c r="O19" s="370"/>
+      <c r="P19" s="370"/>
+      <c r="Q19" s="370"/>
+      <c r="R19" s="370"/>
+      <c r="S19" s="370"/>
+      <c r="T19" s="385"/>
+      <c r="U19" s="370"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="370"/>
-      <c r="B20" s="379"/>
+      <c r="A20" s="371"/>
+      <c r="B20" s="380"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -19218,15 +19238,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="370"/>
-      <c r="N20" s="382"/>
-      <c r="O20" s="370"/>
-      <c r="P20" s="370"/>
-      <c r="Q20" s="370"/>
-      <c r="R20" s="370"/>
-      <c r="S20" s="370"/>
-      <c r="T20" s="385"/>
-      <c r="U20" s="370"/>
+      <c r="M20" s="371"/>
+      <c r="N20" s="383"/>
+      <c r="O20" s="371"/>
+      <c r="P20" s="371"/>
+      <c r="Q20" s="371"/>
+      <c r="R20" s="371"/>
+      <c r="S20" s="371"/>
+      <c r="T20" s="386"/>
+      <c r="U20" s="371"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -19235,7 +19255,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="377" t="s">
+      <c r="B21" s="378" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -19269,33 +19289,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="368">
+      <c r="M21" s="369">
         <v>60</v>
       </c>
-      <c r="N21" s="380" t="s">
+      <c r="N21" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="368">
+      <c r="O21" s="369">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="368">
+      <c r="P21" s="369">
         <v>3</v>
       </c>
-      <c r="Q21" s="368">
+      <c r="Q21" s="369">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="368">
+      <c r="R21" s="369">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="368"/>
-      <c r="T21" s="383">
+      <c r="S21" s="369"/>
+      <c r="T21" s="384">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="368">
+      <c r="U21" s="369">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -19312,7 +19332,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="378"/>
+      <c r="B22" s="379"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -19344,24 +19364,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="369"/>
-      <c r="N22" s="381"/>
-      <c r="O22" s="369"/>
-      <c r="P22" s="369"/>
-      <c r="Q22" s="369"/>
-      <c r="R22" s="369"/>
-      <c r="S22" s="369"/>
-      <c r="T22" s="384"/>
-      <c r="U22" s="369"/>
+      <c r="M22" s="370"/>
+      <c r="N22" s="382"/>
+      <c r="O22" s="370"/>
+      <c r="P22" s="370"/>
+      <c r="Q22" s="370"/>
+      <c r="R22" s="370"/>
+      <c r="S22" s="370"/>
+      <c r="T22" s="385"/>
+      <c r="U22" s="370"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="388" t="s">
+      <c r="A23" s="389" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="378"/>
+      <c r="B23" s="379"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -19372,22 +19392,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="369"/>
-      <c r="N23" s="381"/>
-      <c r="O23" s="369"/>
-      <c r="P23" s="369"/>
-      <c r="Q23" s="369"/>
-      <c r="R23" s="369"/>
-      <c r="S23" s="369"/>
-      <c r="T23" s="384"/>
-      <c r="U23" s="369"/>
+      <c r="M23" s="370"/>
+      <c r="N23" s="382"/>
+      <c r="O23" s="370"/>
+      <c r="P23" s="370"/>
+      <c r="Q23" s="370"/>
+      <c r="R23" s="370"/>
+      <c r="S23" s="370"/>
+      <c r="T23" s="385"/>
+      <c r="U23" s="370"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="389"/>
-      <c r="B24" s="379"/>
+      <c r="A24" s="390"/>
+      <c r="B24" s="380"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -19398,15 +19418,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="370"/>
-      <c r="N24" s="382"/>
-      <c r="O24" s="370"/>
-      <c r="P24" s="370"/>
-      <c r="Q24" s="370"/>
-      <c r="R24" s="370"/>
-      <c r="S24" s="370"/>
-      <c r="T24" s="385"/>
-      <c r="U24" s="370"/>
+      <c r="M24" s="371"/>
+      <c r="N24" s="383"/>
+      <c r="O24" s="371"/>
+      <c r="P24" s="371"/>
+      <c r="Q24" s="371"/>
+      <c r="R24" s="371"/>
+      <c r="S24" s="371"/>
+      <c r="T24" s="386"/>
+      <c r="U24" s="371"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -19432,13 +19452,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="390" t="s">
+      <c r="H27" s="391" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="390"/>
-      <c r="J27" s="390"/>
-      <c r="K27" s="390"/>
-      <c r="L27" s="390"/>
+      <c r="I27" s="391"/>
+      <c r="J27" s="391"/>
+      <c r="K27" s="391"/>
+      <c r="L27" s="391"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -19718,19 +19738,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="393" t="s">
+      <c r="D40" s="394" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="393"/>
-      <c r="F40" s="393"/>
-      <c r="G40" s="393"/>
-      <c r="H40" s="393"/>
-      <c r="I40" s="393" t="s">
+      <c r="E40" s="394"/>
+      <c r="F40" s="394"/>
+      <c r="G40" s="394"/>
+      <c r="H40" s="394"/>
+      <c r="I40" s="394" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="393"/>
-      <c r="K40" s="393"/>
-      <c r="L40" s="393"/>
+      <c r="J40" s="394"/>
+      <c r="K40" s="394"/>
+      <c r="L40" s="394"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -19854,19 +19874,19 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="394"/>
+      <c r="B42" s="395"/>
       <c r="C42" s="110"/>
       <c r="D42" s="111"/>
       <c r="E42" s="111"/>
       <c r="F42" s="125"/>
       <c r="G42" s="125"/>
-      <c r="H42" s="392"/>
+      <c r="H42" s="393"/>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="125"/>
       <c r="L42" s="125"/>
-      <c r="M42" s="392"/>
-      <c r="N42" s="419"/>
+      <c r="M42" s="393"/>
+      <c r="N42" s="420"/>
       <c r="P42" s="91"/>
       <c r="Q42" s="91"/>
       <c r="U42" s="64"/>
@@ -19912,19 +19932,19 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="394"/>
+      <c r="B43" s="395"/>
       <c r="C43" s="110"/>
       <c r="D43" s="125"/>
       <c r="E43" s="111"/>
       <c r="F43" s="125"/>
       <c r="G43" s="103"/>
-      <c r="H43" s="392"/>
+      <c r="H43" s="393"/>
       <c r="I43" s="111"/>
       <c r="J43" s="111"/>
       <c r="K43" s="103"/>
       <c r="L43" s="103"/>
-      <c r="M43" s="392"/>
-      <c r="N43" s="392"/>
+      <c r="M43" s="393"/>
+      <c r="N43" s="393"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -19970,19 +19990,19 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="394"/>
+      <c r="B44" s="395"/>
       <c r="C44" s="110"/>
       <c r="D44" s="111"/>
       <c r="E44" s="111"/>
       <c r="F44" s="125"/>
       <c r="G44" s="125"/>
-      <c r="H44" s="392"/>
+      <c r="H44" s="393"/>
       <c r="I44" s="111"/>
       <c r="J44" s="111"/>
       <c r="K44" s="125"/>
       <c r="L44" s="125"/>
-      <c r="M44" s="392"/>
-      <c r="N44" s="392"/>
+      <c r="M44" s="393"/>
+      <c r="N44" s="393"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -20028,19 +20048,19 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="394"/>
+      <c r="B45" s="395"/>
       <c r="C45" s="110"/>
       <c r="D45" s="111"/>
       <c r="E45" s="111"/>
       <c r="F45" s="125"/>
       <c r="G45" s="125"/>
-      <c r="H45" s="392"/>
+      <c r="H45" s="393"/>
       <c r="I45" s="111"/>
       <c r="J45" s="111"/>
       <c r="K45" s="125"/>
       <c r="L45" s="125"/>
-      <c r="M45" s="392"/>
-      <c r="N45" s="392"/>
+      <c r="M45" s="393"/>
+      <c r="N45" s="393"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -20086,19 +20106,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="394"/>
+      <c r="B46" s="395"/>
       <c r="C46" s="110"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="125"/>
       <c r="G46" s="125"/>
-      <c r="H46" s="392"/>
+      <c r="H46" s="393"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="125"/>
       <c r="L46" s="125"/>
-      <c r="M46" s="392"/>
-      <c r="N46" s="420"/>
+      <c r="M46" s="393"/>
+      <c r="N46" s="421"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -20144,19 +20164,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="394"/>
+      <c r="B47" s="395"/>
       <c r="C47" s="110"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="392"/>
+      <c r="H47" s="393"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="392"/>
-      <c r="N47" s="396"/>
+      <c r="M47" s="393"/>
+      <c r="N47" s="397"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -20204,19 +20224,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="394"/>
+      <c r="B48" s="395"/>
       <c r="C48" s="110"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="392"/>
+      <c r="H48" s="393"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="392"/>
-      <c r="N48" s="396"/>
+      <c r="M48" s="393"/>
+      <c r="N48" s="397"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -20264,19 +20284,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="394"/>
+      <c r="B49" s="395"/>
       <c r="C49" s="110"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="392"/>
+      <c r="H49" s="393"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="392"/>
-      <c r="N49" s="396"/>
+      <c r="M49" s="393"/>
+      <c r="N49" s="397"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -20324,19 +20344,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="397"/>
+      <c r="B50" s="398"/>
       <c r="C50" s="112"/>
       <c r="D50" s="113"/>
       <c r="E50" s="113"/>
       <c r="F50" s="113"/>
       <c r="G50" s="113"/>
-      <c r="H50" s="398"/>
+      <c r="H50" s="399"/>
       <c r="I50" s="113"/>
       <c r="J50" s="113"/>
       <c r="K50" s="113"/>
       <c r="L50" s="113"/>
-      <c r="M50" s="398"/>
-      <c r="N50" s="421"/>
+      <c r="M50" s="399"/>
+      <c r="N50" s="422"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -20357,19 +20377,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="397"/>
+      <c r="B51" s="398"/>
       <c r="C51" s="112"/>
       <c r="D51" s="113"/>
       <c r="E51" s="113"/>
       <c r="F51" s="113"/>
       <c r="G51" s="113"/>
-      <c r="H51" s="398"/>
+      <c r="H51" s="399"/>
       <c r="I51" s="113"/>
       <c r="J51" s="113"/>
       <c r="K51" s="113"/>
       <c r="L51" s="113"/>
-      <c r="M51" s="398"/>
-      <c r="N51" s="400"/>
+      <c r="M51" s="399"/>
+      <c r="N51" s="401"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -20400,19 +20420,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="397"/>
+      <c r="B52" s="398"/>
       <c r="C52" s="112"/>
       <c r="D52" s="113"/>
       <c r="E52" s="113"/>
       <c r="F52" s="113"/>
       <c r="G52" s="113"/>
-      <c r="H52" s="398"/>
+      <c r="H52" s="399"/>
       <c r="I52" s="113"/>
       <c r="J52" s="113"/>
       <c r="K52" s="113"/>
       <c r="L52" s="113"/>
-      <c r="M52" s="398"/>
-      <c r="N52" s="400"/>
+      <c r="M52" s="399"/>
+      <c r="N52" s="401"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -20476,19 +20496,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="397"/>
+      <c r="B53" s="398"/>
       <c r="C53" s="112"/>
       <c r="D53" s="113"/>
       <c r="E53" s="113"/>
       <c r="F53" s="113"/>
       <c r="G53" s="113"/>
-      <c r="H53" s="398"/>
+      <c r="H53" s="399"/>
       <c r="I53" s="113"/>
       <c r="J53" s="113"/>
       <c r="K53" s="113"/>
       <c r="L53" s="113"/>
-      <c r="M53" s="398"/>
-      <c r="N53" s="400"/>
+      <c r="M53" s="399"/>
+      <c r="N53" s="401"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -20537,19 +20557,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="397"/>
+      <c r="B54" s="398"/>
       <c r="C54" s="112"/>
       <c r="D54" s="113"/>
       <c r="E54" s="113"/>
       <c r="F54" s="113"/>
       <c r="G54" s="113"/>
-      <c r="H54" s="398"/>
+      <c r="H54" s="399"/>
       <c r="I54" s="113"/>
       <c r="J54" s="113"/>
       <c r="K54" s="113"/>
       <c r="L54" s="113"/>
-      <c r="M54" s="398"/>
-      <c r="N54" s="422"/>
+      <c r="M54" s="399"/>
+      <c r="N54" s="423"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -20596,19 +20616,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="397"/>
+      <c r="B55" s="398"/>
       <c r="C55" s="112"/>
       <c r="D55" s="113"/>
       <c r="E55" s="113"/>
       <c r="F55" s="113"/>
       <c r="G55" s="113"/>
-      <c r="H55" s="398"/>
+      <c r="H55" s="399"/>
       <c r="I55" s="113"/>
       <c r="J55" s="113"/>
       <c r="K55" s="113"/>
       <c r="L55" s="113"/>
-      <c r="M55" s="398"/>
-      <c r="N55" s="400"/>
+      <c r="M55" s="399"/>
+      <c r="N55" s="401"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -20655,19 +20675,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="397"/>
+      <c r="B56" s="398"/>
       <c r="C56" s="112"/>
       <c r="D56" s="113"/>
       <c r="E56" s="113"/>
       <c r="F56" s="113"/>
       <c r="G56" s="113"/>
-      <c r="H56" s="398"/>
+      <c r="H56" s="399"/>
       <c r="I56" s="113"/>
       <c r="J56" s="113"/>
       <c r="K56" s="113"/>
       <c r="L56" s="113"/>
-      <c r="M56" s="398"/>
-      <c r="N56" s="400"/>
+      <c r="M56" s="399"/>
+      <c r="N56" s="401"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -20714,19 +20734,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="397"/>
+      <c r="B57" s="398"/>
       <c r="C57" s="112"/>
       <c r="D57" s="113"/>
       <c r="E57" s="113"/>
       <c r="F57" s="113"/>
       <c r="G57" s="113"/>
-      <c r="H57" s="398"/>
+      <c r="H57" s="399"/>
       <c r="I57" s="113"/>
       <c r="J57" s="113"/>
       <c r="K57" s="113"/>
       <c r="L57" s="113"/>
-      <c r="M57" s="398"/>
-      <c r="N57" s="400"/>
+      <c r="M57" s="399"/>
+      <c r="N57" s="401"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -20773,19 +20793,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="402"/>
+      <c r="B58" s="403"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
       <c r="E58" s="115"/>
       <c r="F58" s="115"/>
       <c r="G58" s="115"/>
-      <c r="H58" s="403"/>
+      <c r="H58" s="404"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115"/>
       <c r="K58" s="115"/>
       <c r="L58" s="115"/>
-      <c r="M58" s="403"/>
-      <c r="N58" s="423"/>
+      <c r="M58" s="404"/>
+      <c r="N58" s="424"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -20832,19 +20852,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="402"/>
+      <c r="B59" s="403"/>
       <c r="C59" s="114"/>
       <c r="D59" s="115"/>
       <c r="E59" s="115"/>
       <c r="F59" s="115"/>
       <c r="G59" s="115"/>
-      <c r="H59" s="403"/>
+      <c r="H59" s="404"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115"/>
       <c r="K59" s="115"/>
       <c r="L59" s="115"/>
-      <c r="M59" s="403"/>
-      <c r="N59" s="405"/>
+      <c r="M59" s="404"/>
+      <c r="N59" s="406"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -20891,19 +20911,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="402"/>
+      <c r="B60" s="403"/>
       <c r="C60" s="114"/>
       <c r="D60" s="115"/>
       <c r="E60" s="115"/>
       <c r="F60" s="115"/>
       <c r="G60" s="115"/>
-      <c r="H60" s="403"/>
+      <c r="H60" s="404"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115"/>
       <c r="K60" s="115"/>
       <c r="L60" s="115"/>
-      <c r="M60" s="403"/>
-      <c r="N60" s="405"/>
+      <c r="M60" s="404"/>
+      <c r="N60" s="406"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -20950,247 +20970,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="402"/>
+      <c r="B61" s="403"/>
       <c r="C61" s="114"/>
       <c r="D61" s="115"/>
       <c r="E61" s="115"/>
       <c r="F61" s="115"/>
       <c r="G61" s="115"/>
-      <c r="H61" s="403"/>
+      <c r="H61" s="404"/>
       <c r="I61" s="115"/>
       <c r="J61" s="115"/>
       <c r="K61" s="115"/>
       <c r="L61" s="115"/>
-      <c r="M61" s="403"/>
-      <c r="N61" s="405"/>
+      <c r="M61" s="404"/>
+      <c r="N61" s="406"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="402"/>
+      <c r="B62" s="403"/>
       <c r="C62" s="114"/>
       <c r="D62" s="115"/>
       <c r="E62" s="115"/>
       <c r="F62" s="115"/>
       <c r="G62" s="115"/>
-      <c r="H62" s="403"/>
+      <c r="H62" s="404"/>
       <c r="I62" s="115"/>
       <c r="J62" s="115"/>
       <c r="K62" s="115"/>
       <c r="L62" s="115"/>
-      <c r="M62" s="403"/>
-      <c r="N62" s="424"/>
+      <c r="M62" s="404"/>
+      <c r="N62" s="425"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="402"/>
+      <c r="B63" s="403"/>
       <c r="C63" s="114"/>
       <c r="D63" s="115"/>
       <c r="E63" s="115"/>
       <c r="F63" s="115"/>
       <c r="G63" s="115"/>
-      <c r="H63" s="403"/>
+      <c r="H63" s="404"/>
       <c r="I63" s="115"/>
       <c r="J63" s="115"/>
       <c r="K63" s="115"/>
       <c r="L63" s="115"/>
-      <c r="M63" s="403"/>
-      <c r="N63" s="405"/>
+      <c r="M63" s="404"/>
+      <c r="N63" s="406"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="402"/>
+      <c r="B64" s="403"/>
       <c r="C64" s="114"/>
       <c r="D64" s="115"/>
       <c r="E64" s="115"/>
       <c r="F64" s="115"/>
       <c r="G64" s="115"/>
-      <c r="H64" s="403"/>
+      <c r="H64" s="404"/>
       <c r="I64" s="115"/>
       <c r="J64" s="115"/>
       <c r="K64" s="115"/>
       <c r="L64" s="115"/>
-      <c r="M64" s="403"/>
-      <c r="N64" s="405"/>
+      <c r="M64" s="404"/>
+      <c r="N64" s="406"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="402"/>
+      <c r="B65" s="403"/>
       <c r="C65" s="114"/>
       <c r="D65" s="115"/>
       <c r="E65" s="115"/>
       <c r="F65" s="115"/>
       <c r="G65" s="115"/>
-      <c r="H65" s="403"/>
+      <c r="H65" s="404"/>
       <c r="I65" s="115"/>
       <c r="J65" s="115"/>
       <c r="K65" s="115"/>
       <c r="L65" s="115"/>
-      <c r="M65" s="403"/>
-      <c r="N65" s="405"/>
+      <c r="M65" s="404"/>
+      <c r="N65" s="406"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="406"/>
+      <c r="B66" s="407"/>
       <c r="C66" s="128"/>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
       <c r="F66" s="116"/>
       <c r="G66" s="116"/>
-      <c r="H66" s="407"/>
+      <c r="H66" s="408"/>
       <c r="I66" s="116"/>
       <c r="J66" s="116"/>
       <c r="K66" s="116"/>
       <c r="L66" s="116"/>
-      <c r="M66" s="407"/>
-      <c r="N66" s="425"/>
+      <c r="M66" s="408"/>
+      <c r="N66" s="426"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="406"/>
+      <c r="B67" s="407"/>
       <c r="C67" s="128"/>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
       <c r="F67" s="116"/>
       <c r="G67" s="116"/>
-      <c r="H67" s="407"/>
+      <c r="H67" s="408"/>
       <c r="I67" s="116"/>
       <c r="J67" s="116"/>
       <c r="K67" s="116"/>
       <c r="L67" s="116"/>
-      <c r="M67" s="407"/>
-      <c r="N67" s="409"/>
+      <c r="M67" s="408"/>
+      <c r="N67" s="410"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="406"/>
+      <c r="B68" s="407"/>
       <c r="C68" s="128"/>
       <c r="D68" s="116"/>
       <c r="E68" s="116"/>
       <c r="F68" s="116"/>
       <c r="G68" s="116"/>
-      <c r="H68" s="407"/>
+      <c r="H68" s="408"/>
       <c r="I68" s="116"/>
       <c r="J68" s="116"/>
       <c r="K68" s="116"/>
       <c r="L68" s="116"/>
-      <c r="M68" s="407"/>
-      <c r="N68" s="409"/>
+      <c r="M68" s="408"/>
+      <c r="N68" s="410"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="406"/>
+      <c r="B69" s="407"/>
       <c r="C69" s="128"/>
       <c r="D69" s="116"/>
       <c r="E69" s="116"/>
       <c r="F69" s="116"/>
       <c r="G69" s="116"/>
-      <c r="H69" s="407"/>
+      <c r="H69" s="408"/>
       <c r="I69" s="116"/>
       <c r="J69" s="116"/>
       <c r="K69" s="116"/>
       <c r="L69" s="116"/>
-      <c r="M69" s="407"/>
-      <c r="N69" s="409"/>
+      <c r="M69" s="408"/>
+      <c r="N69" s="410"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="406"/>
+      <c r="B70" s="407"/>
       <c r="C70" s="128"/>
       <c r="D70" s="116"/>
       <c r="E70" s="116"/>
       <c r="F70" s="116"/>
       <c r="G70" s="116"/>
-      <c r="H70" s="407"/>
+      <c r="H70" s="408"/>
       <c r="I70" s="116"/>
       <c r="J70" s="116"/>
       <c r="K70" s="116"/>
       <c r="L70" s="116"/>
-      <c r="M70" s="407"/>
-      <c r="N70" s="426"/>
+      <c r="M70" s="408"/>
+      <c r="N70" s="427"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="406"/>
+      <c r="B71" s="407"/>
       <c r="C71" s="128"/>
       <c r="D71" s="116"/>
       <c r="E71" s="116"/>
       <c r="F71" s="116"/>
       <c r="G71" s="116"/>
-      <c r="H71" s="407"/>
+      <c r="H71" s="408"/>
       <c r="I71" s="116"/>
       <c r="J71" s="116"/>
       <c r="K71" s="116"/>
       <c r="L71" s="116"/>
-      <c r="M71" s="407"/>
-      <c r="N71" s="409"/>
+      <c r="M71" s="408"/>
+      <c r="N71" s="410"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="406"/>
+      <c r="B72" s="407"/>
       <c r="C72" s="128"/>
       <c r="D72" s="116"/>
       <c r="E72" s="116"/>
       <c r="F72" s="116"/>
       <c r="G72" s="116"/>
-      <c r="H72" s="407"/>
+      <c r="H72" s="408"/>
       <c r="I72" s="116"/>
       <c r="J72" s="116"/>
       <c r="K72" s="116"/>
       <c r="L72" s="116"/>
-      <c r="M72" s="407"/>
-      <c r="N72" s="409"/>
+      <c r="M72" s="408"/>
+      <c r="N72" s="410"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="406"/>
+      <c r="B73" s="407"/>
       <c r="C73" s="128"/>
       <c r="D73" s="116"/>
       <c r="E73" s="116"/>
       <c r="F73" s="116"/>
       <c r="G73" s="116"/>
-      <c r="H73" s="407"/>
+      <c r="H73" s="408"/>
       <c r="I73" s="116"/>
       <c r="J73" s="116"/>
       <c r="K73" s="116"/>
       <c r="L73" s="116"/>
-      <c r="M73" s="407"/>
-      <c r="N73" s="409"/>
+      <c r="M73" s="408"/>
+      <c r="N73" s="410"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>

</xml_diff>

<commit_message>
Completed manual and Campaign Calculation
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -850,10 +850,10 @@
     <t>Tenant ID:</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>Solid</t>
+  </si>
+  <si>
+    <t>Campaign</t>
   </si>
 </sst>
 </file>
@@ -9534,7 +9534,7 @@
   <dimension ref="A1:AU434"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -10511,10 +10511,10 @@
     </row>
     <row r="40" spans="1:41" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="314" t="s">
+        <v>246</v>
+      </c>
+      <c r="B40" s="315" t="s">
         <v>245</v>
-      </c>
-      <c r="B40" s="315" t="s">
-        <v>246</v>
       </c>
       <c r="D40" s="104"/>
       <c r="E40" s="105"/>

</xml_diff>

<commit_message>
Cleaning agent calculation done
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -850,10 +850,10 @@
     <t>Tenant ID:</t>
   </si>
   <si>
+    <t>Manual</t>
+  </si>
+  <si>
     <t>Solid</t>
-  </si>
-  <si>
-    <t>Campaign</t>
   </si>
 </sst>
 </file>
@@ -2474,53 +2474,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="25" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2530,23 +2483,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2569,30 +2522,77 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2614,14 +2614,14 @@
     <xf numFmtId="3" fontId="25" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5041,15 +5041,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="380" t="s">
+      <c r="F1" s="345" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="380"/>
-      <c r="H1" s="380"/>
-      <c r="I1" s="380"/>
-      <c r="J1" s="380"/>
-      <c r="K1" s="380"/>
-      <c r="L1" s="380"/>
+      <c r="G1" s="345"/>
+      <c r="H1" s="345"/>
+      <c r="I1" s="345"/>
+      <c r="J1" s="345"/>
+      <c r="K1" s="345"/>
+      <c r="L1" s="345"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -5138,22 +5138,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="381" t="s">
+      <c r="D6" s="346" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="382"/>
-      <c r="F6" s="382"/>
-      <c r="G6" s="382"/>
-      <c r="H6" s="383"/>
+      <c r="E6" s="347"/>
+      <c r="F6" s="347"/>
+      <c r="G6" s="347"/>
+      <c r="H6" s="348"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="381" t="s">
+      <c r="M6" s="346" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="382"/>
-      <c r="O6" s="382"/>
-      <c r="P6" s="382"/>
-      <c r="Q6" s="383"/>
+      <c r="N6" s="347"/>
+      <c r="O6" s="347"/>
+      <c r="P6" s="347"/>
+      <c r="Q6" s="348"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -5171,10 +5171,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="384" t="s">
+      <c r="F7" s="349" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="385"/>
+      <c r="G7" s="350"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -5197,10 +5197,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="384" t="s">
+      <c r="P7" s="349" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="385"/>
+      <c r="Q7" s="350"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -5277,7 +5277,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="372" t="s">
+      <c r="B9" s="351" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5311,33 +5311,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="363">
+      <c r="M9" s="342">
         <v>20</v>
       </c>
-      <c r="N9" s="375" t="s">
+      <c r="N9" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="363">
+      <c r="O9" s="342">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="363">
+      <c r="P9" s="342">
         <v>3</v>
       </c>
-      <c r="Q9" s="363">
+      <c r="Q9" s="342">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="363">
+      <c r="R9" s="342">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="363"/>
-      <c r="T9" s="366">
+      <c r="S9" s="342"/>
+      <c r="T9" s="357">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="363">
+      <c r="U9" s="342">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -5362,7 +5362,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="373"/>
+      <c r="B10" s="352"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -5394,15 +5394,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="364"/>
-      <c r="N10" s="376"/>
-      <c r="O10" s="364"/>
-      <c r="P10" s="364"/>
-      <c r="Q10" s="364"/>
-      <c r="R10" s="364"/>
-      <c r="S10" s="364"/>
-      <c r="T10" s="367"/>
-      <c r="U10" s="364"/>
+      <c r="M10" s="343"/>
+      <c r="N10" s="355"/>
+      <c r="O10" s="343"/>
+      <c r="P10" s="343"/>
+      <c r="Q10" s="343"/>
+      <c r="R10" s="343"/>
+      <c r="S10" s="343"/>
+      <c r="T10" s="358"/>
+      <c r="U10" s="343"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -5410,10 +5410,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="363" t="s">
+      <c r="A11" s="342" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="373"/>
+      <c r="B11" s="352"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -5424,15 +5424,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="364"/>
-      <c r="N11" s="376"/>
-      <c r="O11" s="364"/>
-      <c r="P11" s="364"/>
-      <c r="Q11" s="364"/>
-      <c r="R11" s="364"/>
-      <c r="S11" s="364"/>
-      <c r="T11" s="367"/>
-      <c r="U11" s="364"/>
+      <c r="M11" s="343"/>
+      <c r="N11" s="355"/>
+      <c r="O11" s="343"/>
+      <c r="P11" s="343"/>
+      <c r="Q11" s="343"/>
+      <c r="R11" s="343"/>
+      <c r="S11" s="343"/>
+      <c r="T11" s="358"/>
+      <c r="U11" s="343"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -5451,8 +5451,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="365"/>
-      <c r="B12" s="374"/>
+      <c r="A12" s="344"/>
+      <c r="B12" s="353"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -5463,15 +5463,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="365"/>
-      <c r="N12" s="377"/>
-      <c r="O12" s="365"/>
-      <c r="P12" s="365"/>
-      <c r="Q12" s="365"/>
-      <c r="R12" s="365"/>
-      <c r="S12" s="365"/>
-      <c r="T12" s="368"/>
-      <c r="U12" s="365"/>
+      <c r="M12" s="344"/>
+      <c r="N12" s="356"/>
+      <c r="O12" s="344"/>
+      <c r="P12" s="344"/>
+      <c r="Q12" s="344"/>
+      <c r="R12" s="344"/>
+      <c r="S12" s="344"/>
+      <c r="T12" s="359"/>
+      <c r="U12" s="344"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -5487,7 +5487,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="372" t="s">
+      <c r="B13" s="351" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5521,33 +5521,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="363">
+      <c r="M13" s="342">
         <v>80</v>
       </c>
-      <c r="N13" s="375" t="s">
+      <c r="N13" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="363">
+      <c r="O13" s="342">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="363">
+      <c r="P13" s="342">
         <v>2</v>
       </c>
-      <c r="Q13" s="363">
+      <c r="Q13" s="342">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="363">
+      <c r="R13" s="342">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="363"/>
-      <c r="T13" s="366">
+      <c r="S13" s="342"/>
+      <c r="T13" s="357">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="363">
+      <c r="U13" s="342">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -5570,7 +5570,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="373"/>
+      <c r="B14" s="352"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -5602,15 +5602,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="364"/>
-      <c r="N14" s="376"/>
-      <c r="O14" s="364"/>
-      <c r="P14" s="364"/>
-      <c r="Q14" s="364"/>
-      <c r="R14" s="364"/>
-      <c r="S14" s="364"/>
-      <c r="T14" s="367"/>
-      <c r="U14" s="364"/>
+      <c r="M14" s="343"/>
+      <c r="N14" s="355"/>
+      <c r="O14" s="343"/>
+      <c r="P14" s="343"/>
+      <c r="Q14" s="343"/>
+      <c r="R14" s="343"/>
+      <c r="S14" s="343"/>
+      <c r="T14" s="358"/>
+      <c r="U14" s="343"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -5618,10 +5618,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="378" t="s">
+      <c r="A15" s="360" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="373"/>
+      <c r="B15" s="352"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -5632,15 +5632,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="364"/>
-      <c r="N15" s="376"/>
-      <c r="O15" s="364"/>
-      <c r="P15" s="364"/>
-      <c r="Q15" s="364"/>
-      <c r="R15" s="364"/>
-      <c r="S15" s="364"/>
-      <c r="T15" s="367"/>
-      <c r="U15" s="364"/>
+      <c r="M15" s="343"/>
+      <c r="N15" s="355"/>
+      <c r="O15" s="343"/>
+      <c r="P15" s="343"/>
+      <c r="Q15" s="343"/>
+      <c r="R15" s="343"/>
+      <c r="S15" s="343"/>
+      <c r="T15" s="358"/>
+      <c r="U15" s="343"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -5650,8 +5650,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="379"/>
-      <c r="B16" s="374"/>
+      <c r="A16" s="361"/>
+      <c r="B16" s="353"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -5662,15 +5662,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="365"/>
-      <c r="N16" s="377"/>
-      <c r="O16" s="365"/>
-      <c r="P16" s="365"/>
-      <c r="Q16" s="365"/>
-      <c r="R16" s="365"/>
-      <c r="S16" s="365"/>
-      <c r="T16" s="368"/>
-      <c r="U16" s="365"/>
+      <c r="M16" s="344"/>
+      <c r="N16" s="356"/>
+      <c r="O16" s="344"/>
+      <c r="P16" s="344"/>
+      <c r="Q16" s="344"/>
+      <c r="R16" s="344"/>
+      <c r="S16" s="344"/>
+      <c r="T16" s="359"/>
+      <c r="U16" s="344"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -5681,7 +5681,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="372" t="s">
+      <c r="B17" s="351" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5715,33 +5715,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="363">
+      <c r="M17" s="342">
         <v>70</v>
       </c>
-      <c r="N17" s="375" t="s">
+      <c r="N17" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="363">
+      <c r="O17" s="342">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="363">
+      <c r="P17" s="342">
         <v>2</v>
       </c>
-      <c r="Q17" s="363">
+      <c r="Q17" s="342">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="363">
+      <c r="R17" s="342">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="363"/>
-      <c r="T17" s="366">
+      <c r="S17" s="342"/>
+      <c r="T17" s="357">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="363">
+      <c r="U17" s="342">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -5760,7 +5760,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="373"/>
+      <c r="B18" s="352"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -5792,24 +5792,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="364"/>
-      <c r="N18" s="376"/>
-      <c r="O18" s="364"/>
-      <c r="P18" s="364"/>
-      <c r="Q18" s="364"/>
-      <c r="R18" s="364"/>
-      <c r="S18" s="364"/>
-      <c r="T18" s="367"/>
-      <c r="U18" s="364"/>
+      <c r="M18" s="343"/>
+      <c r="N18" s="355"/>
+      <c r="O18" s="343"/>
+      <c r="P18" s="343"/>
+      <c r="Q18" s="343"/>
+      <c r="R18" s="343"/>
+      <c r="S18" s="343"/>
+      <c r="T18" s="358"/>
+      <c r="U18" s="343"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="363" t="s">
+      <c r="A19" s="342" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="373"/>
+      <c r="B19" s="352"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -5820,22 +5820,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="364"/>
-      <c r="N19" s="376"/>
-      <c r="O19" s="364"/>
-      <c r="P19" s="364"/>
-      <c r="Q19" s="364"/>
-      <c r="R19" s="364"/>
-      <c r="S19" s="364"/>
-      <c r="T19" s="367"/>
-      <c r="U19" s="364"/>
+      <c r="M19" s="343"/>
+      <c r="N19" s="355"/>
+      <c r="O19" s="343"/>
+      <c r="P19" s="343"/>
+      <c r="Q19" s="343"/>
+      <c r="R19" s="343"/>
+      <c r="S19" s="343"/>
+      <c r="T19" s="358"/>
+      <c r="U19" s="343"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="365"/>
-      <c r="B20" s="374"/>
+      <c r="A20" s="344"/>
+      <c r="B20" s="353"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -5846,15 +5846,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="365"/>
-      <c r="N20" s="377"/>
-      <c r="O20" s="365"/>
-      <c r="P20" s="365"/>
-      <c r="Q20" s="365"/>
-      <c r="R20" s="365"/>
-      <c r="S20" s="365"/>
-      <c r="T20" s="368"/>
-      <c r="U20" s="365"/>
+      <c r="M20" s="344"/>
+      <c r="N20" s="356"/>
+      <c r="O20" s="344"/>
+      <c r="P20" s="344"/>
+      <c r="Q20" s="344"/>
+      <c r="R20" s="344"/>
+      <c r="S20" s="344"/>
+      <c r="T20" s="359"/>
+      <c r="U20" s="344"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -5863,7 +5863,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="372" t="s">
+      <c r="B21" s="351" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5897,33 +5897,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="363">
+      <c r="M21" s="342">
         <v>60</v>
       </c>
-      <c r="N21" s="375" t="s">
+      <c r="N21" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="363">
+      <c r="O21" s="342">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="363">
+      <c r="P21" s="342">
         <v>3</v>
       </c>
-      <c r="Q21" s="363">
+      <c r="Q21" s="342">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="363">
+      <c r="R21" s="342">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="363"/>
-      <c r="T21" s="366">
+      <c r="S21" s="342"/>
+      <c r="T21" s="357">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="363">
+      <c r="U21" s="342">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -5940,7 +5940,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="373"/>
+      <c r="B22" s="352"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -5972,24 +5972,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="364"/>
-      <c r="N22" s="376"/>
-      <c r="O22" s="364"/>
-      <c r="P22" s="364"/>
-      <c r="Q22" s="364"/>
-      <c r="R22" s="364"/>
-      <c r="S22" s="364"/>
-      <c r="T22" s="367"/>
-      <c r="U22" s="364"/>
+      <c r="M22" s="343"/>
+      <c r="N22" s="355"/>
+      <c r="O22" s="343"/>
+      <c r="P22" s="343"/>
+      <c r="Q22" s="343"/>
+      <c r="R22" s="343"/>
+      <c r="S22" s="343"/>
+      <c r="T22" s="358"/>
+      <c r="U22" s="343"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="369" t="s">
+      <c r="A23" s="362" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="373"/>
+      <c r="B23" s="352"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -6000,22 +6000,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="364"/>
-      <c r="N23" s="376"/>
-      <c r="O23" s="364"/>
-      <c r="P23" s="364"/>
-      <c r="Q23" s="364"/>
-      <c r="R23" s="364"/>
-      <c r="S23" s="364"/>
-      <c r="T23" s="367"/>
-      <c r="U23" s="364"/>
+      <c r="M23" s="343"/>
+      <c r="N23" s="355"/>
+      <c r="O23" s="343"/>
+      <c r="P23" s="343"/>
+      <c r="Q23" s="343"/>
+      <c r="R23" s="343"/>
+      <c r="S23" s="343"/>
+      <c r="T23" s="358"/>
+      <c r="U23" s="343"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="370"/>
-      <c r="B24" s="374"/>
+      <c r="A24" s="363"/>
+      <c r="B24" s="353"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -6026,15 +6026,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="365"/>
-      <c r="N24" s="377"/>
-      <c r="O24" s="365"/>
-      <c r="P24" s="365"/>
-      <c r="Q24" s="365"/>
-      <c r="R24" s="365"/>
-      <c r="S24" s="365"/>
-      <c r="T24" s="368"/>
-      <c r="U24" s="365"/>
+      <c r="M24" s="344"/>
+      <c r="N24" s="356"/>
+      <c r="O24" s="344"/>
+      <c r="P24" s="344"/>
+      <c r="Q24" s="344"/>
+      <c r="R24" s="344"/>
+      <c r="S24" s="344"/>
+      <c r="T24" s="359"/>
+      <c r="U24" s="344"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -6060,13 +6060,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="371" t="s">
+      <c r="H27" s="364" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="371"/>
-      <c r="J27" s="371"/>
-      <c r="K27" s="371"/>
-      <c r="L27" s="371"/>
+      <c r="I27" s="364"/>
+      <c r="J27" s="364"/>
+      <c r="K27" s="364"/>
+      <c r="L27" s="364"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -6346,19 +6346,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="361" t="s">
+      <c r="D40" s="367" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="361"/>
-      <c r="F40" s="361"/>
-      <c r="G40" s="361"/>
-      <c r="H40" s="361"/>
-      <c r="I40" s="361" t="s">
+      <c r="E40" s="367"/>
+      <c r="F40" s="367"/>
+      <c r="G40" s="367"/>
+      <c r="H40" s="367"/>
+      <c r="I40" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="361"/>
-      <c r="K40" s="361"/>
-      <c r="L40" s="361"/>
+      <c r="J40" s="367"/>
+      <c r="K40" s="367"/>
+      <c r="L40" s="367"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -6482,7 +6482,7 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="356" t="s">
+      <c r="B42" s="368" t="s">
         <v>226</v>
       </c>
       <c r="C42" s="190"/>
@@ -6490,17 +6490,17 @@
       <c r="E42" s="111"/>
       <c r="F42" s="189"/>
       <c r="G42" s="189"/>
-      <c r="H42" s="357">
+      <c r="H42" s="366">
         <v>3.095975611358881E-3</v>
       </c>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="189"/>
       <c r="L42" s="189"/>
-      <c r="M42" s="357">
+      <c r="M42" s="366">
         <v>1</v>
       </c>
-      <c r="N42" s="362" t="s">
+      <c r="N42" s="365" t="s">
         <v>59</v>
       </c>
       <c r="P42" s="91"/>
@@ -6548,7 +6548,7 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="356"/>
+      <c r="B43" s="368"/>
       <c r="C43" s="190" t="s">
         <v>220</v>
       </c>
@@ -6564,7 +6564,7 @@
       <c r="G43" s="103">
         <v>97.126746422628088</v>
       </c>
-      <c r="H43" s="357"/>
+      <c r="H43" s="366"/>
       <c r="I43" s="111">
         <v>1</v>
       </c>
@@ -6577,8 +6577,8 @@
       <c r="L43" s="103">
         <v>1</v>
       </c>
-      <c r="M43" s="357"/>
-      <c r="N43" s="357"/>
+      <c r="M43" s="366"/>
+      <c r="N43" s="366"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -6624,7 +6624,7 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="356"/>
+      <c r="B44" s="368"/>
       <c r="C44" s="190" t="s">
         <v>218</v>
       </c>
@@ -6640,7 +6640,7 @@
       <c r="G44" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H44" s="357"/>
+      <c r="H44" s="366"/>
       <c r="I44" s="111">
         <v>1</v>
       </c>
@@ -6653,8 +6653,8 @@
       <c r="L44" s="189">
         <v>1</v>
       </c>
-      <c r="M44" s="357"/>
-      <c r="N44" s="357"/>
+      <c r="M44" s="366"/>
+      <c r="N44" s="366"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -6700,7 +6700,7 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="356"/>
+      <c r="B45" s="368"/>
       <c r="C45" s="190" t="s">
         <v>219</v>
       </c>
@@ -6716,7 +6716,7 @@
       <c r="G45" s="189">
         <v>3.0959756012671502E-3</v>
       </c>
-      <c r="H45" s="357"/>
+      <c r="H45" s="366"/>
       <c r="I45" s="111">
         <v>1</v>
       </c>
@@ -6729,8 +6729,8 @@
       <c r="L45" s="189">
         <v>1</v>
       </c>
-      <c r="M45" s="357"/>
-      <c r="N45" s="357"/>
+      <c r="M45" s="366"/>
+      <c r="N45" s="366"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -6776,19 +6776,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="356"/>
+      <c r="B46" s="368"/>
       <c r="C46" s="190"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="189"/>
       <c r="G46" s="189"/>
-      <c r="H46" s="357"/>
+      <c r="H46" s="366"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="189"/>
       <c r="L46" s="189"/>
-      <c r="M46" s="357"/>
-      <c r="N46" s="358"/>
+      <c r="M46" s="366"/>
+      <c r="N46" s="369"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -6834,19 +6834,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="356"/>
+      <c r="B47" s="368"/>
       <c r="C47" s="190"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="357"/>
+      <c r="H47" s="366"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="357"/>
-      <c r="N47" s="359"/>
+      <c r="M47" s="366"/>
+      <c r="N47" s="370"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -6894,19 +6894,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="356"/>
+      <c r="B48" s="368"/>
       <c r="C48" s="190"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="357"/>
+      <c r="H48" s="366"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="357"/>
-      <c r="N48" s="359"/>
+      <c r="M48" s="366"/>
+      <c r="N48" s="370"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -6954,19 +6954,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="356"/>
+      <c r="B49" s="368"/>
       <c r="C49" s="190"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="357"/>
+      <c r="H49" s="366"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="357"/>
-      <c r="N49" s="359"/>
+      <c r="M49" s="366"/>
+      <c r="N49" s="370"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -7014,19 +7014,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="351"/>
+      <c r="B50" s="371"/>
       <c r="C50" s="191"/>
       <c r="D50" s="187"/>
       <c r="E50" s="187"/>
       <c r="F50" s="187"/>
       <c r="G50" s="187"/>
-      <c r="H50" s="352"/>
+      <c r="H50" s="372"/>
       <c r="I50" s="187"/>
       <c r="J50" s="187"/>
       <c r="K50" s="187"/>
       <c r="L50" s="187"/>
-      <c r="M50" s="352"/>
-      <c r="N50" s="360"/>
+      <c r="M50" s="372"/>
+      <c r="N50" s="373"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -7047,19 +7047,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="351"/>
+      <c r="B51" s="371"/>
       <c r="C51" s="191"/>
       <c r="D51" s="187"/>
       <c r="E51" s="187"/>
       <c r="F51" s="187"/>
       <c r="G51" s="187"/>
-      <c r="H51" s="352"/>
+      <c r="H51" s="372"/>
       <c r="I51" s="187"/>
       <c r="J51" s="187"/>
       <c r="K51" s="187"/>
       <c r="L51" s="187"/>
-      <c r="M51" s="352"/>
-      <c r="N51" s="354"/>
+      <c r="M51" s="372"/>
+      <c r="N51" s="374"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -7090,19 +7090,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="351"/>
+      <c r="B52" s="371"/>
       <c r="C52" s="191"/>
       <c r="D52" s="187"/>
       <c r="E52" s="187"/>
       <c r="F52" s="187"/>
       <c r="G52" s="187"/>
-      <c r="H52" s="352"/>
+      <c r="H52" s="372"/>
       <c r="I52" s="187"/>
       <c r="J52" s="187"/>
       <c r="K52" s="187"/>
       <c r="L52" s="187"/>
-      <c r="M52" s="352"/>
-      <c r="N52" s="354"/>
+      <c r="M52" s="372"/>
+      <c r="N52" s="374"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -7166,19 +7166,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="351"/>
+      <c r="B53" s="371"/>
       <c r="C53" s="191"/>
       <c r="D53" s="187"/>
       <c r="E53" s="187"/>
       <c r="F53" s="187"/>
       <c r="G53" s="187"/>
-      <c r="H53" s="352"/>
+      <c r="H53" s="372"/>
       <c r="I53" s="187"/>
       <c r="J53" s="187"/>
       <c r="K53" s="187"/>
       <c r="L53" s="187"/>
-      <c r="M53" s="352"/>
-      <c r="N53" s="354"/>
+      <c r="M53" s="372"/>
+      <c r="N53" s="374"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -7227,19 +7227,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="351"/>
+      <c r="B54" s="371"/>
       <c r="C54" s="191"/>
       <c r="D54" s="187"/>
       <c r="E54" s="187"/>
       <c r="F54" s="187"/>
       <c r="G54" s="187"/>
-      <c r="H54" s="352"/>
+      <c r="H54" s="372"/>
       <c r="I54" s="187"/>
       <c r="J54" s="187"/>
       <c r="K54" s="187"/>
       <c r="L54" s="187"/>
-      <c r="M54" s="352"/>
-      <c r="N54" s="353"/>
+      <c r="M54" s="372"/>
+      <c r="N54" s="375"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -7286,19 +7286,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="351"/>
+      <c r="B55" s="371"/>
       <c r="C55" s="191"/>
       <c r="D55" s="187"/>
       <c r="E55" s="187"/>
       <c r="F55" s="187"/>
       <c r="G55" s="187"/>
-      <c r="H55" s="352"/>
+      <c r="H55" s="372"/>
       <c r="I55" s="187"/>
       <c r="J55" s="187"/>
       <c r="K55" s="187"/>
       <c r="L55" s="187"/>
-      <c r="M55" s="352"/>
-      <c r="N55" s="354"/>
+      <c r="M55" s="372"/>
+      <c r="N55" s="374"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -7345,19 +7345,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="351"/>
+      <c r="B56" s="371"/>
       <c r="C56" s="191"/>
       <c r="D56" s="187"/>
       <c r="E56" s="187"/>
       <c r="F56" s="187"/>
       <c r="G56" s="187"/>
-      <c r="H56" s="352"/>
+      <c r="H56" s="372"/>
       <c r="I56" s="187"/>
       <c r="J56" s="187"/>
       <c r="K56" s="187"/>
       <c r="L56" s="187"/>
-      <c r="M56" s="352"/>
-      <c r="N56" s="354"/>
+      <c r="M56" s="372"/>
+      <c r="N56" s="374"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -7404,19 +7404,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="351"/>
+      <c r="B57" s="371"/>
       <c r="C57" s="191"/>
       <c r="D57" s="187"/>
       <c r="E57" s="187"/>
       <c r="F57" s="187"/>
       <c r="G57" s="187"/>
-      <c r="H57" s="352"/>
+      <c r="H57" s="372"/>
       <c r="I57" s="187"/>
       <c r="J57" s="187"/>
       <c r="K57" s="187"/>
       <c r="L57" s="187"/>
-      <c r="M57" s="352"/>
-      <c r="N57" s="354"/>
+      <c r="M57" s="372"/>
+      <c r="N57" s="374"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -7463,19 +7463,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="346"/>
+      <c r="B58" s="376"/>
       <c r="C58" s="185"/>
       <c r="D58" s="192"/>
       <c r="E58" s="192"/>
       <c r="F58" s="192"/>
       <c r="G58" s="192"/>
-      <c r="H58" s="347"/>
+      <c r="H58" s="377"/>
       <c r="I58" s="192"/>
       <c r="J58" s="192"/>
       <c r="K58" s="192"/>
       <c r="L58" s="192"/>
-      <c r="M58" s="347"/>
-      <c r="N58" s="355"/>
+      <c r="M58" s="377"/>
+      <c r="N58" s="378"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -7522,19 +7522,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="346"/>
+      <c r="B59" s="376"/>
       <c r="C59" s="185"/>
       <c r="D59" s="192"/>
       <c r="E59" s="192"/>
       <c r="F59" s="192"/>
       <c r="G59" s="192"/>
-      <c r="H59" s="347"/>
+      <c r="H59" s="377"/>
       <c r="I59" s="192"/>
       <c r="J59" s="192"/>
       <c r="K59" s="192"/>
       <c r="L59" s="192"/>
-      <c r="M59" s="347"/>
-      <c r="N59" s="349"/>
+      <c r="M59" s="377"/>
+      <c r="N59" s="379"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -7581,19 +7581,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="346"/>
+      <c r="B60" s="376"/>
       <c r="C60" s="185"/>
       <c r="D60" s="192"/>
       <c r="E60" s="192"/>
       <c r="F60" s="192"/>
       <c r="G60" s="192"/>
-      <c r="H60" s="347"/>
+      <c r="H60" s="377"/>
       <c r="I60" s="192"/>
       <c r="J60" s="192"/>
       <c r="K60" s="192"/>
       <c r="L60" s="192"/>
-      <c r="M60" s="347"/>
-      <c r="N60" s="349"/>
+      <c r="M60" s="377"/>
+      <c r="N60" s="379"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -7640,247 +7640,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="346"/>
+      <c r="B61" s="376"/>
       <c r="C61" s="185"/>
       <c r="D61" s="192"/>
       <c r="E61" s="192"/>
       <c r="F61" s="192"/>
       <c r="G61" s="192"/>
-      <c r="H61" s="347"/>
+      <c r="H61" s="377"/>
       <c r="I61" s="192"/>
       <c r="J61" s="192"/>
       <c r="K61" s="192"/>
       <c r="L61" s="192"/>
-      <c r="M61" s="347"/>
-      <c r="N61" s="349"/>
+      <c r="M61" s="377"/>
+      <c r="N61" s="379"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="346"/>
+      <c r="B62" s="376"/>
       <c r="C62" s="185"/>
       <c r="D62" s="192"/>
       <c r="E62" s="192"/>
       <c r="F62" s="192"/>
       <c r="G62" s="192"/>
-      <c r="H62" s="347"/>
+      <c r="H62" s="377"/>
       <c r="I62" s="192"/>
       <c r="J62" s="192"/>
       <c r="K62" s="192"/>
       <c r="L62" s="192"/>
-      <c r="M62" s="347"/>
-      <c r="N62" s="348"/>
+      <c r="M62" s="377"/>
+      <c r="N62" s="384"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="346"/>
+      <c r="B63" s="376"/>
       <c r="C63" s="185"/>
       <c r="D63" s="192"/>
       <c r="E63" s="192"/>
       <c r="F63" s="192"/>
       <c r="G63" s="192"/>
-      <c r="H63" s="347"/>
+      <c r="H63" s="377"/>
       <c r="I63" s="192"/>
       <c r="J63" s="192"/>
       <c r="K63" s="192"/>
       <c r="L63" s="192"/>
-      <c r="M63" s="347"/>
-      <c r="N63" s="349"/>
+      <c r="M63" s="377"/>
+      <c r="N63" s="379"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="346"/>
+      <c r="B64" s="376"/>
       <c r="C64" s="185"/>
       <c r="D64" s="192"/>
       <c r="E64" s="192"/>
       <c r="F64" s="192"/>
       <c r="G64" s="192"/>
-      <c r="H64" s="347"/>
+      <c r="H64" s="377"/>
       <c r="I64" s="192"/>
       <c r="J64" s="192"/>
       <c r="K64" s="192"/>
       <c r="L64" s="192"/>
-      <c r="M64" s="347"/>
-      <c r="N64" s="349"/>
+      <c r="M64" s="377"/>
+      <c r="N64" s="379"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="346"/>
+      <c r="B65" s="376"/>
       <c r="C65" s="185"/>
       <c r="D65" s="192"/>
       <c r="E65" s="192"/>
       <c r="F65" s="192"/>
       <c r="G65" s="192"/>
-      <c r="H65" s="347"/>
+      <c r="H65" s="377"/>
       <c r="I65" s="192"/>
       <c r="J65" s="192"/>
       <c r="K65" s="192"/>
       <c r="L65" s="192"/>
-      <c r="M65" s="347"/>
-      <c r="N65" s="349"/>
+      <c r="M65" s="377"/>
+      <c r="N65" s="379"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="342"/>
+      <c r="B66" s="380"/>
       <c r="C66" s="186"/>
       <c r="D66" s="188"/>
       <c r="E66" s="188"/>
       <c r="F66" s="188"/>
       <c r="G66" s="188"/>
-      <c r="H66" s="343"/>
+      <c r="H66" s="381"/>
       <c r="I66" s="188"/>
       <c r="J66" s="188"/>
       <c r="K66" s="188"/>
       <c r="L66" s="188"/>
-      <c r="M66" s="343"/>
-      <c r="N66" s="350"/>
+      <c r="M66" s="381"/>
+      <c r="N66" s="385"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="342"/>
+      <c r="B67" s="380"/>
       <c r="C67" s="186"/>
       <c r="D67" s="188"/>
       <c r="E67" s="188"/>
       <c r="F67" s="188"/>
       <c r="G67" s="188"/>
-      <c r="H67" s="343"/>
+      <c r="H67" s="381"/>
       <c r="I67" s="188"/>
       <c r="J67" s="188"/>
       <c r="K67" s="188"/>
       <c r="L67" s="188"/>
-      <c r="M67" s="343"/>
-      <c r="N67" s="345"/>
+      <c r="M67" s="381"/>
+      <c r="N67" s="383"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="342"/>
+      <c r="B68" s="380"/>
       <c r="C68" s="186"/>
       <c r="D68" s="188"/>
       <c r="E68" s="188"/>
       <c r="F68" s="188"/>
       <c r="G68" s="188"/>
-      <c r="H68" s="343"/>
+      <c r="H68" s="381"/>
       <c r="I68" s="188"/>
       <c r="J68" s="188"/>
       <c r="K68" s="188"/>
       <c r="L68" s="188"/>
-      <c r="M68" s="343"/>
-      <c r="N68" s="345"/>
+      <c r="M68" s="381"/>
+      <c r="N68" s="383"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="342"/>
+      <c r="B69" s="380"/>
       <c r="C69" s="186"/>
       <c r="D69" s="188"/>
       <c r="E69" s="188"/>
       <c r="F69" s="188"/>
       <c r="G69" s="188"/>
-      <c r="H69" s="343"/>
+      <c r="H69" s="381"/>
       <c r="I69" s="188"/>
       <c r="J69" s="188"/>
       <c r="K69" s="188"/>
       <c r="L69" s="188"/>
-      <c r="M69" s="343"/>
-      <c r="N69" s="345"/>
+      <c r="M69" s="381"/>
+      <c r="N69" s="383"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="342"/>
+      <c r="B70" s="380"/>
       <c r="C70" s="186"/>
       <c r="D70" s="188"/>
       <c r="E70" s="188"/>
       <c r="F70" s="188"/>
       <c r="G70" s="188"/>
-      <c r="H70" s="343"/>
+      <c r="H70" s="381"/>
       <c r="I70" s="188"/>
       <c r="J70" s="188"/>
       <c r="K70" s="188"/>
       <c r="L70" s="188"/>
-      <c r="M70" s="343"/>
-      <c r="N70" s="344"/>
+      <c r="M70" s="381"/>
+      <c r="N70" s="382"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="342"/>
+      <c r="B71" s="380"/>
       <c r="C71" s="186"/>
       <c r="D71" s="188"/>
       <c r="E71" s="188"/>
       <c r="F71" s="188"/>
       <c r="G71" s="188"/>
-      <c r="H71" s="343"/>
+      <c r="H71" s="381"/>
       <c r="I71" s="188"/>
       <c r="J71" s="188"/>
       <c r="K71" s="188"/>
       <c r="L71" s="188"/>
-      <c r="M71" s="343"/>
-      <c r="N71" s="345"/>
+      <c r="M71" s="381"/>
+      <c r="N71" s="383"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="342"/>
+      <c r="B72" s="380"/>
       <c r="C72" s="186"/>
       <c r="D72" s="188"/>
       <c r="E72" s="188"/>
       <c r="F72" s="188"/>
       <c r="G72" s="188"/>
-      <c r="H72" s="343"/>
+      <c r="H72" s="381"/>
       <c r="I72" s="188"/>
       <c r="J72" s="188"/>
       <c r="K72" s="188"/>
       <c r="L72" s="188"/>
-      <c r="M72" s="343"/>
-      <c r="N72" s="345"/>
+      <c r="M72" s="381"/>
+      <c r="N72" s="383"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="342"/>
+      <c r="B73" s="380"/>
       <c r="C73" s="186"/>
       <c r="D73" s="188"/>
       <c r="E73" s="188"/>
       <c r="F73" s="188"/>
       <c r="G73" s="188"/>
-      <c r="H73" s="343"/>
+      <c r="H73" s="381"/>
       <c r="I73" s="188"/>
       <c r="J73" s="188"/>
       <c r="K73" s="188"/>
       <c r="L73" s="188"/>
-      <c r="M73" s="343"/>
-      <c r="N73" s="345"/>
+      <c r="M73" s="381"/>
+      <c r="N73" s="383"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>
@@ -9433,23 +9433,57 @@
     <row r="140" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="N70:N73"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="M62:M65"/>
+    <mergeCell ref="N62:N65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="M66:M69"/>
+    <mergeCell ref="N66:N69"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="M54:M57"/>
+    <mergeCell ref="N54:N57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="N58:N61"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="M46:M49"/>
+    <mergeCell ref="N46:N49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="M50:M53"/>
+    <mergeCell ref="N50:N53"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="M42:M45"/>
+    <mergeCell ref="N42:N45"/>
+    <mergeCell ref="R21:R24"/>
+    <mergeCell ref="S21:S24"/>
+    <mergeCell ref="T21:T24"/>
+    <mergeCell ref="U21:U24"/>
+    <mergeCell ref="O21:O24"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="Q21:Q24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="M21:M24"/>
+    <mergeCell ref="N21:N24"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="U17:U20"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="R13:R16"/>
     <mergeCell ref="S13:S16"/>
@@ -9466,57 +9500,23 @@
     <mergeCell ref="N13:N16"/>
     <mergeCell ref="O13:O16"/>
     <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="U17:U20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="M21:M24"/>
-    <mergeCell ref="N21:N24"/>
-    <mergeCell ref="N42:N45"/>
-    <mergeCell ref="R21:R24"/>
-    <mergeCell ref="S21:S24"/>
-    <mergeCell ref="T21:T24"/>
-    <mergeCell ref="U21:U24"/>
-    <mergeCell ref="O21:O24"/>
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="Q21:Q24"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="M42:M45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="M46:M49"/>
-    <mergeCell ref="N46:N49"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="H50:H53"/>
-    <mergeCell ref="M50:M53"/>
-    <mergeCell ref="N50:N53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="M54:M57"/>
-    <mergeCell ref="N54:N57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="N58:N61"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="M70:M73"/>
-    <mergeCell ref="N70:N73"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="M62:M65"/>
-    <mergeCell ref="N62:N65"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="M66:M69"/>
-    <mergeCell ref="N66:N69"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">
@@ -9534,7 +9534,7 @@
   <dimension ref="A1:AU434"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -9582,15 +9582,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="380" t="s">
+      <c r="F1" s="345" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="380"/>
-      <c r="H1" s="380"/>
-      <c r="I1" s="380"/>
-      <c r="J1" s="380"/>
-      <c r="K1" s="380"/>
-      <c r="L1" s="380"/>
+      <c r="G1" s="345"/>
+      <c r="H1" s="345"/>
+      <c r="I1" s="345"/>
+      <c r="J1" s="345"/>
+      <c r="K1" s="345"/>
+      <c r="L1" s="345"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -9639,22 +9639,22 @@
       <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="381" t="s">
+      <c r="D6" s="346" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="382"/>
-      <c r="F6" s="382"/>
-      <c r="G6" s="382"/>
-      <c r="H6" s="383"/>
+      <c r="E6" s="347"/>
+      <c r="F6" s="347"/>
+      <c r="G6" s="347"/>
+      <c r="H6" s="348"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="381" t="s">
+      <c r="M6" s="346" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="382"/>
-      <c r="O6" s="382"/>
-      <c r="P6" s="382"/>
-      <c r="Q6" s="383"/>
+      <c r="N6" s="347"/>
+      <c r="O6" s="347"/>
+      <c r="P6" s="347"/>
+      <c r="Q6" s="348"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -9672,10 +9672,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="384" t="s">
+      <c r="F7" s="349" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="385"/>
+      <c r="G7" s="350"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -9698,10 +9698,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="384" t="s">
+      <c r="P7" s="349" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="385"/>
+      <c r="Q7" s="350"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -9769,7 +9769,7 @@
     </row>
     <row r="9" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="39"/>
-      <c r="B9" s="372"/>
+      <c r="B9" s="351"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
       <c r="E9" s="40"/>
@@ -9780,15 +9780,15 @@
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="42"/>
-      <c r="M9" s="363"/>
-      <c r="N9" s="375"/>
-      <c r="O9" s="363"/>
-      <c r="P9" s="363"/>
-      <c r="Q9" s="363"/>
-      <c r="R9" s="363"/>
-      <c r="S9" s="363"/>
-      <c r="T9" s="366"/>
-      <c r="U9" s="363"/>
+      <c r="M9" s="342"/>
+      <c r="N9" s="354"/>
+      <c r="O9" s="342"/>
+      <c r="P9" s="342"/>
+      <c r="Q9" s="342"/>
+      <c r="R9" s="342"/>
+      <c r="S9" s="342"/>
+      <c r="T9" s="357"/>
+      <c r="U9" s="342"/>
       <c r="V9" s="41"/>
       <c r="W9" s="36"/>
       <c r="X9" s="36"/>
@@ -9798,7 +9798,7 @@
     </row>
     <row r="10" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
-      <c r="B10" s="373"/>
+      <c r="B10" s="352"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
@@ -9809,15 +9809,15 @@
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
       <c r="L10" s="42"/>
-      <c r="M10" s="364"/>
-      <c r="N10" s="376"/>
-      <c r="O10" s="364"/>
-      <c r="P10" s="364"/>
-      <c r="Q10" s="364"/>
-      <c r="R10" s="364"/>
-      <c r="S10" s="364"/>
-      <c r="T10" s="367"/>
-      <c r="U10" s="364"/>
+      <c r="M10" s="343"/>
+      <c r="N10" s="355"/>
+      <c r="O10" s="343"/>
+      <c r="P10" s="343"/>
+      <c r="Q10" s="343"/>
+      <c r="R10" s="343"/>
+      <c r="S10" s="343"/>
+      <c r="T10" s="358"/>
+      <c r="U10" s="343"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -9825,8 +9825,8 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="363"/>
-      <c r="B11" s="373"/>
+      <c r="A11" s="342"/>
+      <c r="B11" s="352"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -9837,15 +9837,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="364"/>
-      <c r="N11" s="376"/>
-      <c r="O11" s="364"/>
-      <c r="P11" s="364"/>
-      <c r="Q11" s="364"/>
-      <c r="R11" s="364"/>
-      <c r="S11" s="364"/>
-      <c r="T11" s="367"/>
-      <c r="U11" s="364"/>
+      <c r="M11" s="343"/>
+      <c r="N11" s="355"/>
+      <c r="O11" s="343"/>
+      <c r="P11" s="343"/>
+      <c r="Q11" s="343"/>
+      <c r="R11" s="343"/>
+      <c r="S11" s="343"/>
+      <c r="T11" s="358"/>
+      <c r="U11" s="343"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -9855,8 +9855,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="365"/>
-      <c r="B12" s="374"/>
+      <c r="A12" s="344"/>
+      <c r="B12" s="353"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -9867,15 +9867,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="365"/>
-      <c r="N12" s="377"/>
-      <c r="O12" s="365"/>
-      <c r="P12" s="365"/>
-      <c r="Q12" s="365"/>
-      <c r="R12" s="365"/>
-      <c r="S12" s="365"/>
-      <c r="T12" s="368"/>
-      <c r="U12" s="365"/>
+      <c r="M12" s="344"/>
+      <c r="N12" s="356"/>
+      <c r="O12" s="344"/>
+      <c r="P12" s="344"/>
+      <c r="Q12" s="344"/>
+      <c r="R12" s="344"/>
+      <c r="S12" s="344"/>
+      <c r="T12" s="359"/>
+      <c r="U12" s="344"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -9884,7 +9884,7 @@
     </row>
     <row r="13" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="43"/>
-      <c r="B13" s="372"/>
+      <c r="B13" s="351"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
@@ -9895,15 +9895,15 @@
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
       <c r="L13" s="42"/>
-      <c r="M13" s="363"/>
-      <c r="N13" s="375"/>
-      <c r="O13" s="363"/>
-      <c r="P13" s="363"/>
-      <c r="Q13" s="363"/>
-      <c r="R13" s="363"/>
-      <c r="S13" s="363"/>
-      <c r="T13" s="366"/>
-      <c r="U13" s="363"/>
+      <c r="M13" s="342"/>
+      <c r="N13" s="354"/>
+      <c r="O13" s="342"/>
+      <c r="P13" s="342"/>
+      <c r="Q13" s="342"/>
+      <c r="R13" s="342"/>
+      <c r="S13" s="342"/>
+      <c r="T13" s="357"/>
+      <c r="U13" s="342"/>
       <c r="V13" s="41"/>
       <c r="W13" s="36"/>
       <c r="X13" s="36"/>
@@ -9912,7 +9912,7 @@
     </row>
     <row r="14" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44"/>
-      <c r="B14" s="373"/>
+      <c r="B14" s="352"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
@@ -9923,15 +9923,15 @@
       <c r="J14" s="36"/>
       <c r="K14" s="36"/>
       <c r="L14" s="42"/>
-      <c r="M14" s="364"/>
-      <c r="N14" s="376"/>
-      <c r="O14" s="364"/>
-      <c r="P14" s="364"/>
-      <c r="Q14" s="364"/>
-      <c r="R14" s="364"/>
-      <c r="S14" s="364"/>
-      <c r="T14" s="367"/>
-      <c r="U14" s="364"/>
+      <c r="M14" s="343"/>
+      <c r="N14" s="355"/>
+      <c r="O14" s="343"/>
+      <c r="P14" s="343"/>
+      <c r="Q14" s="343"/>
+      <c r="R14" s="343"/>
+      <c r="S14" s="343"/>
+      <c r="T14" s="358"/>
+      <c r="U14" s="343"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -9939,8 +9939,8 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="378"/>
-      <c r="B15" s="373"/>
+      <c r="A15" s="360"/>
+      <c r="B15" s="352"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -9951,15 +9951,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="364"/>
-      <c r="N15" s="376"/>
-      <c r="O15" s="364"/>
-      <c r="P15" s="364"/>
-      <c r="Q15" s="364"/>
-      <c r="R15" s="364"/>
-      <c r="S15" s="364"/>
-      <c r="T15" s="367"/>
-      <c r="U15" s="364"/>
+      <c r="M15" s="343"/>
+      <c r="N15" s="355"/>
+      <c r="O15" s="343"/>
+      <c r="P15" s="343"/>
+      <c r="Q15" s="343"/>
+      <c r="R15" s="343"/>
+      <c r="S15" s="343"/>
+      <c r="T15" s="358"/>
+      <c r="U15" s="343"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -9967,8 +9967,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="379"/>
-      <c r="B16" s="374"/>
+      <c r="A16" s="361"/>
+      <c r="B16" s="353"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -9979,15 +9979,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="365"/>
-      <c r="N16" s="377"/>
-      <c r="O16" s="365"/>
-      <c r="P16" s="365"/>
-      <c r="Q16" s="365"/>
-      <c r="R16" s="365"/>
-      <c r="S16" s="365"/>
-      <c r="T16" s="368"/>
-      <c r="U16" s="365"/>
+      <c r="M16" s="344"/>
+      <c r="N16" s="356"/>
+      <c r="O16" s="344"/>
+      <c r="P16" s="344"/>
+      <c r="Q16" s="344"/>
+      <c r="R16" s="344"/>
+      <c r="S16" s="344"/>
+      <c r="T16" s="359"/>
+      <c r="U16" s="344"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -9996,7 +9996,7 @@
     </row>
     <row r="17" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
-      <c r="B17" s="372"/>
+      <c r="B17" s="351"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
       <c r="E17" s="40"/>
@@ -10007,15 +10007,15 @@
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
       <c r="L17" s="42"/>
-      <c r="M17" s="363"/>
-      <c r="N17" s="375"/>
-      <c r="O17" s="363"/>
-      <c r="P17" s="363"/>
-      <c r="Q17" s="363"/>
-      <c r="R17" s="363"/>
-      <c r="S17" s="363"/>
-      <c r="T17" s="366"/>
-      <c r="U17" s="363"/>
+      <c r="M17" s="342"/>
+      <c r="N17" s="354"/>
+      <c r="O17" s="342"/>
+      <c r="P17" s="342"/>
+      <c r="Q17" s="342"/>
+      <c r="R17" s="342"/>
+      <c r="S17" s="342"/>
+      <c r="T17" s="357"/>
+      <c r="U17" s="342"/>
       <c r="V17" s="41"/>
       <c r="W17" s="36"/>
       <c r="X17" s="36"/>
@@ -10024,7 +10024,7 @@
     </row>
     <row r="18" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="40"/>
-      <c r="B18" s="373"/>
+      <c r="B18" s="352"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
       <c r="E18" s="40"/>
@@ -10035,22 +10035,22 @@
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="364"/>
-      <c r="N18" s="376"/>
-      <c r="O18" s="364"/>
-      <c r="P18" s="364"/>
-      <c r="Q18" s="364"/>
-      <c r="R18" s="364"/>
-      <c r="S18" s="364"/>
-      <c r="T18" s="367"/>
-      <c r="U18" s="364"/>
+      <c r="M18" s="343"/>
+      <c r="N18" s="355"/>
+      <c r="O18" s="343"/>
+      <c r="P18" s="343"/>
+      <c r="Q18" s="343"/>
+      <c r="R18" s="343"/>
+      <c r="S18" s="343"/>
+      <c r="T18" s="358"/>
+      <c r="U18" s="343"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="363"/>
-      <c r="B19" s="373"/>
+      <c r="A19" s="342"/>
+      <c r="B19" s="352"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -10061,22 +10061,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="364"/>
-      <c r="N19" s="376"/>
-      <c r="O19" s="364"/>
-      <c r="P19" s="364"/>
-      <c r="Q19" s="364"/>
-      <c r="R19" s="364"/>
-      <c r="S19" s="364"/>
-      <c r="T19" s="367"/>
-      <c r="U19" s="364"/>
+      <c r="M19" s="343"/>
+      <c r="N19" s="355"/>
+      <c r="O19" s="343"/>
+      <c r="P19" s="343"/>
+      <c r="Q19" s="343"/>
+      <c r="R19" s="343"/>
+      <c r="S19" s="343"/>
+      <c r="T19" s="358"/>
+      <c r="U19" s="343"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="365"/>
-      <c r="B20" s="374"/>
+      <c r="A20" s="344"/>
+      <c r="B20" s="353"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -10087,22 +10087,22 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="365"/>
-      <c r="N20" s="377"/>
-      <c r="O20" s="365"/>
-      <c r="P20" s="365"/>
-      <c r="Q20" s="365"/>
-      <c r="R20" s="365"/>
-      <c r="S20" s="365"/>
-      <c r="T20" s="368"/>
-      <c r="U20" s="365"/>
+      <c r="M20" s="344"/>
+      <c r="N20" s="356"/>
+      <c r="O20" s="344"/>
+      <c r="P20" s="344"/>
+      <c r="Q20" s="344"/>
+      <c r="R20" s="344"/>
+      <c r="S20" s="344"/>
+      <c r="T20" s="359"/>
+      <c r="U20" s="344"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
     </row>
     <row r="21" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="39"/>
-      <c r="B21" s="372"/>
+      <c r="B21" s="351"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
@@ -10113,22 +10113,22 @@
       <c r="J21" s="36"/>
       <c r="K21" s="36"/>
       <c r="L21" s="42"/>
-      <c r="M21" s="363"/>
-      <c r="N21" s="375"/>
-      <c r="O21" s="363"/>
-      <c r="P21" s="363"/>
-      <c r="Q21" s="363"/>
-      <c r="R21" s="363"/>
-      <c r="S21" s="363"/>
-      <c r="T21" s="366"/>
-      <c r="U21" s="363"/>
+      <c r="M21" s="342"/>
+      <c r="N21" s="354"/>
+      <c r="O21" s="342"/>
+      <c r="P21" s="342"/>
+      <c r="Q21" s="342"/>
+      <c r="R21" s="342"/>
+      <c r="S21" s="342"/>
+      <c r="T21" s="357"/>
+      <c r="U21" s="342"/>
       <c r="V21" s="41"/>
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
     </row>
     <row r="22" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
-      <c r="B22" s="373"/>
+      <c r="B22" s="352"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
@@ -10139,22 +10139,22 @@
       <c r="J22" s="36"/>
       <c r="K22" s="36"/>
       <c r="L22" s="42"/>
-      <c r="M22" s="364"/>
-      <c r="N22" s="376"/>
-      <c r="O22" s="364"/>
-      <c r="P22" s="364"/>
-      <c r="Q22" s="364"/>
-      <c r="R22" s="364"/>
-      <c r="S22" s="364"/>
-      <c r="T22" s="367"/>
-      <c r="U22" s="364"/>
+      <c r="M22" s="343"/>
+      <c r="N22" s="355"/>
+      <c r="O22" s="343"/>
+      <c r="P22" s="343"/>
+      <c r="Q22" s="343"/>
+      <c r="R22" s="343"/>
+      <c r="S22" s="343"/>
+      <c r="T22" s="358"/>
+      <c r="U22" s="343"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="369"/>
-      <c r="B23" s="373"/>
+      <c r="A23" s="362"/>
+      <c r="B23" s="352"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -10165,22 +10165,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="364"/>
-      <c r="N23" s="376"/>
-      <c r="O23" s="364"/>
-      <c r="P23" s="364"/>
-      <c r="Q23" s="364"/>
-      <c r="R23" s="364"/>
-      <c r="S23" s="364"/>
-      <c r="T23" s="367"/>
-      <c r="U23" s="364"/>
+      <c r="M23" s="343"/>
+      <c r="N23" s="355"/>
+      <c r="O23" s="343"/>
+      <c r="P23" s="343"/>
+      <c r="Q23" s="343"/>
+      <c r="R23" s="343"/>
+      <c r="S23" s="343"/>
+      <c r="T23" s="358"/>
+      <c r="U23" s="343"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="370"/>
-      <c r="B24" s="374"/>
+      <c r="A24" s="363"/>
+      <c r="B24" s="353"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -10191,15 +10191,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="365"/>
-      <c r="N24" s="377"/>
-      <c r="O24" s="365"/>
-      <c r="P24" s="365"/>
-      <c r="Q24" s="365"/>
-      <c r="R24" s="365"/>
-      <c r="S24" s="365"/>
-      <c r="T24" s="368"/>
-      <c r="U24" s="365"/>
+      <c r="M24" s="344"/>
+      <c r="N24" s="356"/>
+      <c r="O24" s="344"/>
+      <c r="P24" s="344"/>
+      <c r="Q24" s="344"/>
+      <c r="R24" s="344"/>
+      <c r="S24" s="344"/>
+      <c r="T24" s="359"/>
+      <c r="U24" s="344"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -10511,10 +10511,10 @@
     </row>
     <row r="40" spans="1:41" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="314" t="s">
+        <v>245</v>
+      </c>
+      <c r="B40" s="315" t="s">
         <v>246</v>
-      </c>
-      <c r="B40" s="315" t="s">
-        <v>245</v>
       </c>
       <c r="D40" s="104"/>
       <c r="E40" s="105"/>
@@ -18335,44 +18335,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="S13:S16"/>
-    <mergeCell ref="T13:T16"/>
-    <mergeCell ref="U13:U16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="U17:U20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
     <mergeCell ref="Q40:Y40"/>
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="J40:M40"/>
@@ -18387,6 +18349,44 @@
     <mergeCell ref="R21:R24"/>
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
+    <mergeCell ref="U17:U20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="T13:T16"/>
+    <mergeCell ref="U13:U16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q9:Q12"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">
@@ -18448,15 +18448,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="380" t="s">
+      <c r="F1" s="345" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="380"/>
-      <c r="H1" s="380"/>
-      <c r="I1" s="380"/>
-      <c r="J1" s="380"/>
-      <c r="K1" s="380"/>
-      <c r="L1" s="380"/>
+      <c r="G1" s="345"/>
+      <c r="H1" s="345"/>
+      <c r="I1" s="345"/>
+      <c r="J1" s="345"/>
+      <c r="K1" s="345"/>
+      <c r="L1" s="345"/>
       <c r="U1" s="22" t="s">
         <v>62</v>
       </c>
@@ -18545,22 +18545,22 @@
       </c>
     </row>
     <row r="6" spans="1:47" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="381" t="s">
+      <c r="D6" s="346" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="382"/>
-      <c r="F6" s="382"/>
-      <c r="G6" s="382"/>
-      <c r="H6" s="383"/>
+      <c r="E6" s="347"/>
+      <c r="F6" s="347"/>
+      <c r="G6" s="347"/>
+      <c r="H6" s="348"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="M6" s="381" t="s">
+      <c r="M6" s="346" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="382"/>
-      <c r="O6" s="382"/>
-      <c r="P6" s="382"/>
-      <c r="Q6" s="383"/>
+      <c r="N6" s="347"/>
+      <c r="O6" s="347"/>
+      <c r="P6" s="347"/>
+      <c r="Q6" s="348"/>
     </row>
     <row r="7" spans="1:47" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="24" t="s">
@@ -18578,10 +18578,10 @@
       <c r="E7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="384" t="s">
+      <c r="F7" s="349" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="385"/>
+      <c r="G7" s="350"/>
       <c r="H7" s="24" t="s">
         <v>73</v>
       </c>
@@ -18604,10 +18604,10 @@
         <v>79</v>
       </c>
       <c r="O7" s="29"/>
-      <c r="P7" s="384" t="s">
+      <c r="P7" s="349" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="385"/>
+      <c r="Q7" s="350"/>
       <c r="R7" s="30" t="s">
         <v>74</v>
       </c>
@@ -18684,7 +18684,7 @@
       <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="372" t="s">
+      <c r="B9" s="351" t="s">
         <v>194</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -18718,33 +18718,33 @@
         <f t="shared" ref="L9:L22" si="0">MIN(I9:K9)</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M9" s="363">
+      <c r="M9" s="342">
         <v>20</v>
       </c>
-      <c r="N9" s="375" t="s">
+      <c r="N9" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="363">
+      <c r="O9" s="342">
         <f>IF(N9="daily",1,IF(N9="week",7,IF(N9="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P9" s="363">
+      <c r="P9" s="342">
         <v>3</v>
       </c>
-      <c r="Q9" s="363">
+      <c r="Q9" s="342">
         <f>P9/O9</f>
         <v>3</v>
       </c>
-      <c r="R9" s="363">
+      <c r="R9" s="342">
         <f>M9*Q9</f>
         <v>60</v>
       </c>
-      <c r="S9" s="363"/>
-      <c r="T9" s="366">
+      <c r="S9" s="342"/>
+      <c r="T9" s="357">
         <f>MIN(R9:S12)</f>
         <v>60</v>
       </c>
-      <c r="U9" s="363">
+      <c r="U9" s="342">
         <v>500</v>
       </c>
       <c r="V9" s="41">
@@ -18769,7 +18769,7 @@
       <c r="A10" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="373"/>
+      <c r="B10" s="352"/>
       <c r="C10" s="40" t="s">
         <v>198</v>
       </c>
@@ -18801,15 +18801,15 @@
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
-      <c r="M10" s="364"/>
-      <c r="N10" s="376"/>
-      <c r="O10" s="364"/>
-      <c r="P10" s="364"/>
-      <c r="Q10" s="364"/>
-      <c r="R10" s="364"/>
-      <c r="S10" s="364"/>
-      <c r="T10" s="367"/>
-      <c r="U10" s="364"/>
+      <c r="M10" s="343"/>
+      <c r="N10" s="355"/>
+      <c r="O10" s="343"/>
+      <c r="P10" s="343"/>
+      <c r="Q10" s="343"/>
+      <c r="R10" s="343"/>
+      <c r="S10" s="343"/>
+      <c r="T10" s="358"/>
+      <c r="U10" s="343"/>
       <c r="V10" s="41"/>
       <c r="W10" s="36"/>
       <c r="X10" s="36"/>
@@ -18817,10 +18817,10 @@
       <c r="AK10" s="46"/>
     </row>
     <row r="11" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="363" t="s">
+      <c r="A11" s="342" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="373"/>
+      <c r="B11" s="352"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
@@ -18831,15 +18831,15 @@
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="364"/>
-      <c r="N11" s="376"/>
-      <c r="O11" s="364"/>
-      <c r="P11" s="364"/>
-      <c r="Q11" s="364"/>
-      <c r="R11" s="364"/>
-      <c r="S11" s="364"/>
-      <c r="T11" s="367"/>
-      <c r="U11" s="364"/>
+      <c r="M11" s="343"/>
+      <c r="N11" s="355"/>
+      <c r="O11" s="343"/>
+      <c r="P11" s="343"/>
+      <c r="Q11" s="343"/>
+      <c r="R11" s="343"/>
+      <c r="S11" s="343"/>
+      <c r="T11" s="358"/>
+      <c r="U11" s="343"/>
       <c r="V11" s="41"/>
       <c r="W11" s="36"/>
       <c r="X11" s="36"/>
@@ -18858,8 +18858,8 @@
       <c r="AU11" s="65"/>
     </row>
     <row r="12" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="365"/>
-      <c r="B12" s="374"/>
+      <c r="A12" s="344"/>
+      <c r="B12" s="353"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
@@ -18870,15 +18870,15 @@
       <c r="J12" s="36"/>
       <c r="K12" s="36"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="365"/>
-      <c r="N12" s="377"/>
-      <c r="O12" s="365"/>
-      <c r="P12" s="365"/>
-      <c r="Q12" s="365"/>
-      <c r="R12" s="365"/>
-      <c r="S12" s="365"/>
-      <c r="T12" s="368"/>
-      <c r="U12" s="365"/>
+      <c r="M12" s="344"/>
+      <c r="N12" s="356"/>
+      <c r="O12" s="344"/>
+      <c r="P12" s="344"/>
+      <c r="Q12" s="344"/>
+      <c r="R12" s="344"/>
+      <c r="S12" s="344"/>
+      <c r="T12" s="359"/>
+      <c r="U12" s="344"/>
       <c r="V12" s="41"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
@@ -18894,7 +18894,7 @@
       <c r="A13" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="372" t="s">
+      <c r="B13" s="351" t="s">
         <v>195</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -18928,33 +18928,33 @@
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="M13" s="363">
+      <c r="M13" s="342">
         <v>80</v>
       </c>
-      <c r="N13" s="375" t="s">
+      <c r="N13" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="363">
+      <c r="O13" s="342">
         <f>IF(N13="daily",1,IF(N13="week",7,IF(N13="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P13" s="363">
+      <c r="P13" s="342">
         <v>2</v>
       </c>
-      <c r="Q13" s="363">
+      <c r="Q13" s="342">
         <f>P13/O13</f>
         <v>2</v>
       </c>
-      <c r="R13" s="363">
+      <c r="R13" s="342">
         <f>M13*Q13</f>
         <v>160</v>
       </c>
-      <c r="S13" s="363"/>
-      <c r="T13" s="366">
+      <c r="S13" s="342"/>
+      <c r="T13" s="357">
         <f>MIN(R13:S16)</f>
         <v>160</v>
       </c>
-      <c r="U13" s="363">
+      <c r="U13" s="342">
         <v>600</v>
       </c>
       <c r="V13" s="41">
@@ -18977,7 +18977,7 @@
       <c r="A14" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="373"/>
+      <c r="B14" s="352"/>
       <c r="C14" s="40" t="s">
         <v>200</v>
       </c>
@@ -19009,15 +19009,15 @@
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="M14" s="364"/>
-      <c r="N14" s="376"/>
-      <c r="O14" s="364"/>
-      <c r="P14" s="364"/>
-      <c r="Q14" s="364"/>
-      <c r="R14" s="364"/>
-      <c r="S14" s="364"/>
-      <c r="T14" s="367"/>
-      <c r="U14" s="364"/>
+      <c r="M14" s="343"/>
+      <c r="N14" s="355"/>
+      <c r="O14" s="343"/>
+      <c r="P14" s="343"/>
+      <c r="Q14" s="343"/>
+      <c r="R14" s="343"/>
+      <c r="S14" s="343"/>
+      <c r="T14" s="358"/>
+      <c r="U14" s="343"/>
       <c r="V14" s="41"/>
       <c r="W14" s="36"/>
       <c r="X14" s="36"/>
@@ -19025,10 +19025,10 @@
       <c r="AT14" s="70"/>
     </row>
     <row r="15" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="378" t="s">
+      <c r="A15" s="360" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="373"/>
+      <c r="B15" s="352"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
@@ -19039,15 +19039,15 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="42"/>
-      <c r="M15" s="364"/>
-      <c r="N15" s="376"/>
-      <c r="O15" s="364"/>
-      <c r="P15" s="364"/>
-      <c r="Q15" s="364"/>
-      <c r="R15" s="364"/>
-      <c r="S15" s="364"/>
-      <c r="T15" s="367"/>
-      <c r="U15" s="364"/>
+      <c r="M15" s="343"/>
+      <c r="N15" s="355"/>
+      <c r="O15" s="343"/>
+      <c r="P15" s="343"/>
+      <c r="Q15" s="343"/>
+      <c r="R15" s="343"/>
+      <c r="S15" s="343"/>
+      <c r="T15" s="358"/>
+      <c r="U15" s="343"/>
       <c r="V15" s="41"/>
       <c r="W15" s="36"/>
       <c r="X15" s="36"/>
@@ -19057,8 +19057,8 @@
       <c r="AT15" s="46"/>
     </row>
     <row r="16" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="379"/>
-      <c r="B16" s="374"/>
+      <c r="A16" s="361"/>
+      <c r="B16" s="353"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -19069,15 +19069,15 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="42"/>
-      <c r="M16" s="365"/>
-      <c r="N16" s="377"/>
-      <c r="O16" s="365"/>
-      <c r="P16" s="365"/>
-      <c r="Q16" s="365"/>
-      <c r="R16" s="365"/>
-      <c r="S16" s="365"/>
-      <c r="T16" s="368"/>
-      <c r="U16" s="365"/>
+      <c r="M16" s="344"/>
+      <c r="N16" s="356"/>
+      <c r="O16" s="344"/>
+      <c r="P16" s="344"/>
+      <c r="Q16" s="344"/>
+      <c r="R16" s="344"/>
+      <c r="S16" s="344"/>
+      <c r="T16" s="359"/>
+      <c r="U16" s="344"/>
       <c r="V16" s="41"/>
       <c r="W16" s="36"/>
       <c r="X16" s="36"/>
@@ -19088,7 +19088,7 @@
       <c r="A17" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="372" t="s">
+      <c r="B17" s="351" t="s">
         <v>196</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -19122,33 +19122,33 @@
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="M17" s="363">
+      <c r="M17" s="342">
         <v>70</v>
       </c>
-      <c r="N17" s="375" t="s">
+      <c r="N17" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O17" s="363">
+      <c r="O17" s="342">
         <f>IF(N17="daily",1,IF(N17="week",7,IF(N17="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P17" s="363">
+      <c r="P17" s="342">
         <v>2</v>
       </c>
-      <c r="Q17" s="363">
+      <c r="Q17" s="342">
         <f>P17/O17</f>
         <v>2</v>
       </c>
-      <c r="R17" s="363">
+      <c r="R17" s="342">
         <f>M17*Q17</f>
         <v>140</v>
       </c>
-      <c r="S17" s="363"/>
-      <c r="T17" s="366">
+      <c r="S17" s="342"/>
+      <c r="T17" s="357">
         <f>MIN(R17:S20)</f>
         <v>140</v>
       </c>
-      <c r="U17" s="363">
+      <c r="U17" s="342">
         <v>850</v>
       </c>
       <c r="V17" s="41">
@@ -19167,7 +19167,7 @@
       <c r="A18" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="373"/>
+      <c r="B18" s="352"/>
       <c r="C18" s="40" t="s">
         <v>202</v>
       </c>
@@ -19199,24 +19199,24 @@
         <f t="shared" si="0"/>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="M18" s="364"/>
-      <c r="N18" s="376"/>
-      <c r="O18" s="364"/>
-      <c r="P18" s="364"/>
-      <c r="Q18" s="364"/>
-      <c r="R18" s="364"/>
-      <c r="S18" s="364"/>
-      <c r="T18" s="367"/>
-      <c r="U18" s="364"/>
+      <c r="M18" s="343"/>
+      <c r="N18" s="355"/>
+      <c r="O18" s="343"/>
+      <c r="P18" s="343"/>
+      <c r="Q18" s="343"/>
+      <c r="R18" s="343"/>
+      <c r="S18" s="343"/>
+      <c r="T18" s="358"/>
+      <c r="U18" s="343"/>
       <c r="V18" s="41"/>
       <c r="W18" s="36"/>
       <c r="X18" s="36"/>
     </row>
     <row r="19" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="363" t="s">
+      <c r="A19" s="342" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="373"/>
+      <c r="B19" s="352"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
@@ -19227,22 +19227,22 @@
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="364"/>
-      <c r="N19" s="376"/>
-      <c r="O19" s="364"/>
-      <c r="P19" s="364"/>
-      <c r="Q19" s="364"/>
-      <c r="R19" s="364"/>
-      <c r="S19" s="364"/>
-      <c r="T19" s="367"/>
-      <c r="U19" s="364"/>
+      <c r="M19" s="343"/>
+      <c r="N19" s="355"/>
+      <c r="O19" s="343"/>
+      <c r="P19" s="343"/>
+      <c r="Q19" s="343"/>
+      <c r="R19" s="343"/>
+      <c r="S19" s="343"/>
+      <c r="T19" s="358"/>
+      <c r="U19" s="343"/>
       <c r="V19" s="41"/>
       <c r="W19" s="36"/>
       <c r="X19" s="36"/>
     </row>
     <row r="20" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="365"/>
-      <c r="B20" s="374"/>
+      <c r="A20" s="344"/>
+      <c r="B20" s="353"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
@@ -19253,15 +19253,15 @@
       <c r="J20" s="36"/>
       <c r="K20" s="36"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="365"/>
-      <c r="N20" s="377"/>
-      <c r="O20" s="365"/>
-      <c r="P20" s="365"/>
-      <c r="Q20" s="365"/>
-      <c r="R20" s="365"/>
-      <c r="S20" s="365"/>
-      <c r="T20" s="368"/>
-      <c r="U20" s="365"/>
+      <c r="M20" s="344"/>
+      <c r="N20" s="356"/>
+      <c r="O20" s="344"/>
+      <c r="P20" s="344"/>
+      <c r="Q20" s="344"/>
+      <c r="R20" s="344"/>
+      <c r="S20" s="344"/>
+      <c r="T20" s="359"/>
+      <c r="U20" s="344"/>
       <c r="V20" s="41"/>
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
@@ -19270,7 +19270,7 @@
       <c r="A21" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="372" t="s">
+      <c r="B21" s="351" t="s">
         <v>197</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -19304,33 +19304,33 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M21" s="363">
+      <c r="M21" s="342">
         <v>60</v>
       </c>
-      <c r="N21" s="375" t="s">
+      <c r="N21" s="354" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="363">
+      <c r="O21" s="342">
         <f>IF(N21="daily",1,IF(N21="week",7,IF(N21="month",30)))</f>
         <v>1</v>
       </c>
-      <c r="P21" s="363">
+      <c r="P21" s="342">
         <v>3</v>
       </c>
-      <c r="Q21" s="363">
+      <c r="Q21" s="342">
         <f>P21/O21</f>
         <v>3</v>
       </c>
-      <c r="R21" s="363">
+      <c r="R21" s="342">
         <f>M21*Q21</f>
         <v>180</v>
       </c>
-      <c r="S21" s="363"/>
-      <c r="T21" s="366">
+      <c r="S21" s="342"/>
+      <c r="T21" s="357">
         <f>MIN(R21:S24)</f>
         <v>180</v>
       </c>
-      <c r="U21" s="363">
+      <c r="U21" s="342">
         <v>700</v>
       </c>
       <c r="V21" s="41">
@@ -19347,7 +19347,7 @@
       <c r="A22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="373"/>
+      <c r="B22" s="352"/>
       <c r="C22" s="40" t="s">
         <v>204</v>
       </c>
@@ -19379,24 +19379,24 @@
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="M22" s="364"/>
-      <c r="N22" s="376"/>
-      <c r="O22" s="364"/>
-      <c r="P22" s="364"/>
-      <c r="Q22" s="364"/>
-      <c r="R22" s="364"/>
-      <c r="S22" s="364"/>
-      <c r="T22" s="367"/>
-      <c r="U22" s="364"/>
+      <c r="M22" s="343"/>
+      <c r="N22" s="355"/>
+      <c r="O22" s="343"/>
+      <c r="P22" s="343"/>
+      <c r="Q22" s="343"/>
+      <c r="R22" s="343"/>
+      <c r="S22" s="343"/>
+      <c r="T22" s="358"/>
+      <c r="U22" s="343"/>
       <c r="V22" s="41"/>
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
     <row r="23" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="369" t="s">
+      <c r="A23" s="362" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="373"/>
+      <c r="B23" s="352"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
@@ -19407,22 +19407,22 @@
       <c r="J23" s="36"/>
       <c r="K23" s="36"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="364"/>
-      <c r="N23" s="376"/>
-      <c r="O23" s="364"/>
-      <c r="P23" s="364"/>
-      <c r="Q23" s="364"/>
-      <c r="R23" s="364"/>
-      <c r="S23" s="364"/>
-      <c r="T23" s="367"/>
-      <c r="U23" s="364"/>
+      <c r="M23" s="343"/>
+      <c r="N23" s="355"/>
+      <c r="O23" s="343"/>
+      <c r="P23" s="343"/>
+      <c r="Q23" s="343"/>
+      <c r="R23" s="343"/>
+      <c r="S23" s="343"/>
+      <c r="T23" s="358"/>
+      <c r="U23" s="343"/>
       <c r="V23" s="41"/>
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
     <row r="24" spans="1:46" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="370"/>
-      <c r="B24" s="374"/>
+      <c r="A24" s="363"/>
+      <c r="B24" s="353"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -19433,15 +19433,15 @@
       <c r="J24" s="36"/>
       <c r="K24" s="36"/>
       <c r="L24" s="42"/>
-      <c r="M24" s="365"/>
-      <c r="N24" s="377"/>
-      <c r="O24" s="365"/>
-      <c r="P24" s="365"/>
-      <c r="Q24" s="365"/>
-      <c r="R24" s="365"/>
-      <c r="S24" s="365"/>
-      <c r="T24" s="368"/>
-      <c r="U24" s="365"/>
+      <c r="M24" s="344"/>
+      <c r="N24" s="356"/>
+      <c r="O24" s="344"/>
+      <c r="P24" s="344"/>
+      <c r="Q24" s="344"/>
+      <c r="R24" s="344"/>
+      <c r="S24" s="344"/>
+      <c r="T24" s="359"/>
+      <c r="U24" s="344"/>
       <c r="V24" s="41"/>
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
@@ -19467,13 +19467,13 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="371" t="s">
+      <c r="H27" s="364" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="371"/>
-      <c r="J27" s="371"/>
-      <c r="K27" s="371"/>
-      <c r="L27" s="371"/>
+      <c r="I27" s="364"/>
+      <c r="J27" s="364"/>
+      <c r="K27" s="364"/>
+      <c r="L27" s="364"/>
       <c r="M27" s="48"/>
       <c r="N27" s="48"/>
       <c r="O27" s="46"/>
@@ -19753,19 +19753,19 @@
     <row r="40" spans="1:40" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="104"/>
       <c r="C40" s="105"/>
-      <c r="D40" s="361" t="s">
+      <c r="D40" s="367" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="361"/>
-      <c r="F40" s="361"/>
-      <c r="G40" s="361"/>
-      <c r="H40" s="361"/>
-      <c r="I40" s="361" t="s">
+      <c r="E40" s="367"/>
+      <c r="F40" s="367"/>
+      <c r="G40" s="367"/>
+      <c r="H40" s="367"/>
+      <c r="I40" s="367" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="361"/>
-      <c r="K40" s="361"/>
-      <c r="L40" s="361"/>
+      <c r="J40" s="367"/>
+      <c r="K40" s="367"/>
+      <c r="L40" s="367"/>
       <c r="M40" s="117"/>
       <c r="N40" s="118" t="s">
         <v>48</v>
@@ -19889,19 +19889,19 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="356"/>
+      <c r="B42" s="368"/>
       <c r="C42" s="110"/>
       <c r="D42" s="111"/>
       <c r="E42" s="111"/>
       <c r="F42" s="125"/>
       <c r="G42" s="125"/>
-      <c r="H42" s="357"/>
+      <c r="H42" s="366"/>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
       <c r="K42" s="125"/>
       <c r="L42" s="125"/>
-      <c r="M42" s="357"/>
-      <c r="N42" s="398"/>
+      <c r="M42" s="366"/>
+      <c r="N42" s="393"/>
       <c r="P42" s="91"/>
       <c r="Q42" s="91"/>
       <c r="U42" s="64"/>
@@ -19947,19 +19947,19 @@
       <c r="AN42" s="88"/>
     </row>
     <row r="43" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="356"/>
+      <c r="B43" s="368"/>
       <c r="C43" s="110"/>
       <c r="D43" s="125"/>
       <c r="E43" s="111"/>
       <c r="F43" s="125"/>
       <c r="G43" s="103"/>
-      <c r="H43" s="357"/>
+      <c r="H43" s="366"/>
       <c r="I43" s="111"/>
       <c r="J43" s="111"/>
       <c r="K43" s="103"/>
       <c r="L43" s="103"/>
-      <c r="M43" s="357"/>
-      <c r="N43" s="357"/>
+      <c r="M43" s="366"/>
+      <c r="N43" s="366"/>
       <c r="P43" s="92"/>
       <c r="Q43" s="92"/>
       <c r="U43" s="64"/>
@@ -20005,19 +20005,19 @@
       <c r="AN43" s="88"/>
     </row>
     <row r="44" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="356"/>
+      <c r="B44" s="368"/>
       <c r="C44" s="110"/>
       <c r="D44" s="111"/>
       <c r="E44" s="111"/>
       <c r="F44" s="125"/>
       <c r="G44" s="125"/>
-      <c r="H44" s="357"/>
+      <c r="H44" s="366"/>
       <c r="I44" s="111"/>
       <c r="J44" s="111"/>
       <c r="K44" s="125"/>
       <c r="L44" s="125"/>
-      <c r="M44" s="357"/>
-      <c r="N44" s="357"/>
+      <c r="M44" s="366"/>
+      <c r="N44" s="366"/>
       <c r="P44" s="91"/>
       <c r="Q44" s="91"/>
       <c r="U44" s="64"/>
@@ -20063,19 +20063,19 @@
       <c r="AN44" s="88"/>
     </row>
     <row r="45" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="356"/>
+      <c r="B45" s="368"/>
       <c r="C45" s="110"/>
       <c r="D45" s="111"/>
       <c r="E45" s="111"/>
       <c r="F45" s="125"/>
       <c r="G45" s="125"/>
-      <c r="H45" s="357"/>
+      <c r="H45" s="366"/>
       <c r="I45" s="111"/>
       <c r="J45" s="111"/>
       <c r="K45" s="125"/>
       <c r="L45" s="125"/>
-      <c r="M45" s="357"/>
-      <c r="N45" s="357"/>
+      <c r="M45" s="366"/>
+      <c r="N45" s="366"/>
       <c r="P45" s="91"/>
       <c r="Q45" s="91"/>
       <c r="U45" s="64"/>
@@ -20121,19 +20121,19 @@
       <c r="AN45" s="88"/>
     </row>
     <row r="46" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="356"/>
+      <c r="B46" s="368"/>
       <c r="C46" s="110"/>
       <c r="D46" s="111"/>
       <c r="E46" s="111"/>
       <c r="F46" s="125"/>
       <c r="G46" s="125"/>
-      <c r="H46" s="357"/>
+      <c r="H46" s="366"/>
       <c r="I46" s="111"/>
       <c r="J46" s="111"/>
       <c r="K46" s="125"/>
       <c r="L46" s="125"/>
-      <c r="M46" s="357"/>
-      <c r="N46" s="399"/>
+      <c r="M46" s="366"/>
+      <c r="N46" s="394"/>
       <c r="P46" s="91"/>
       <c r="Q46" s="91"/>
       <c r="U46" s="64"/>
@@ -20179,19 +20179,19 @@
       <c r="AN46" s="88"/>
     </row>
     <row r="47" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="356"/>
+      <c r="B47" s="368"/>
       <c r="C47" s="110"/>
       <c r="D47" s="111"/>
       <c r="E47" s="111"/>
       <c r="F47" s="111"/>
       <c r="G47" s="111"/>
-      <c r="H47" s="357"/>
+      <c r="H47" s="366"/>
       <c r="I47" s="111"/>
       <c r="J47" s="111"/>
       <c r="K47" s="111"/>
       <c r="L47" s="111"/>
-      <c r="M47" s="357"/>
-      <c r="N47" s="359"/>
+      <c r="M47" s="366"/>
+      <c r="N47" s="370"/>
       <c r="P47" s="81"/>
       <c r="Q47" s="81"/>
       <c r="S47" s="69"/>
@@ -20239,19 +20239,19 @@
       <c r="AN47" s="88"/>
     </row>
     <row r="48" spans="1:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="356"/>
+      <c r="B48" s="368"/>
       <c r="C48" s="110"/>
       <c r="D48" s="111"/>
       <c r="E48" s="111"/>
       <c r="F48" s="111"/>
       <c r="G48" s="111"/>
-      <c r="H48" s="357"/>
+      <c r="H48" s="366"/>
       <c r="I48" s="111"/>
       <c r="J48" s="111"/>
       <c r="K48" s="111"/>
       <c r="L48" s="111"/>
-      <c r="M48" s="357"/>
-      <c r="N48" s="359"/>
+      <c r="M48" s="366"/>
+      <c r="N48" s="370"/>
       <c r="P48" s="81"/>
       <c r="Q48" s="81"/>
       <c r="S48" s="69"/>
@@ -20299,19 +20299,19 @@
       <c r="AN48" s="88"/>
     </row>
     <row r="49" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="356"/>
+      <c r="B49" s="368"/>
       <c r="C49" s="110"/>
       <c r="D49" s="111"/>
       <c r="E49" s="111"/>
       <c r="F49" s="111"/>
       <c r="G49" s="111"/>
-      <c r="H49" s="357"/>
+      <c r="H49" s="366"/>
       <c r="I49" s="111"/>
       <c r="J49" s="111"/>
       <c r="K49" s="111"/>
       <c r="L49" s="111"/>
-      <c r="M49" s="357"/>
-      <c r="N49" s="359"/>
+      <c r="M49" s="366"/>
+      <c r="N49" s="370"/>
       <c r="P49" s="81"/>
       <c r="Q49" s="81"/>
       <c r="S49" s="69"/>
@@ -20359,19 +20359,19 @@
       <c r="AN49" s="89"/>
     </row>
     <row r="50" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="351"/>
+      <c r="B50" s="371"/>
       <c r="C50" s="112"/>
       <c r="D50" s="113"/>
       <c r="E50" s="113"/>
       <c r="F50" s="113"/>
       <c r="G50" s="113"/>
-      <c r="H50" s="352"/>
+      <c r="H50" s="372"/>
       <c r="I50" s="113"/>
       <c r="J50" s="113"/>
       <c r="K50" s="113"/>
       <c r="L50" s="113"/>
-      <c r="M50" s="352"/>
-      <c r="N50" s="400"/>
+      <c r="M50" s="372"/>
+      <c r="N50" s="395"/>
       <c r="P50" s="81"/>
       <c r="Q50" s="81"/>
       <c r="S50" s="69"/>
@@ -20392,19 +20392,19 @@
       <c r="AN50" s="64"/>
     </row>
     <row r="51" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="351"/>
+      <c r="B51" s="371"/>
       <c r="C51" s="112"/>
       <c r="D51" s="113"/>
       <c r="E51" s="113"/>
       <c r="F51" s="113"/>
       <c r="G51" s="113"/>
-      <c r="H51" s="352"/>
+      <c r="H51" s="372"/>
       <c r="I51" s="113"/>
       <c r="J51" s="113"/>
       <c r="K51" s="113"/>
       <c r="L51" s="113"/>
-      <c r="M51" s="352"/>
-      <c r="N51" s="354"/>
+      <c r="M51" s="372"/>
+      <c r="N51" s="374"/>
       <c r="P51" s="81"/>
       <c r="Q51" s="81"/>
       <c r="S51" s="69"/>
@@ -20435,19 +20435,19 @@
       <c r="AN51" s="46"/>
     </row>
     <row r="52" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="351"/>
+      <c r="B52" s="371"/>
       <c r="C52" s="112"/>
       <c r="D52" s="113"/>
       <c r="E52" s="113"/>
       <c r="F52" s="113"/>
       <c r="G52" s="113"/>
-      <c r="H52" s="352"/>
+      <c r="H52" s="372"/>
       <c r="I52" s="113"/>
       <c r="J52" s="113"/>
       <c r="K52" s="113"/>
       <c r="L52" s="113"/>
-      <c r="M52" s="352"/>
-      <c r="N52" s="354"/>
+      <c r="M52" s="372"/>
+      <c r="N52" s="374"/>
       <c r="P52" s="81"/>
       <c r="Q52" s="81"/>
       <c r="S52" s="69"/>
@@ -20511,19 +20511,19 @@
       </c>
     </row>
     <row r="53" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="351"/>
+      <c r="B53" s="371"/>
       <c r="C53" s="112"/>
       <c r="D53" s="113"/>
       <c r="E53" s="113"/>
       <c r="F53" s="113"/>
       <c r="G53" s="113"/>
-      <c r="H53" s="352"/>
+      <c r="H53" s="372"/>
       <c r="I53" s="113"/>
       <c r="J53" s="113"/>
       <c r="K53" s="113"/>
       <c r="L53" s="113"/>
-      <c r="M53" s="352"/>
-      <c r="N53" s="354"/>
+      <c r="M53" s="372"/>
+      <c r="N53" s="374"/>
       <c r="P53" s="81"/>
       <c r="Q53" s="81"/>
       <c r="S53" s="69"/>
@@ -20572,19 +20572,19 @@
       <c r="AN53" s="88"/>
     </row>
     <row r="54" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="351"/>
+      <c r="B54" s="371"/>
       <c r="C54" s="112"/>
       <c r="D54" s="113"/>
       <c r="E54" s="113"/>
       <c r="F54" s="113"/>
       <c r="G54" s="113"/>
-      <c r="H54" s="352"/>
+      <c r="H54" s="372"/>
       <c r="I54" s="113"/>
       <c r="J54" s="113"/>
       <c r="K54" s="113"/>
       <c r="L54" s="113"/>
-      <c r="M54" s="352"/>
-      <c r="N54" s="393"/>
+      <c r="M54" s="372"/>
+      <c r="N54" s="396"/>
       <c r="P54" s="81"/>
       <c r="Q54" s="81"/>
       <c r="S54" s="69"/>
@@ -20631,19 +20631,19 @@
       <c r="AN54" s="88"/>
     </row>
     <row r="55" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="351"/>
+      <c r="B55" s="371"/>
       <c r="C55" s="112"/>
       <c r="D55" s="113"/>
       <c r="E55" s="113"/>
       <c r="F55" s="113"/>
       <c r="G55" s="113"/>
-      <c r="H55" s="352"/>
+      <c r="H55" s="372"/>
       <c r="I55" s="113"/>
       <c r="J55" s="113"/>
       <c r="K55" s="113"/>
       <c r="L55" s="113"/>
-      <c r="M55" s="352"/>
-      <c r="N55" s="354"/>
+      <c r="M55" s="372"/>
+      <c r="N55" s="374"/>
       <c r="P55" s="81"/>
       <c r="Q55" s="81"/>
       <c r="S55" s="69"/>
@@ -20690,19 +20690,19 @@
       <c r="AN55" s="88"/>
     </row>
     <row r="56" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="351"/>
+      <c r="B56" s="371"/>
       <c r="C56" s="112"/>
       <c r="D56" s="113"/>
       <c r="E56" s="113"/>
       <c r="F56" s="113"/>
       <c r="G56" s="113"/>
-      <c r="H56" s="352"/>
+      <c r="H56" s="372"/>
       <c r="I56" s="113"/>
       <c r="J56" s="113"/>
       <c r="K56" s="113"/>
       <c r="L56" s="113"/>
-      <c r="M56" s="352"/>
-      <c r="N56" s="354"/>
+      <c r="M56" s="372"/>
+      <c r="N56" s="374"/>
       <c r="P56" s="81"/>
       <c r="Q56" s="81"/>
       <c r="S56" s="69"/>
@@ -20749,19 +20749,19 @@
       <c r="AN56" s="88"/>
     </row>
     <row r="57" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="351"/>
+      <c r="B57" s="371"/>
       <c r="C57" s="112"/>
       <c r="D57" s="113"/>
       <c r="E57" s="113"/>
       <c r="F57" s="113"/>
       <c r="G57" s="113"/>
-      <c r="H57" s="352"/>
+      <c r="H57" s="372"/>
       <c r="I57" s="113"/>
       <c r="J57" s="113"/>
       <c r="K57" s="113"/>
       <c r="L57" s="113"/>
-      <c r="M57" s="352"/>
-      <c r="N57" s="354"/>
+      <c r="M57" s="372"/>
+      <c r="N57" s="374"/>
       <c r="P57" s="81"/>
       <c r="Q57" s="81"/>
       <c r="S57" s="69"/>
@@ -20808,19 +20808,19 @@
       <c r="AN57" s="88"/>
     </row>
     <row r="58" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="346"/>
+      <c r="B58" s="376"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
       <c r="E58" s="115"/>
       <c r="F58" s="115"/>
       <c r="G58" s="115"/>
-      <c r="H58" s="347"/>
+      <c r="H58" s="377"/>
       <c r="I58" s="115"/>
       <c r="J58" s="115"/>
       <c r="K58" s="115"/>
       <c r="L58" s="115"/>
-      <c r="M58" s="347"/>
-      <c r="N58" s="394"/>
+      <c r="M58" s="377"/>
+      <c r="N58" s="397"/>
       <c r="P58" s="81"/>
       <c r="Q58" s="81"/>
       <c r="S58" s="69"/>
@@ -20867,19 +20867,19 @@
       <c r="AN58" s="88"/>
     </row>
     <row r="59" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="346"/>
+      <c r="B59" s="376"/>
       <c r="C59" s="114"/>
       <c r="D59" s="115"/>
       <c r="E59" s="115"/>
       <c r="F59" s="115"/>
       <c r="G59" s="115"/>
-      <c r="H59" s="347"/>
+      <c r="H59" s="377"/>
       <c r="I59" s="115"/>
       <c r="J59" s="115"/>
       <c r="K59" s="115"/>
       <c r="L59" s="115"/>
-      <c r="M59" s="347"/>
-      <c r="N59" s="349"/>
+      <c r="M59" s="377"/>
+      <c r="N59" s="379"/>
       <c r="P59" s="81"/>
       <c r="Q59" s="81"/>
       <c r="S59" s="69"/>
@@ -20926,19 +20926,19 @@
       <c r="AN59" s="88"/>
     </row>
     <row r="60" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="346"/>
+      <c r="B60" s="376"/>
       <c r="C60" s="114"/>
       <c r="D60" s="115"/>
       <c r="E60" s="115"/>
       <c r="F60" s="115"/>
       <c r="G60" s="115"/>
-      <c r="H60" s="347"/>
+      <c r="H60" s="377"/>
       <c r="I60" s="115"/>
       <c r="J60" s="115"/>
       <c r="K60" s="115"/>
       <c r="L60" s="115"/>
-      <c r="M60" s="347"/>
-      <c r="N60" s="349"/>
+      <c r="M60" s="377"/>
+      <c r="N60" s="379"/>
       <c r="P60" s="81"/>
       <c r="Q60" s="81"/>
       <c r="S60" s="69"/>
@@ -20985,247 +20985,247 @@
       <c r="AN60" s="89"/>
     </row>
     <row r="61" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="346"/>
+      <c r="B61" s="376"/>
       <c r="C61" s="114"/>
       <c r="D61" s="115"/>
       <c r="E61" s="115"/>
       <c r="F61" s="115"/>
       <c r="G61" s="115"/>
-      <c r="H61" s="347"/>
+      <c r="H61" s="377"/>
       <c r="I61" s="115"/>
       <c r="J61" s="115"/>
       <c r="K61" s="115"/>
       <c r="L61" s="115"/>
-      <c r="M61" s="347"/>
-      <c r="N61" s="349"/>
+      <c r="M61" s="377"/>
+      <c r="N61" s="379"/>
       <c r="P61" s="81"/>
       <c r="Q61" s="81"/>
       <c r="S61" s="69"/>
       <c r="T61" s="69"/>
     </row>
     <row r="62" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="346"/>
+      <c r="B62" s="376"/>
       <c r="C62" s="114"/>
       <c r="D62" s="115"/>
       <c r="E62" s="115"/>
       <c r="F62" s="115"/>
       <c r="G62" s="115"/>
-      <c r="H62" s="347"/>
+      <c r="H62" s="377"/>
       <c r="I62" s="115"/>
       <c r="J62" s="115"/>
       <c r="K62" s="115"/>
       <c r="L62" s="115"/>
-      <c r="M62" s="347"/>
-      <c r="N62" s="395"/>
+      <c r="M62" s="377"/>
+      <c r="N62" s="398"/>
       <c r="P62" s="81"/>
       <c r="Q62" s="81"/>
       <c r="S62" s="69"/>
       <c r="T62" s="69"/>
     </row>
     <row r="63" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="346"/>
+      <c r="B63" s="376"/>
       <c r="C63" s="114"/>
       <c r="D63" s="115"/>
       <c r="E63" s="115"/>
       <c r="F63" s="115"/>
       <c r="G63" s="115"/>
-      <c r="H63" s="347"/>
+      <c r="H63" s="377"/>
       <c r="I63" s="115"/>
       <c r="J63" s="115"/>
       <c r="K63" s="115"/>
       <c r="L63" s="115"/>
-      <c r="M63" s="347"/>
-      <c r="N63" s="349"/>
+      <c r="M63" s="377"/>
+      <c r="N63" s="379"/>
       <c r="P63" s="81"/>
       <c r="Q63" s="81"/>
       <c r="S63" s="69"/>
       <c r="T63" s="69"/>
     </row>
     <row r="64" spans="2:40" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="346"/>
+      <c r="B64" s="376"/>
       <c r="C64" s="114"/>
       <c r="D64" s="115"/>
       <c r="E64" s="115"/>
       <c r="F64" s="115"/>
       <c r="G64" s="115"/>
-      <c r="H64" s="347"/>
+      <c r="H64" s="377"/>
       <c r="I64" s="115"/>
       <c r="J64" s="115"/>
       <c r="K64" s="115"/>
       <c r="L64" s="115"/>
-      <c r="M64" s="347"/>
-      <c r="N64" s="349"/>
+      <c r="M64" s="377"/>
+      <c r="N64" s="379"/>
       <c r="P64" s="81"/>
       <c r="Q64" s="81"/>
       <c r="S64" s="69"/>
       <c r="T64" s="69"/>
     </row>
     <row r="65" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="346"/>
+      <c r="B65" s="376"/>
       <c r="C65" s="114"/>
       <c r="D65" s="115"/>
       <c r="E65" s="115"/>
       <c r="F65" s="115"/>
       <c r="G65" s="115"/>
-      <c r="H65" s="347"/>
+      <c r="H65" s="377"/>
       <c r="I65" s="115"/>
       <c r="J65" s="115"/>
       <c r="K65" s="115"/>
       <c r="L65" s="115"/>
-      <c r="M65" s="347"/>
-      <c r="N65" s="349"/>
+      <c r="M65" s="377"/>
+      <c r="N65" s="379"/>
       <c r="P65" s="81"/>
       <c r="Q65" s="81"/>
       <c r="S65" s="69"/>
       <c r="T65" s="69"/>
     </row>
     <row r="66" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="342"/>
+      <c r="B66" s="380"/>
       <c r="C66" s="128"/>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
       <c r="F66" s="116"/>
       <c r="G66" s="116"/>
-      <c r="H66" s="343"/>
+      <c r="H66" s="381"/>
       <c r="I66" s="116"/>
       <c r="J66" s="116"/>
       <c r="K66" s="116"/>
       <c r="L66" s="116"/>
-      <c r="M66" s="343"/>
-      <c r="N66" s="396"/>
+      <c r="M66" s="381"/>
+      <c r="N66" s="399"/>
       <c r="P66" s="81"/>
       <c r="Q66" s="81"/>
       <c r="S66" s="69"/>
       <c r="T66" s="69"/>
     </row>
     <row r="67" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="342"/>
+      <c r="B67" s="380"/>
       <c r="C67" s="128"/>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
       <c r="F67" s="116"/>
       <c r="G67" s="116"/>
-      <c r="H67" s="343"/>
+      <c r="H67" s="381"/>
       <c r="I67" s="116"/>
       <c r="J67" s="116"/>
       <c r="K67" s="116"/>
       <c r="L67" s="116"/>
-      <c r="M67" s="343"/>
-      <c r="N67" s="345"/>
+      <c r="M67" s="381"/>
+      <c r="N67" s="383"/>
       <c r="P67" s="81"/>
       <c r="Q67" s="81"/>
       <c r="S67" s="69"/>
       <c r="T67" s="69"/>
     </row>
     <row r="68" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="342"/>
+      <c r="B68" s="380"/>
       <c r="C68" s="128"/>
       <c r="D68" s="116"/>
       <c r="E68" s="116"/>
       <c r="F68" s="116"/>
       <c r="G68" s="116"/>
-      <c r="H68" s="343"/>
+      <c r="H68" s="381"/>
       <c r="I68" s="116"/>
       <c r="J68" s="116"/>
       <c r="K68" s="116"/>
       <c r="L68" s="116"/>
-      <c r="M68" s="343"/>
-      <c r="N68" s="345"/>
+      <c r="M68" s="381"/>
+      <c r="N68" s="383"/>
       <c r="P68" s="81"/>
       <c r="Q68" s="81"/>
       <c r="S68" s="69"/>
       <c r="T68" s="69"/>
     </row>
     <row r="69" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="342"/>
+      <c r="B69" s="380"/>
       <c r="C69" s="128"/>
       <c r="D69" s="116"/>
       <c r="E69" s="116"/>
       <c r="F69" s="116"/>
       <c r="G69" s="116"/>
-      <c r="H69" s="343"/>
+      <c r="H69" s="381"/>
       <c r="I69" s="116"/>
       <c r="J69" s="116"/>
       <c r="K69" s="116"/>
       <c r="L69" s="116"/>
-      <c r="M69" s="343"/>
-      <c r="N69" s="345"/>
+      <c r="M69" s="381"/>
+      <c r="N69" s="383"/>
       <c r="P69" s="81"/>
       <c r="Q69" s="81"/>
       <c r="S69" s="69"/>
       <c r="T69" s="69"/>
     </row>
     <row r="70" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="342"/>
+      <c r="B70" s="380"/>
       <c r="C70" s="128"/>
       <c r="D70" s="116"/>
       <c r="E70" s="116"/>
       <c r="F70" s="116"/>
       <c r="G70" s="116"/>
-      <c r="H70" s="343"/>
+      <c r="H70" s="381"/>
       <c r="I70" s="116"/>
       <c r="J70" s="116"/>
       <c r="K70" s="116"/>
       <c r="L70" s="116"/>
-      <c r="M70" s="343"/>
-      <c r="N70" s="397"/>
+      <c r="M70" s="381"/>
+      <c r="N70" s="400"/>
       <c r="P70" s="81"/>
       <c r="Q70" s="81"/>
       <c r="S70" s="69"/>
       <c r="T70" s="69"/>
     </row>
     <row r="71" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="342"/>
+      <c r="B71" s="380"/>
       <c r="C71" s="128"/>
       <c r="D71" s="116"/>
       <c r="E71" s="116"/>
       <c r="F71" s="116"/>
       <c r="G71" s="116"/>
-      <c r="H71" s="343"/>
+      <c r="H71" s="381"/>
       <c r="I71" s="116"/>
       <c r="J71" s="116"/>
       <c r="K71" s="116"/>
       <c r="L71" s="116"/>
-      <c r="M71" s="343"/>
-      <c r="N71" s="345"/>
+      <c r="M71" s="381"/>
+      <c r="N71" s="383"/>
       <c r="P71" s="81"/>
       <c r="Q71" s="81"/>
       <c r="S71" s="69"/>
       <c r="T71" s="69"/>
     </row>
     <row r="72" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="342"/>
+      <c r="B72" s="380"/>
       <c r="C72" s="128"/>
       <c r="D72" s="116"/>
       <c r="E72" s="116"/>
       <c r="F72" s="116"/>
       <c r="G72" s="116"/>
-      <c r="H72" s="343"/>
+      <c r="H72" s="381"/>
       <c r="I72" s="116"/>
       <c r="J72" s="116"/>
       <c r="K72" s="116"/>
       <c r="L72" s="116"/>
-      <c r="M72" s="343"/>
-      <c r="N72" s="345"/>
+      <c r="M72" s="381"/>
+      <c r="N72" s="383"/>
       <c r="P72" s="81"/>
       <c r="Q72" s="81"/>
       <c r="S72" s="69"/>
       <c r="T72" s="69"/>
     </row>
     <row r="73" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="342"/>
+      <c r="B73" s="380"/>
       <c r="C73" s="128"/>
       <c r="D73" s="116"/>
       <c r="E73" s="116"/>
       <c r="F73" s="116"/>
       <c r="G73" s="116"/>
-      <c r="H73" s="343"/>
+      <c r="H73" s="381"/>
       <c r="I73" s="116"/>
       <c r="J73" s="116"/>
       <c r="K73" s="116"/>
       <c r="L73" s="116"/>
-      <c r="M73" s="343"/>
-      <c r="N73" s="345"/>
+      <c r="M73" s="381"/>
+      <c r="N73" s="383"/>
       <c r="P73" s="81"/>
       <c r="Q73" s="81"/>
       <c r="S73" s="69"/>
@@ -22706,24 +22706,56 @@
     <row r="140" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="H54:H57"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="M66:M69"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="M54:M57"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="M58:M61"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="M62:M65"/>
+    <mergeCell ref="N54:N57"/>
+    <mergeCell ref="N58:N61"/>
+    <mergeCell ref="N62:N65"/>
+    <mergeCell ref="N66:N69"/>
+    <mergeCell ref="N70:N73"/>
+    <mergeCell ref="U21:U24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="M21:M24"/>
+    <mergeCell ref="N21:N24"/>
+    <mergeCell ref="O21:O24"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="Q21:Q24"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="T21:T24"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="R21:R24"/>
+    <mergeCell ref="S21:S24"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="M50:M53"/>
+    <mergeCell ref="N42:N45"/>
+    <mergeCell ref="N46:N49"/>
+    <mergeCell ref="N50:N53"/>
+    <mergeCell ref="M42:M45"/>
+    <mergeCell ref="M46:M49"/>
     <mergeCell ref="U17:U20"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="R13:R16"/>
@@ -22740,56 +22772,24 @@
     <mergeCell ref="M13:M16"/>
     <mergeCell ref="N13:N16"/>
     <mergeCell ref="O13:O16"/>
-    <mergeCell ref="M50:M53"/>
-    <mergeCell ref="N42:N45"/>
-    <mergeCell ref="N46:N49"/>
-    <mergeCell ref="N50:N53"/>
-    <mergeCell ref="M42:M45"/>
-    <mergeCell ref="M46:M49"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="T21:T24"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="R21:R24"/>
-    <mergeCell ref="S21:S24"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="U21:U24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="M21:M24"/>
-    <mergeCell ref="N21:N24"/>
-    <mergeCell ref="O21:O24"/>
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="Q21:Q24"/>
-    <mergeCell ref="N54:N57"/>
-    <mergeCell ref="N58:N61"/>
-    <mergeCell ref="N62:N65"/>
-    <mergeCell ref="N66:N69"/>
-    <mergeCell ref="N70:N73"/>
-    <mergeCell ref="M66:M69"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="M70:M73"/>
-    <mergeCell ref="M54:M57"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="M58:M61"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="M62:M65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="H50:H53"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">

</xml_diff>

<commit_message>
Equipment & eq group - sanity test updated
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -1698,29 +1698,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1731,7 +1734,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1761,48 +1770,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3689,8 +3679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB39" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AM42" sqref="AM42"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -3739,15 +3729,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="248" t="s">
+      <c r="F1" s="269" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="248"/>
-      <c r="H1" s="248"/>
-      <c r="I1" s="248"/>
-      <c r="J1" s="248"/>
-      <c r="K1" s="248"/>
-      <c r="L1" s="248"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
+      <c r="I1" s="269"/>
+      <c r="J1" s="269"/>
+      <c r="K1" s="269"/>
+      <c r="L1" s="269"/>
       <c r="U1" s="20" t="s">
         <v>53</v>
       </c>
@@ -3796,22 +3786,22 @@
       <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="249" t="s">
+      <c r="D6" s="270" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="250"/>
-      <c r="F6" s="250"/>
-      <c r="G6" s="250"/>
-      <c r="H6" s="251"/>
+      <c r="E6" s="271"/>
+      <c r="F6" s="271"/>
+      <c r="G6" s="271"/>
+      <c r="H6" s="272"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="M6" s="249" t="s">
+      <c r="M6" s="270" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="250"/>
-      <c r="O6" s="250"/>
-      <c r="P6" s="250"/>
-      <c r="Q6" s="251"/>
+      <c r="N6" s="271"/>
+      <c r="O6" s="271"/>
+      <c r="P6" s="271"/>
+      <c r="Q6" s="272"/>
     </row>
     <row r="7" spans="1:48" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
@@ -3829,10 +3819,10 @@
       <c r="E7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="252" t="s">
+      <c r="F7" s="273" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="253"/>
+      <c r="G7" s="274"/>
       <c r="H7" s="22" t="s">
         <v>63</v>
       </c>
@@ -3855,10 +3845,10 @@
         <v>69</v>
       </c>
       <c r="O7" s="27"/>
-      <c r="P7" s="252" t="s">
+      <c r="P7" s="273" t="s">
         <v>70</v>
       </c>
-      <c r="Q7" s="253"/>
+      <c r="Q7" s="274"/>
       <c r="R7" s="28" t="s">
         <v>64</v>
       </c>
@@ -3926,7 +3916,7 @@
     </row>
     <row r="9" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37"/>
-      <c r="B9" s="254"/>
+      <c r="B9" s="255"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -3937,15 +3927,15 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="40"/>
-      <c r="M9" s="246"/>
-      <c r="N9" s="258"/>
-      <c r="O9" s="246"/>
-      <c r="P9" s="246"/>
-      <c r="Q9" s="246"/>
-      <c r="R9" s="246"/>
-      <c r="S9" s="246"/>
-      <c r="T9" s="261"/>
-      <c r="U9" s="246"/>
+      <c r="M9" s="258"/>
+      <c r="N9" s="261"/>
+      <c r="O9" s="258"/>
+      <c r="P9" s="258"/>
+      <c r="Q9" s="258"/>
+      <c r="R9" s="258"/>
+      <c r="S9" s="258"/>
+      <c r="T9" s="264"/>
+      <c r="U9" s="258"/>
       <c r="V9" s="39"/>
       <c r="W9" s="34"/>
       <c r="X9" s="34"/>
@@ -3955,7 +3945,7 @@
     </row>
     <row r="10" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="38"/>
-      <c r="B10" s="255"/>
+      <c r="B10" s="256"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
@@ -3966,15 +3956,15 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="40"/>
-      <c r="M10" s="257"/>
-      <c r="N10" s="259"/>
-      <c r="O10" s="257"/>
-      <c r="P10" s="257"/>
-      <c r="Q10" s="257"/>
-      <c r="R10" s="257"/>
-      <c r="S10" s="257"/>
-      <c r="T10" s="262"/>
-      <c r="U10" s="257"/>
+      <c r="M10" s="259"/>
+      <c r="N10" s="262"/>
+      <c r="O10" s="259"/>
+      <c r="P10" s="259"/>
+      <c r="Q10" s="259"/>
+      <c r="R10" s="259"/>
+      <c r="S10" s="259"/>
+      <c r="T10" s="265"/>
+      <c r="U10" s="259"/>
       <c r="V10" s="39"/>
       <c r="W10" s="34"/>
       <c r="X10" s="34"/>
@@ -3982,8 +3972,8 @@
       <c r="AK10" s="44"/>
     </row>
     <row r="11" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="246"/>
-      <c r="B11" s="255"/>
+      <c r="A11" s="258"/>
+      <c r="B11" s="256"/>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
@@ -3994,15 +3984,15 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="40"/>
-      <c r="M11" s="257"/>
-      <c r="N11" s="259"/>
-      <c r="O11" s="257"/>
-      <c r="P11" s="257"/>
-      <c r="Q11" s="257"/>
-      <c r="R11" s="257"/>
-      <c r="S11" s="257"/>
-      <c r="T11" s="262"/>
-      <c r="U11" s="257"/>
+      <c r="M11" s="259"/>
+      <c r="N11" s="262"/>
+      <c r="O11" s="259"/>
+      <c r="P11" s="259"/>
+      <c r="Q11" s="259"/>
+      <c r="R11" s="259"/>
+      <c r="S11" s="259"/>
+      <c r="T11" s="265"/>
+      <c r="U11" s="259"/>
       <c r="V11" s="39"/>
       <c r="W11" s="34"/>
       <c r="X11" s="34"/>
@@ -4012,8 +4002,8 @@
       <c r="AV11" s="54"/>
     </row>
     <row r="12" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="247"/>
-      <c r="B12" s="256"/>
+      <c r="A12" s="260"/>
+      <c r="B12" s="257"/>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
@@ -4024,15 +4014,15 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="40"/>
-      <c r="M12" s="247"/>
-      <c r="N12" s="260"/>
-      <c r="O12" s="247"/>
-      <c r="P12" s="247"/>
-      <c r="Q12" s="247"/>
-      <c r="R12" s="247"/>
-      <c r="S12" s="247"/>
-      <c r="T12" s="263"/>
-      <c r="U12" s="247"/>
+      <c r="M12" s="260"/>
+      <c r="N12" s="263"/>
+      <c r="O12" s="260"/>
+      <c r="P12" s="260"/>
+      <c r="Q12" s="260"/>
+      <c r="R12" s="260"/>
+      <c r="S12" s="260"/>
+      <c r="T12" s="266"/>
+      <c r="U12" s="260"/>
       <c r="V12" s="39"/>
       <c r="W12" s="34"/>
       <c r="X12" s="34"/>
@@ -4041,7 +4031,7 @@
     </row>
     <row r="13" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="41"/>
-      <c r="B13" s="254"/>
+      <c r="B13" s="255"/>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -4052,15 +4042,15 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
       <c r="L13" s="40"/>
-      <c r="M13" s="246"/>
-      <c r="N13" s="258"/>
-      <c r="O13" s="246"/>
-      <c r="P13" s="246"/>
-      <c r="Q13" s="246"/>
-      <c r="R13" s="246"/>
-      <c r="S13" s="246"/>
-      <c r="T13" s="261"/>
-      <c r="U13" s="246"/>
+      <c r="M13" s="258"/>
+      <c r="N13" s="261"/>
+      <c r="O13" s="258"/>
+      <c r="P13" s="258"/>
+      <c r="Q13" s="258"/>
+      <c r="R13" s="258"/>
+      <c r="S13" s="258"/>
+      <c r="T13" s="264"/>
+      <c r="U13" s="258"/>
       <c r="V13" s="39"/>
       <c r="W13" s="34"/>
       <c r="X13" s="34"/>
@@ -4069,7 +4059,7 @@
     </row>
     <row r="14" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="42"/>
-      <c r="B14" s="255"/>
+      <c r="B14" s="256"/>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
@@ -4080,15 +4070,15 @@
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="40"/>
-      <c r="M14" s="257"/>
-      <c r="N14" s="259"/>
-      <c r="O14" s="257"/>
-      <c r="P14" s="257"/>
-      <c r="Q14" s="257"/>
-      <c r="R14" s="257"/>
-      <c r="S14" s="257"/>
-      <c r="T14" s="262"/>
-      <c r="U14" s="257"/>
+      <c r="M14" s="259"/>
+      <c r="N14" s="262"/>
+      <c r="O14" s="259"/>
+      <c r="P14" s="259"/>
+      <c r="Q14" s="259"/>
+      <c r="R14" s="259"/>
+      <c r="S14" s="259"/>
+      <c r="T14" s="265"/>
+      <c r="U14" s="259"/>
       <c r="V14" s="39"/>
       <c r="W14" s="34"/>
       <c r="X14" s="34"/>
@@ -4096,8 +4086,8 @@
       <c r="AU14" s="59"/>
     </row>
     <row r="15" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="264"/>
-      <c r="B15" s="255"/>
+      <c r="A15" s="267"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
@@ -4108,15 +4098,15 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="40"/>
-      <c r="M15" s="257"/>
-      <c r="N15" s="259"/>
-      <c r="O15" s="257"/>
-      <c r="P15" s="257"/>
-      <c r="Q15" s="257"/>
-      <c r="R15" s="257"/>
-      <c r="S15" s="257"/>
-      <c r="T15" s="262"/>
-      <c r="U15" s="257"/>
+      <c r="M15" s="259"/>
+      <c r="N15" s="262"/>
+      <c r="O15" s="259"/>
+      <c r="P15" s="259"/>
+      <c r="Q15" s="259"/>
+      <c r="R15" s="259"/>
+      <c r="S15" s="259"/>
+      <c r="T15" s="265"/>
+      <c r="U15" s="259"/>
       <c r="V15" s="39"/>
       <c r="W15" s="34"/>
       <c r="X15" s="34"/>
@@ -4124,8 +4114,8 @@
       <c r="AU15" s="44"/>
     </row>
     <row r="16" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="265"/>
-      <c r="B16" s="256"/>
+      <c r="A16" s="268"/>
+      <c r="B16" s="257"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
@@ -4136,15 +4126,15 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="40"/>
-      <c r="M16" s="247"/>
-      <c r="N16" s="260"/>
-      <c r="O16" s="247"/>
-      <c r="P16" s="247"/>
-      <c r="Q16" s="247"/>
-      <c r="R16" s="247"/>
-      <c r="S16" s="247"/>
-      <c r="T16" s="263"/>
-      <c r="U16" s="247"/>
+      <c r="M16" s="260"/>
+      <c r="N16" s="263"/>
+      <c r="O16" s="260"/>
+      <c r="P16" s="260"/>
+      <c r="Q16" s="260"/>
+      <c r="R16" s="260"/>
+      <c r="S16" s="260"/>
+      <c r="T16" s="266"/>
+      <c r="U16" s="260"/>
       <c r="V16" s="39"/>
       <c r="W16" s="34"/>
       <c r="X16" s="34"/>
@@ -4153,7 +4143,7 @@
     </row>
     <row r="17" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="37"/>
-      <c r="B17" s="254"/>
+      <c r="B17" s="255"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
@@ -4164,15 +4154,15 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="40"/>
-      <c r="M17" s="246"/>
-      <c r="N17" s="258"/>
-      <c r="O17" s="246"/>
-      <c r="P17" s="246"/>
-      <c r="Q17" s="246"/>
-      <c r="R17" s="246"/>
-      <c r="S17" s="246"/>
-      <c r="T17" s="261"/>
-      <c r="U17" s="246"/>
+      <c r="M17" s="258"/>
+      <c r="N17" s="261"/>
+      <c r="O17" s="258"/>
+      <c r="P17" s="258"/>
+      <c r="Q17" s="258"/>
+      <c r="R17" s="258"/>
+      <c r="S17" s="258"/>
+      <c r="T17" s="264"/>
+      <c r="U17" s="258"/>
       <c r="V17" s="39"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
@@ -4181,7 +4171,7 @@
     </row>
     <row r="18" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
-      <c r="B18" s="255"/>
+      <c r="B18" s="256"/>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
       <c r="E18" s="38"/>
@@ -4192,22 +4182,22 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="40"/>
-      <c r="M18" s="257"/>
-      <c r="N18" s="259"/>
-      <c r="O18" s="257"/>
-      <c r="P18" s="257"/>
-      <c r="Q18" s="257"/>
-      <c r="R18" s="257"/>
-      <c r="S18" s="257"/>
-      <c r="T18" s="262"/>
-      <c r="U18" s="257"/>
+      <c r="M18" s="259"/>
+      <c r="N18" s="262"/>
+      <c r="O18" s="259"/>
+      <c r="P18" s="259"/>
+      <c r="Q18" s="259"/>
+      <c r="R18" s="259"/>
+      <c r="S18" s="259"/>
+      <c r="T18" s="265"/>
+      <c r="U18" s="259"/>
       <c r="V18" s="39"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
     </row>
     <row r="19" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="246"/>
-      <c r="B19" s="255"/>
+      <c r="A19" s="258"/>
+      <c r="B19" s="256"/>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
@@ -4218,22 +4208,22 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="40"/>
-      <c r="M19" s="257"/>
-      <c r="N19" s="259"/>
-      <c r="O19" s="257"/>
-      <c r="P19" s="257"/>
-      <c r="Q19" s="257"/>
-      <c r="R19" s="257"/>
-      <c r="S19" s="257"/>
-      <c r="T19" s="262"/>
-      <c r="U19" s="257"/>
+      <c r="M19" s="259"/>
+      <c r="N19" s="262"/>
+      <c r="O19" s="259"/>
+      <c r="P19" s="259"/>
+      <c r="Q19" s="259"/>
+      <c r="R19" s="259"/>
+      <c r="S19" s="259"/>
+      <c r="T19" s="265"/>
+      <c r="U19" s="259"/>
       <c r="V19" s="39"/>
       <c r="W19" s="34"/>
       <c r="X19" s="34"/>
     </row>
     <row r="20" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="247"/>
-      <c r="B20" s="256"/>
+      <c r="A20" s="260"/>
+      <c r="B20" s="257"/>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
@@ -4244,22 +4234,22 @@
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
       <c r="L20" s="40"/>
-      <c r="M20" s="247"/>
-      <c r="N20" s="260"/>
-      <c r="O20" s="247"/>
-      <c r="P20" s="247"/>
-      <c r="Q20" s="247"/>
-      <c r="R20" s="247"/>
-      <c r="S20" s="247"/>
-      <c r="T20" s="263"/>
-      <c r="U20" s="247"/>
+      <c r="M20" s="260"/>
+      <c r="N20" s="263"/>
+      <c r="O20" s="260"/>
+      <c r="P20" s="260"/>
+      <c r="Q20" s="260"/>
+      <c r="R20" s="260"/>
+      <c r="S20" s="260"/>
+      <c r="T20" s="266"/>
+      <c r="U20" s="260"/>
       <c r="V20" s="39"/>
       <c r="W20" s="34"/>
       <c r="X20" s="34"/>
     </row>
     <row r="21" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="37"/>
-      <c r="B21" s="254"/>
+      <c r="B21" s="255"/>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
@@ -4270,22 +4260,22 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="40"/>
-      <c r="M21" s="246"/>
-      <c r="N21" s="258"/>
-      <c r="O21" s="246"/>
-      <c r="P21" s="246"/>
-      <c r="Q21" s="246"/>
-      <c r="R21" s="246"/>
-      <c r="S21" s="246"/>
-      <c r="T21" s="261"/>
-      <c r="U21" s="246"/>
+      <c r="M21" s="258"/>
+      <c r="N21" s="261"/>
+      <c r="O21" s="258"/>
+      <c r="P21" s="258"/>
+      <c r="Q21" s="258"/>
+      <c r="R21" s="258"/>
+      <c r="S21" s="258"/>
+      <c r="T21" s="264"/>
+      <c r="U21" s="258"/>
       <c r="V21" s="39"/>
       <c r="W21" s="34"/>
       <c r="X21" s="34"/>
     </row>
     <row r="22" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="38"/>
-      <c r="B22" s="255"/>
+      <c r="B22" s="256"/>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
@@ -4296,22 +4286,22 @@
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
       <c r="L22" s="40"/>
-      <c r="M22" s="257"/>
-      <c r="N22" s="259"/>
-      <c r="O22" s="257"/>
-      <c r="P22" s="257"/>
-      <c r="Q22" s="257"/>
-      <c r="R22" s="257"/>
-      <c r="S22" s="257"/>
-      <c r="T22" s="262"/>
-      <c r="U22" s="257"/>
+      <c r="M22" s="259"/>
+      <c r="N22" s="262"/>
+      <c r="O22" s="259"/>
+      <c r="P22" s="259"/>
+      <c r="Q22" s="259"/>
+      <c r="R22" s="259"/>
+      <c r="S22" s="259"/>
+      <c r="T22" s="265"/>
+      <c r="U22" s="259"/>
       <c r="V22" s="39"/>
       <c r="W22" s="34"/>
       <c r="X22" s="34"/>
     </row>
     <row r="23" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="273"/>
-      <c r="B23" s="255"/>
+      <c r="A23" s="253"/>
+      <c r="B23" s="256"/>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
@@ -4322,22 +4312,22 @@
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
       <c r="L23" s="40"/>
-      <c r="M23" s="257"/>
-      <c r="N23" s="259"/>
-      <c r="O23" s="257"/>
-      <c r="P23" s="257"/>
-      <c r="Q23" s="257"/>
-      <c r="R23" s="257"/>
-      <c r="S23" s="257"/>
-      <c r="T23" s="262"/>
-      <c r="U23" s="257"/>
+      <c r="M23" s="259"/>
+      <c r="N23" s="262"/>
+      <c r="O23" s="259"/>
+      <c r="P23" s="259"/>
+      <c r="Q23" s="259"/>
+      <c r="R23" s="259"/>
+      <c r="S23" s="259"/>
+      <c r="T23" s="265"/>
+      <c r="U23" s="259"/>
       <c r="V23" s="39"/>
       <c r="W23" s="34"/>
       <c r="X23" s="34"/>
     </row>
     <row r="24" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="274"/>
-      <c r="B24" s="256"/>
+      <c r="A24" s="254"/>
+      <c r="B24" s="257"/>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
@@ -4348,15 +4338,15 @@
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
       <c r="L24" s="40"/>
-      <c r="M24" s="247"/>
-      <c r="N24" s="260"/>
-      <c r="O24" s="247"/>
-      <c r="P24" s="247"/>
-      <c r="Q24" s="247"/>
-      <c r="R24" s="247"/>
-      <c r="S24" s="247"/>
-      <c r="T24" s="263"/>
-      <c r="U24" s="247"/>
+      <c r="M24" s="260"/>
+      <c r="N24" s="263"/>
+      <c r="O24" s="260"/>
+      <c r="P24" s="260"/>
+      <c r="Q24" s="260"/>
+      <c r="R24" s="260"/>
+      <c r="S24" s="260"/>
+      <c r="T24" s="266"/>
+      <c r="U24" s="260"/>
       <c r="V24" s="39"/>
       <c r="W24" s="34"/>
       <c r="X24" s="34"/>
@@ -4676,33 +4666,33 @@
       </c>
       <c r="D40" s="77"/>
       <c r="E40" s="78"/>
-      <c r="F40" s="267" t="s">
+      <c r="F40" s="247" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="268"/>
-      <c r="H40" s="268"/>
-      <c r="I40" s="269"/>
-      <c r="J40" s="270" t="s">
+      <c r="G40" s="248"/>
+      <c r="H40" s="248"/>
+      <c r="I40" s="249"/>
+      <c r="J40" s="250" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="271"/>
-      <c r="L40" s="271"/>
-      <c r="M40" s="272"/>
+      <c r="K40" s="251"/>
+      <c r="L40" s="251"/>
+      <c r="M40" s="252"/>
       <c r="N40" s="79" t="s">
         <v>46</v>
       </c>
       <c r="P40" s="125"/>
-      <c r="Q40" s="266" t="s">
+      <c r="Q40" s="246" t="s">
         <v>116</v>
       </c>
-      <c r="R40" s="266"/>
-      <c r="S40" s="266"/>
-      <c r="T40" s="266"/>
-      <c r="U40" s="266"/>
-      <c r="V40" s="266"/>
-      <c r="W40" s="266"/>
-      <c r="X40" s="266"/>
-      <c r="Y40" s="266"/>
+      <c r="R40" s="246"/>
+      <c r="S40" s="246"/>
+      <c r="T40" s="246"/>
+      <c r="U40" s="246"/>
+      <c r="V40" s="246"/>
+      <c r="W40" s="246"/>
+      <c r="X40" s="246"/>
+      <c r="Y40" s="246"/>
       <c r="Z40" s="44"/>
       <c r="AA40" s="44"/>
       <c r="AB40" s="44"/>
@@ -12962,6 +12952,44 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="T13:T16"/>
+    <mergeCell ref="U13:U16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="U17:U20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
     <mergeCell ref="Q40:Y40"/>
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="J40:M40"/>
@@ -12976,47 +13004,9 @@
     <mergeCell ref="R21:R24"/>
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
-    <mergeCell ref="U17:U20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="S13:S16"/>
-    <mergeCell ref="T13:T16"/>
-    <mergeCell ref="U13:U16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="Q9:Q12"/>
   </mergeCells>
   <conditionalFormatting sqref="AM1:AM1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9 N13 N17 N21">

</xml_diff>

<commit_message>
Equipment - 1st page negative testcase and evaluate calculation done
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -499,9 +499,6 @@
     <t>Max Length</t>
   </si>
   <si>
-    <t>Asser No</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -575,6 +572,12 @@
   </si>
   <si>
     <t>Minimum Batch size cannot be empty</t>
+  </si>
+  <si>
+    <t>Assert No</t>
+  </si>
+  <si>
+    <t>Choose Cleaning Process Type</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1785,32 +1788,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1821,7 +1828,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1851,32 +1864,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3559,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,10 +3636,10 @@
       <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="243" t="s">
+      <c r="B7" s="244" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="243" t="s">
+      <c r="C7" s="244" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -3652,8 +3656,8 @@
       <c r="A8" s="12">
         <v>2</v>
       </c>
-      <c r="B8" s="243"/>
-      <c r="C8" s="243"/>
+      <c r="B8" s="244"/>
+      <c r="C8" s="244"/>
       <c r="D8" s="12" t="s">
         <v>49</v>
       </c>
@@ -3670,8 +3674,8 @@
       <c r="A9" s="12">
         <v>3</v>
       </c>
-      <c r="B9" s="243"/>
-      <c r="C9" s="243"/>
+      <c r="B9" s="244"/>
+      <c r="C9" s="244"/>
       <c r="D9" s="12" t="s">
         <v>50</v>
       </c>
@@ -3688,8 +3692,8 @@
       <c r="A10" s="12">
         <v>4</v>
       </c>
-      <c r="B10" s="243"/>
-      <c r="C10" s="243"/>
+      <c r="B10" s="244"/>
+      <c r="C10" s="244"/>
       <c r="D10" s="12" t="s">
         <v>51</v>
       </c>
@@ -3697,7 +3701,7 @@
         <v>134</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="241"/>
@@ -3706,8 +3710,8 @@
       <c r="A11" s="12">
         <v>5</v>
       </c>
-      <c r="B11" s="243"/>
-      <c r="C11" s="243"/>
+      <c r="B11" s="244"/>
+      <c r="C11" s="244"/>
       <c r="D11" s="12" t="s">
         <v>133</v>
       </c>
@@ -3743,8 +3747,12 @@
       <c r="D13" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="12">
+        <v>75</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
@@ -3754,13 +3762,17 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="12">
+        <v>75</v>
+      </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
@@ -3770,11 +3782,15 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="12">
+        <v>75</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
     </row>
@@ -3791,7 +3807,7 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -3803,11 +3819,11 @@
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
@@ -3835,10 +3851,10 @@
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -3854,7 +3870,7 @@
         <v>133</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F20" s="12">
         <v>123</v>
@@ -3869,10 +3885,10 @@
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="242" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F21" s="12">
         <v>1.23</v>
@@ -3886,13 +3902,17 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="12">
+        <v>75</v>
+      </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
@@ -3902,10 +3922,10 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -3919,7 +3939,7 @@
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -3932,7 +3952,7 @@
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -3946,7 +3966,7 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="242" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>48</v>
@@ -3963,7 +3983,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -3991,7 +4011,7 @@
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -4019,7 +4039,7 @@
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="242" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -4032,7 +4052,7 @@
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -4046,14 +4066,14 @@
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
@@ -4065,11 +4085,11 @@
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -4097,10 +4117,10 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -4116,7 +4136,7 @@
         <v>133</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F37" s="12">
         <v>123</v>
@@ -4131,10 +4151,10 @@
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="242" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F38" s="12">
         <v>1.23</v>
@@ -4148,13 +4168,17 @@
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="E39" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="12">
+        <v>75</v>
+      </c>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
     </row>
@@ -4164,7 +4188,7 @@
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
@@ -4178,13 +4202,15 @@
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
+      <c r="F41" t="s">
+        <v>168</v>
+      </c>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
     </row>
@@ -4194,10 +4220,10 @@
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -4210,13 +4236,17 @@
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="E43" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="12">
+        <v>75</v>
+      </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
     </row>
@@ -4226,7 +4256,7 @@
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>141</v>
@@ -4320,15 +4350,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="246" t="s">
+      <c r="F1" s="268" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
-      <c r="K1" s="246"/>
-      <c r="L1" s="246"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="268"/>
       <c r="U1" s="15" t="s">
         <v>53</v>
       </c>
@@ -4377,22 +4407,22 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="247" t="s">
+      <c r="D6" s="269" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="248"/>
-      <c r="F6" s="248"/>
-      <c r="G6" s="248"/>
-      <c r="H6" s="249"/>
+      <c r="E6" s="270"/>
+      <c r="F6" s="270"/>
+      <c r="G6" s="270"/>
+      <c r="H6" s="271"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-      <c r="M6" s="247" t="s">
+      <c r="M6" s="269" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="248"/>
-      <c r="O6" s="248"/>
-      <c r="P6" s="248"/>
-      <c r="Q6" s="249"/>
+      <c r="N6" s="270"/>
+      <c r="O6" s="270"/>
+      <c r="P6" s="270"/>
+      <c r="Q6" s="271"/>
     </row>
     <row r="7" spans="1:48" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
@@ -4410,10 +4440,10 @@
       <c r="E7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="250" t="s">
+      <c r="F7" s="272" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="251"/>
+      <c r="G7" s="273"/>
       <c r="H7" s="17" t="s">
         <v>63</v>
       </c>
@@ -4436,10 +4466,10 @@
         <v>69</v>
       </c>
       <c r="O7" s="22"/>
-      <c r="P7" s="250" t="s">
+      <c r="P7" s="272" t="s">
         <v>70</v>
       </c>
-      <c r="Q7" s="251"/>
+      <c r="Q7" s="273"/>
       <c r="R7" s="23" t="s">
         <v>64</v>
       </c>
@@ -4507,7 +4537,7 @@
     </row>
     <row r="9" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
-      <c r="B9" s="252"/>
+      <c r="B9" s="254"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
@@ -4518,15 +4548,15 @@
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="244"/>
-      <c r="N9" s="256"/>
-      <c r="O9" s="244"/>
-      <c r="P9" s="244"/>
-      <c r="Q9" s="244"/>
-      <c r="R9" s="244"/>
-      <c r="S9" s="244"/>
-      <c r="T9" s="259"/>
-      <c r="U9" s="244"/>
+      <c r="M9" s="257"/>
+      <c r="N9" s="260"/>
+      <c r="O9" s="257"/>
+      <c r="P9" s="257"/>
+      <c r="Q9" s="257"/>
+      <c r="R9" s="257"/>
+      <c r="S9" s="257"/>
+      <c r="T9" s="263"/>
+      <c r="U9" s="257"/>
       <c r="V9" s="34"/>
       <c r="W9" s="29"/>
       <c r="X9" s="29"/>
@@ -4536,7 +4566,7 @@
     </row>
     <row r="10" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33"/>
-      <c r="B10" s="253"/>
+      <c r="B10" s="255"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
@@ -4547,15 +4577,15 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="35"/>
-      <c r="M10" s="255"/>
-      <c r="N10" s="257"/>
-      <c r="O10" s="255"/>
-      <c r="P10" s="255"/>
-      <c r="Q10" s="255"/>
-      <c r="R10" s="255"/>
-      <c r="S10" s="255"/>
-      <c r="T10" s="260"/>
-      <c r="U10" s="255"/>
+      <c r="M10" s="258"/>
+      <c r="N10" s="261"/>
+      <c r="O10" s="258"/>
+      <c r="P10" s="258"/>
+      <c r="Q10" s="258"/>
+      <c r="R10" s="258"/>
+      <c r="S10" s="258"/>
+      <c r="T10" s="264"/>
+      <c r="U10" s="258"/>
       <c r="V10" s="34"/>
       <c r="W10" s="29"/>
       <c r="X10" s="29"/>
@@ -4563,8 +4593,8 @@
       <c r="AK10" s="39"/>
     </row>
     <row r="11" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="244"/>
-      <c r="B11" s="253"/>
+      <c r="A11" s="257"/>
+      <c r="B11" s="255"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -4575,15 +4605,15 @@
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
       <c r="L11" s="35"/>
-      <c r="M11" s="255"/>
-      <c r="N11" s="257"/>
-      <c r="O11" s="255"/>
-      <c r="P11" s="255"/>
-      <c r="Q11" s="255"/>
-      <c r="R11" s="255"/>
-      <c r="S11" s="255"/>
-      <c r="T11" s="260"/>
-      <c r="U11" s="255"/>
+      <c r="M11" s="258"/>
+      <c r="N11" s="261"/>
+      <c r="O11" s="258"/>
+      <c r="P11" s="258"/>
+      <c r="Q11" s="258"/>
+      <c r="R11" s="258"/>
+      <c r="S11" s="258"/>
+      <c r="T11" s="264"/>
+      <c r="U11" s="258"/>
       <c r="V11" s="34"/>
       <c r="W11" s="29"/>
       <c r="X11" s="29"/>
@@ -4593,8 +4623,8 @@
       <c r="AV11" s="49"/>
     </row>
     <row r="12" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="245"/>
-      <c r="B12" s="254"/>
+      <c r="A12" s="259"/>
+      <c r="B12" s="256"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
@@ -4605,15 +4635,15 @@
       <c r="J12" s="29"/>
       <c r="K12" s="29"/>
       <c r="L12" s="35"/>
-      <c r="M12" s="245"/>
-      <c r="N12" s="258"/>
-      <c r="O12" s="245"/>
-      <c r="P12" s="245"/>
-      <c r="Q12" s="245"/>
-      <c r="R12" s="245"/>
-      <c r="S12" s="245"/>
-      <c r="T12" s="261"/>
-      <c r="U12" s="245"/>
+      <c r="M12" s="259"/>
+      <c r="N12" s="262"/>
+      <c r="O12" s="259"/>
+      <c r="P12" s="259"/>
+      <c r="Q12" s="259"/>
+      <c r="R12" s="259"/>
+      <c r="S12" s="259"/>
+      <c r="T12" s="265"/>
+      <c r="U12" s="259"/>
       <c r="V12" s="34"/>
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
@@ -4622,7 +4652,7 @@
     </row>
     <row r="13" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
-      <c r="B13" s="252"/>
+      <c r="B13" s="254"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
@@ -4633,15 +4663,15 @@
       <c r="J13" s="29"/>
       <c r="K13" s="29"/>
       <c r="L13" s="35"/>
-      <c r="M13" s="244"/>
-      <c r="N13" s="256"/>
-      <c r="O13" s="244"/>
-      <c r="P13" s="244"/>
-      <c r="Q13" s="244"/>
-      <c r="R13" s="244"/>
-      <c r="S13" s="244"/>
-      <c r="T13" s="259"/>
-      <c r="U13" s="244"/>
+      <c r="M13" s="257"/>
+      <c r="N13" s="260"/>
+      <c r="O13" s="257"/>
+      <c r="P13" s="257"/>
+      <c r="Q13" s="257"/>
+      <c r="R13" s="257"/>
+      <c r="S13" s="257"/>
+      <c r="T13" s="263"/>
+      <c r="U13" s="257"/>
       <c r="V13" s="34"/>
       <c r="W13" s="29"/>
       <c r="X13" s="29"/>
@@ -4650,7 +4680,7 @@
     </row>
     <row r="14" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37"/>
-      <c r="B14" s="253"/>
+      <c r="B14" s="255"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
@@ -4661,15 +4691,15 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="255"/>
-      <c r="N14" s="257"/>
-      <c r="O14" s="255"/>
-      <c r="P14" s="255"/>
-      <c r="Q14" s="255"/>
-      <c r="R14" s="255"/>
-      <c r="S14" s="255"/>
-      <c r="T14" s="260"/>
-      <c r="U14" s="255"/>
+      <c r="M14" s="258"/>
+      <c r="N14" s="261"/>
+      <c r="O14" s="258"/>
+      <c r="P14" s="258"/>
+      <c r="Q14" s="258"/>
+      <c r="R14" s="258"/>
+      <c r="S14" s="258"/>
+      <c r="T14" s="264"/>
+      <c r="U14" s="258"/>
       <c r="V14" s="34"/>
       <c r="W14" s="29"/>
       <c r="X14" s="29"/>
@@ -4677,8 +4707,8 @@
       <c r="AU14" s="54"/>
     </row>
     <row r="15" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="262"/>
-      <c r="B15" s="253"/>
+      <c r="A15" s="266"/>
+      <c r="B15" s="255"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -4689,15 +4719,15 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="35"/>
-      <c r="M15" s="255"/>
-      <c r="N15" s="257"/>
-      <c r="O15" s="255"/>
-      <c r="P15" s="255"/>
-      <c r="Q15" s="255"/>
-      <c r="R15" s="255"/>
-      <c r="S15" s="255"/>
-      <c r="T15" s="260"/>
-      <c r="U15" s="255"/>
+      <c r="M15" s="258"/>
+      <c r="N15" s="261"/>
+      <c r="O15" s="258"/>
+      <c r="P15" s="258"/>
+      <c r="Q15" s="258"/>
+      <c r="R15" s="258"/>
+      <c r="S15" s="258"/>
+      <c r="T15" s="264"/>
+      <c r="U15" s="258"/>
       <c r="V15" s="34"/>
       <c r="W15" s="29"/>
       <c r="X15" s="29"/>
@@ -4705,8 +4735,8 @@
       <c r="AU15" s="39"/>
     </row>
     <row r="16" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="263"/>
-      <c r="B16" s="254"/>
+      <c r="A16" s="267"/>
+      <c r="B16" s="256"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -4717,15 +4747,15 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
       <c r="L16" s="35"/>
-      <c r="M16" s="245"/>
-      <c r="N16" s="258"/>
-      <c r="O16" s="245"/>
-      <c r="P16" s="245"/>
-      <c r="Q16" s="245"/>
-      <c r="R16" s="245"/>
-      <c r="S16" s="245"/>
-      <c r="T16" s="261"/>
-      <c r="U16" s="245"/>
+      <c r="M16" s="259"/>
+      <c r="N16" s="262"/>
+      <c r="O16" s="259"/>
+      <c r="P16" s="259"/>
+      <c r="Q16" s="259"/>
+      <c r="R16" s="259"/>
+      <c r="S16" s="259"/>
+      <c r="T16" s="265"/>
+      <c r="U16" s="259"/>
       <c r="V16" s="34"/>
       <c r="W16" s="29"/>
       <c r="X16" s="29"/>
@@ -4734,7 +4764,7 @@
     </row>
     <row r="17" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32"/>
-      <c r="B17" s="252"/>
+      <c r="B17" s="254"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
@@ -4745,15 +4775,15 @@
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
       <c r="L17" s="35"/>
-      <c r="M17" s="244"/>
-      <c r="N17" s="256"/>
-      <c r="O17" s="244"/>
-      <c r="P17" s="244"/>
-      <c r="Q17" s="244"/>
-      <c r="R17" s="244"/>
-      <c r="S17" s="244"/>
-      <c r="T17" s="259"/>
-      <c r="U17" s="244"/>
+      <c r="M17" s="257"/>
+      <c r="N17" s="260"/>
+      <c r="O17" s="257"/>
+      <c r="P17" s="257"/>
+      <c r="Q17" s="257"/>
+      <c r="R17" s="257"/>
+      <c r="S17" s="257"/>
+      <c r="T17" s="263"/>
+      <c r="U17" s="257"/>
       <c r="V17" s="34"/>
       <c r="W17" s="29"/>
       <c r="X17" s="29"/>
@@ -4762,7 +4792,7 @@
     </row>
     <row r="18" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33"/>
-      <c r="B18" s="253"/>
+      <c r="B18" s="255"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -4773,22 +4803,22 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="35"/>
-      <c r="M18" s="255"/>
-      <c r="N18" s="257"/>
-      <c r="O18" s="255"/>
-      <c r="P18" s="255"/>
-      <c r="Q18" s="255"/>
-      <c r="R18" s="255"/>
-      <c r="S18" s="255"/>
-      <c r="T18" s="260"/>
-      <c r="U18" s="255"/>
+      <c r="M18" s="258"/>
+      <c r="N18" s="261"/>
+      <c r="O18" s="258"/>
+      <c r="P18" s="258"/>
+      <c r="Q18" s="258"/>
+      <c r="R18" s="258"/>
+      <c r="S18" s="258"/>
+      <c r="T18" s="264"/>
+      <c r="U18" s="258"/>
       <c r="V18" s="34"/>
       <c r="W18" s="29"/>
       <c r="X18" s="29"/>
     </row>
     <row r="19" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="244"/>
-      <c r="B19" s="253"/>
+      <c r="A19" s="257"/>
+      <c r="B19" s="255"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
@@ -4799,22 +4829,22 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="35"/>
-      <c r="M19" s="255"/>
-      <c r="N19" s="257"/>
-      <c r="O19" s="255"/>
-      <c r="P19" s="255"/>
-      <c r="Q19" s="255"/>
-      <c r="R19" s="255"/>
-      <c r="S19" s="255"/>
-      <c r="T19" s="260"/>
-      <c r="U19" s="255"/>
+      <c r="M19" s="258"/>
+      <c r="N19" s="261"/>
+      <c r="O19" s="258"/>
+      <c r="P19" s="258"/>
+      <c r="Q19" s="258"/>
+      <c r="R19" s="258"/>
+      <c r="S19" s="258"/>
+      <c r="T19" s="264"/>
+      <c r="U19" s="258"/>
       <c r="V19" s="34"/>
       <c r="W19" s="29"/>
       <c r="X19" s="29"/>
     </row>
     <row r="20" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="245"/>
-      <c r="B20" s="254"/>
+      <c r="A20" s="259"/>
+      <c r="B20" s="256"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
@@ -4825,22 +4855,22 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="35"/>
-      <c r="M20" s="245"/>
-      <c r="N20" s="258"/>
-      <c r="O20" s="245"/>
-      <c r="P20" s="245"/>
-      <c r="Q20" s="245"/>
-      <c r="R20" s="245"/>
-      <c r="S20" s="245"/>
-      <c r="T20" s="261"/>
-      <c r="U20" s="245"/>
+      <c r="M20" s="259"/>
+      <c r="N20" s="262"/>
+      <c r="O20" s="259"/>
+      <c r="P20" s="259"/>
+      <c r="Q20" s="259"/>
+      <c r="R20" s="259"/>
+      <c r="S20" s="259"/>
+      <c r="T20" s="265"/>
+      <c r="U20" s="259"/>
       <c r="V20" s="34"/>
       <c r="W20" s="29"/>
       <c r="X20" s="29"/>
     </row>
     <row r="21" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32"/>
-      <c r="B21" s="252"/>
+      <c r="B21" s="254"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
@@ -4851,22 +4881,22 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="35"/>
-      <c r="M21" s="244"/>
-      <c r="N21" s="256"/>
-      <c r="O21" s="244"/>
-      <c r="P21" s="244"/>
-      <c r="Q21" s="244"/>
-      <c r="R21" s="244"/>
-      <c r="S21" s="244"/>
-      <c r="T21" s="259"/>
-      <c r="U21" s="244"/>
+      <c r="M21" s="257"/>
+      <c r="N21" s="260"/>
+      <c r="O21" s="257"/>
+      <c r="P21" s="257"/>
+      <c r="Q21" s="257"/>
+      <c r="R21" s="257"/>
+      <c r="S21" s="257"/>
+      <c r="T21" s="263"/>
+      <c r="U21" s="257"/>
       <c r="V21" s="34"/>
       <c r="W21" s="29"/>
       <c r="X21" s="29"/>
     </row>
     <row r="22" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33"/>
-      <c r="B22" s="253"/>
+      <c r="B22" s="255"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
@@ -4877,22 +4907,22 @@
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="35"/>
-      <c r="M22" s="255"/>
-      <c r="N22" s="257"/>
-      <c r="O22" s="255"/>
-      <c r="P22" s="255"/>
-      <c r="Q22" s="255"/>
-      <c r="R22" s="255"/>
-      <c r="S22" s="255"/>
-      <c r="T22" s="260"/>
-      <c r="U22" s="255"/>
+      <c r="M22" s="258"/>
+      <c r="N22" s="261"/>
+      <c r="O22" s="258"/>
+      <c r="P22" s="258"/>
+      <c r="Q22" s="258"/>
+      <c r="R22" s="258"/>
+      <c r="S22" s="258"/>
+      <c r="T22" s="264"/>
+      <c r="U22" s="258"/>
       <c r="V22" s="34"/>
       <c r="W22" s="29"/>
       <c r="X22" s="29"/>
     </row>
     <row r="23" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="271"/>
-      <c r="B23" s="253"/>
+      <c r="A23" s="252"/>
+      <c r="B23" s="255"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -4903,22 +4933,22 @@
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="35"/>
-      <c r="M23" s="255"/>
-      <c r="N23" s="257"/>
-      <c r="O23" s="255"/>
-      <c r="P23" s="255"/>
-      <c r="Q23" s="255"/>
-      <c r="R23" s="255"/>
-      <c r="S23" s="255"/>
-      <c r="T23" s="260"/>
-      <c r="U23" s="255"/>
+      <c r="M23" s="258"/>
+      <c r="N23" s="261"/>
+      <c r="O23" s="258"/>
+      <c r="P23" s="258"/>
+      <c r="Q23" s="258"/>
+      <c r="R23" s="258"/>
+      <c r="S23" s="258"/>
+      <c r="T23" s="264"/>
+      <c r="U23" s="258"/>
       <c r="V23" s="34"/>
       <c r="W23" s="29"/>
       <c r="X23" s="29"/>
     </row>
     <row r="24" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="272"/>
-      <c r="B24" s="254"/>
+      <c r="A24" s="253"/>
+      <c r="B24" s="256"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
@@ -4929,15 +4959,15 @@
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="245"/>
-      <c r="N24" s="258"/>
-      <c r="O24" s="245"/>
-      <c r="P24" s="245"/>
-      <c r="Q24" s="245"/>
-      <c r="R24" s="245"/>
-      <c r="S24" s="245"/>
-      <c r="T24" s="261"/>
-      <c r="U24" s="245"/>
+      <c r="M24" s="259"/>
+      <c r="N24" s="262"/>
+      <c r="O24" s="259"/>
+      <c r="P24" s="259"/>
+      <c r="Q24" s="259"/>
+      <c r="R24" s="259"/>
+      <c r="S24" s="259"/>
+      <c r="T24" s="265"/>
+      <c r="U24" s="259"/>
       <c r="V24" s="34"/>
       <c r="W24" s="29"/>
       <c r="X24" s="29"/>
@@ -5257,33 +5287,33 @@
       </c>
       <c r="D40" s="72"/>
       <c r="E40" s="73"/>
-      <c r="F40" s="265" t="s">
+      <c r="F40" s="246" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="266"/>
-      <c r="H40" s="266"/>
-      <c r="I40" s="267"/>
-      <c r="J40" s="268" t="s">
+      <c r="G40" s="247"/>
+      <c r="H40" s="247"/>
+      <c r="I40" s="248"/>
+      <c r="J40" s="249" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="269"/>
-      <c r="L40" s="269"/>
-      <c r="M40" s="270"/>
+      <c r="K40" s="250"/>
+      <c r="L40" s="250"/>
+      <c r="M40" s="251"/>
       <c r="N40" s="74" t="s">
         <v>46</v>
       </c>
       <c r="P40" s="120"/>
-      <c r="Q40" s="264" t="s">
+      <c r="Q40" s="245" t="s">
         <v>116</v>
       </c>
-      <c r="R40" s="264"/>
-      <c r="S40" s="264"/>
-      <c r="T40" s="264"/>
-      <c r="U40" s="264"/>
-      <c r="V40" s="264"/>
-      <c r="W40" s="264"/>
-      <c r="X40" s="264"/>
-      <c r="Y40" s="264"/>
+      <c r="R40" s="245"/>
+      <c r="S40" s="245"/>
+      <c r="T40" s="245"/>
+      <c r="U40" s="245"/>
+      <c r="V40" s="245"/>
+      <c r="W40" s="245"/>
+      <c r="X40" s="245"/>
+      <c r="Y40" s="245"/>
       <c r="Z40" s="39"/>
       <c r="AA40" s="39"/>
       <c r="AB40" s="39"/>
@@ -13543,6 +13573,44 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="T13:T16"/>
+    <mergeCell ref="U13:U16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="U17:U20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
     <mergeCell ref="Q40:Y40"/>
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="J40:M40"/>
@@ -13557,44 +13625,6 @@
     <mergeCell ref="R21:R24"/>
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
-    <mergeCell ref="U17:U20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="S13:S16"/>
-    <mergeCell ref="T13:T16"/>
-    <mergeCell ref="U13:U16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="Q9:Q12"/>
   </mergeCells>
   <conditionalFormatting sqref="AM1:AM1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
Equipment Negative Testcase completed
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="169">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -508,27 +508,15 @@
     <t>Alphabets</t>
   </si>
   <si>
-    <t>Two Decimal</t>
-  </si>
-  <si>
     <t>Surface Area Data Source</t>
   </si>
   <si>
     <t>Can Preferential Transfer of Residue Occur with this Equipment?</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Can Preferential Transfer of Residue Occur with this Equipment?: </t>
-  </si>
-  <si>
-    <t>Equipment Surface Area Involved in Preferential Transfer</t>
-  </si>
-  <si>
     <t>Is this Equipment Involved in Primary Packaging?</t>
   </si>
   <si>
@@ -578,6 +566,44 @@
   </si>
   <si>
     <t>Choose Cleaning Process Type</t>
+  </si>
+  <si>
+    <t>Choose an option for preferential transfer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equipment Surface Area Involved in Preferential Transfer: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Equipment Surface Area Involved in Preferential Transfer: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter Preferential Surface area</t>
   </si>
 </sst>
 </file>
@@ -3561,10 +3587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:H46"/>
+  <dimension ref="A5:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,7 +3727,7 @@
         <v>134</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="241"/>
@@ -3751,7 +3777,7 @@
         <v>132</v>
       </c>
       <c r="F13" s="12">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -3762,7 +3788,7 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>141</v>
@@ -3771,7 +3797,7 @@
         <v>132</v>
       </c>
       <c r="F14" s="12">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -3807,7 +3833,7 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -3823,7 +3849,7 @@
       </c>
       <c r="E17" s="12"/>
       <c r="F17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
@@ -3854,7 +3880,7 @@
         <v>144</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -3870,7 +3896,7 @@
         <v>133</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F20" s="12">
         <v>123</v>
@@ -3885,10 +3911,10 @@
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="242" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F21" s="12">
         <v>1.23</v>
@@ -3902,7 +3928,7 @@
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>141</v>
@@ -3922,345 +3948,347 @@
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="80" t="s">
+        <v>165</v>
+      </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>18</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="C24" s="80" t="s">
+        <v>166</v>
+      </c>
       <c r="D24" s="12" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="F24" t="s">
+        <v>168</v>
+      </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>19</v>
-      </c>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>20</v>
-      </c>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="242" t="s">
-        <v>151</v>
-      </c>
+      <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="F26" s="12">
+        <v>6</v>
+      </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>21</v>
-      </c>
+      <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="12"/>
+        <v>144</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
-        <v>22</v>
-      </c>
+      <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+        <v>133</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" s="12">
+        <v>123</v>
+      </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>23</v>
-      </c>
+      <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
-      <c r="D29" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="D29" s="242" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F29" s="12">
+        <v>1.23</v>
+      </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <v>24</v>
-      </c>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12" t="s">
-        <v>133</v>
-      </c>
+      <c r="C30" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="242"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="242" t="s">
-        <v>145</v>
-      </c>
+      <c r="C31" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>149</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>162</v>
+      </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="E33" s="12"/>
-      <c r="F33" s="12" t="s">
-        <v>166</v>
+      <c r="F33" t="s">
+        <v>160</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="F34" t="s">
-        <v>164</v>
+      <c r="F34" s="12">
+        <v>6</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12">
-        <v>6</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="F36" s="12"/>
+        <v>157</v>
+      </c>
+      <c r="F36" s="12">
+        <v>123</v>
+      </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
-      <c r="D37" s="12" t="s">
-        <v>133</v>
+      <c r="D37" s="242" t="s">
+        <v>159</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F37" s="12">
-        <v>123</v>
+        <v>1.23</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="242" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>162</v>
+      <c r="C38" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="243" t="s">
+        <v>132</v>
       </c>
       <c r="F38" s="12">
-        <v>1.23</v>
+        <v>25</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E39" s="243" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="12">
-        <v>75</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" s="12"/>
+        <v>152</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="F40" t="s">
+        <v>164</v>
+      </c>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="E41" s="12"/>
-      <c r="F41" t="s">
-        <v>168</v>
-      </c>
+      <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+        <v>141</v>
+      </c>
+      <c r="E42" s="243" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" s="12">
+        <v>75</v>
+      </c>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="243" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="12">
-        <v>75</v>
-      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
-        <v>38</v>
-      </c>
+      <c r="A44" s="12"/>
       <c r="B44" s="12"/>
-      <c r="C44" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>141</v>
-      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -4275,16 +4303,6 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Completed DMS module smoke testing
</commit_message>
<xml_diff>
--- a/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
+++ b/eResidue_CV_eDocs/bin/Test Data/eResidue_eDocs_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520" tabRatio="663"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520" tabRatio="663" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Microbial_Calculation" sheetId="12" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="229">
   <si>
     <t>Testcase_id</t>
   </si>
@@ -446,12 +446,6 @@
     <t>Limit Selection Type</t>
   </si>
   <si>
-    <t>Test Product5</t>
-  </si>
-  <si>
-    <t>Test Product6</t>
-  </si>
-  <si>
     <t>Tenant ID:</t>
   </si>
   <si>
@@ -765,6 +759,9 @@
   </si>
   <si>
     <t>Equipment Group saved successfully</t>
+  </si>
+  <si>
+    <t>dfg</t>
   </si>
 </sst>
 </file>
@@ -1876,50 +1873,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1929,12 +1887,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1962,6 +1914,51 @@
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3279,8 +3276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A34" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -3326,15 +3323,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="218" t="s">
+      <c r="F1" s="239" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="218"/>
-      <c r="K1" s="218"/>
-      <c r="L1" s="218"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
       <c r="U1" s="15" t="s">
         <v>54</v>
       </c>
@@ -3380,22 +3377,22 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:43" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="219" t="s">
+      <c r="D6" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="220"/>
-      <c r="F6" s="220"/>
-      <c r="G6" s="220"/>
-      <c r="H6" s="221"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="242"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-      <c r="M6" s="219" t="s">
+      <c r="M6" s="240" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="220"/>
-      <c r="O6" s="220"/>
-      <c r="P6" s="220"/>
-      <c r="Q6" s="221"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
     </row>
     <row r="7" spans="1:43" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
@@ -3413,10 +3410,10 @@
       <c r="E7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="222" t="s">
+      <c r="F7" s="243" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="223"/>
+      <c r="G7" s="244"/>
       <c r="H7" s="17" t="s">
         <v>63</v>
       </c>
@@ -3439,10 +3436,10 @@
         <v>69</v>
       </c>
       <c r="O7" s="22"/>
-      <c r="P7" s="222" t="s">
+      <c r="P7" s="243" t="s">
         <v>70</v>
       </c>
-      <c r="Q7" s="223"/>
+      <c r="Q7" s="244"/>
       <c r="R7" s="23" t="s">
         <v>64</v>
       </c>
@@ -3496,7 +3493,7 @@
     </row>
     <row r="9" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
-      <c r="B9" s="224"/>
+      <c r="B9" s="231"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
@@ -3508,13 +3505,13 @@
       <c r="K9" s="29"/>
       <c r="L9" s="35"/>
       <c r="M9" s="216"/>
-      <c r="N9" s="228"/>
+      <c r="N9" s="234"/>
       <c r="O9" s="216"/>
       <c r="P9" s="216"/>
       <c r="Q9" s="216"/>
       <c r="R9" s="216"/>
       <c r="S9" s="216"/>
-      <c r="T9" s="231"/>
+      <c r="T9" s="219"/>
       <c r="U9" s="34"/>
       <c r="AE9" s="39"/>
       <c r="AF9" s="39"/>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="10" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33"/>
-      <c r="B10" s="225"/>
+      <c r="B10" s="232"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
@@ -3533,21 +3530,21 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="35"/>
-      <c r="M10" s="227"/>
-      <c r="N10" s="229"/>
-      <c r="O10" s="227"/>
-      <c r="P10" s="227"/>
-      <c r="Q10" s="227"/>
-      <c r="R10" s="227"/>
-      <c r="S10" s="227"/>
-      <c r="T10" s="232"/>
+      <c r="M10" s="217"/>
+      <c r="N10" s="235"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="217"/>
+      <c r="Q10" s="217"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="217"/>
+      <c r="T10" s="220"/>
       <c r="U10" s="34"/>
       <c r="AE10" s="39"/>
       <c r="AF10" s="39"/>
     </row>
     <row r="11" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="216"/>
-      <c r="B11" s="225"/>
+      <c r="B11" s="232"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -3558,14 +3555,14 @@
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
       <c r="L11" s="35"/>
-      <c r="M11" s="227"/>
-      <c r="N11" s="229"/>
-      <c r="O11" s="227"/>
-      <c r="P11" s="227"/>
-      <c r="Q11" s="227"/>
-      <c r="R11" s="227"/>
-      <c r="S11" s="227"/>
-      <c r="T11" s="232"/>
+      <c r="M11" s="217"/>
+      <c r="N11" s="235"/>
+      <c r="O11" s="217"/>
+      <c r="P11" s="217"/>
+      <c r="Q11" s="217"/>
+      <c r="R11" s="217"/>
+      <c r="S11" s="217"/>
+      <c r="T11" s="220"/>
       <c r="U11" s="34"/>
       <c r="AE11" s="41"/>
       <c r="AF11" s="45"/>
@@ -3573,8 +3570,8 @@
       <c r="AQ11" s="49"/>
     </row>
     <row r="12" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="217"/>
-      <c r="B12" s="226"/>
+      <c r="A12" s="218"/>
+      <c r="B12" s="233"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
@@ -3585,21 +3582,21 @@
       <c r="J12" s="29"/>
       <c r="K12" s="29"/>
       <c r="L12" s="35"/>
-      <c r="M12" s="217"/>
-      <c r="N12" s="230"/>
-      <c r="O12" s="217"/>
-      <c r="P12" s="217"/>
-      <c r="Q12" s="217"/>
-      <c r="R12" s="217"/>
-      <c r="S12" s="217"/>
-      <c r="T12" s="233"/>
+      <c r="M12" s="218"/>
+      <c r="N12" s="236"/>
+      <c r="O12" s="218"/>
+      <c r="P12" s="218"/>
+      <c r="Q12" s="218"/>
+      <c r="R12" s="218"/>
+      <c r="S12" s="218"/>
+      <c r="T12" s="221"/>
       <c r="U12" s="34"/>
       <c r="AE12" s="39"/>
       <c r="AF12" s="39"/>
     </row>
     <row r="13" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
-      <c r="B13" s="224"/>
+      <c r="B13" s="231"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
@@ -3611,20 +3608,20 @@
       <c r="K13" s="29"/>
       <c r="L13" s="35"/>
       <c r="M13" s="216"/>
-      <c r="N13" s="228"/>
+      <c r="N13" s="234"/>
       <c r="O13" s="216"/>
       <c r="P13" s="216"/>
       <c r="Q13" s="216"/>
       <c r="R13" s="216"/>
       <c r="S13" s="216"/>
-      <c r="T13" s="231"/>
+      <c r="T13" s="219"/>
       <c r="U13" s="34"/>
       <c r="AO13" s="53"/>
       <c r="AP13" s="52"/>
     </row>
     <row r="14" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37"/>
-      <c r="B14" s="225"/>
+      <c r="B14" s="232"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
@@ -3635,21 +3632,21 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="227"/>
-      <c r="N14" s="229"/>
-      <c r="O14" s="227"/>
-      <c r="P14" s="227"/>
-      <c r="Q14" s="227"/>
-      <c r="R14" s="227"/>
-      <c r="S14" s="227"/>
-      <c r="T14" s="232"/>
+      <c r="M14" s="217"/>
+      <c r="N14" s="235"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217"/>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="220"/>
       <c r="U14" s="34"/>
       <c r="AO14" s="54"/>
       <c r="AP14" s="54"/>
     </row>
     <row r="15" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="234"/>
-      <c r="B15" s="225"/>
+      <c r="A15" s="237"/>
+      <c r="B15" s="232"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -3660,21 +3657,21 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="35"/>
-      <c r="M15" s="227"/>
-      <c r="N15" s="229"/>
-      <c r="O15" s="227"/>
-      <c r="P15" s="227"/>
-      <c r="Q15" s="227"/>
-      <c r="R15" s="227"/>
-      <c r="S15" s="227"/>
-      <c r="T15" s="232"/>
+      <c r="M15" s="217"/>
+      <c r="N15" s="235"/>
+      <c r="O15" s="217"/>
+      <c r="P15" s="217"/>
+      <c r="Q15" s="217"/>
+      <c r="R15" s="217"/>
+      <c r="S15" s="217"/>
+      <c r="T15" s="220"/>
       <c r="U15" s="34"/>
       <c r="AO15" s="39"/>
       <c r="AP15" s="39"/>
     </row>
     <row r="16" spans="1:43" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="235"/>
-      <c r="B16" s="226"/>
+      <c r="A16" s="238"/>
+      <c r="B16" s="233"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -3685,21 +3682,21 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
       <c r="L16" s="35"/>
-      <c r="M16" s="217"/>
-      <c r="N16" s="230"/>
-      <c r="O16" s="217"/>
-      <c r="P16" s="217"/>
-      <c r="Q16" s="217"/>
-      <c r="R16" s="217"/>
-      <c r="S16" s="217"/>
-      <c r="T16" s="233"/>
+      <c r="M16" s="218"/>
+      <c r="N16" s="236"/>
+      <c r="O16" s="218"/>
+      <c r="P16" s="218"/>
+      <c r="Q16" s="218"/>
+      <c r="R16" s="218"/>
+      <c r="S16" s="218"/>
+      <c r="T16" s="221"/>
       <c r="U16" s="34"/>
       <c r="AO16" s="48"/>
       <c r="AP16" s="48"/>
     </row>
     <row r="17" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32"/>
-      <c r="B17" s="224"/>
+      <c r="B17" s="231"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
@@ -3711,20 +3708,20 @@
       <c r="K17" s="29"/>
       <c r="L17" s="35"/>
       <c r="M17" s="216"/>
-      <c r="N17" s="228"/>
+      <c r="N17" s="234"/>
       <c r="O17" s="216"/>
       <c r="P17" s="216"/>
       <c r="Q17" s="216"/>
       <c r="R17" s="216"/>
       <c r="S17" s="216"/>
-      <c r="T17" s="231"/>
+      <c r="T17" s="219"/>
       <c r="U17" s="34"/>
       <c r="AO17" s="48"/>
       <c r="AP17" s="48"/>
     </row>
     <row r="18" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33"/>
-      <c r="B18" s="225"/>
+      <c r="B18" s="232"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -3735,19 +3732,19 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="35"/>
-      <c r="M18" s="227"/>
-      <c r="N18" s="229"/>
-      <c r="O18" s="227"/>
-      <c r="P18" s="227"/>
-      <c r="Q18" s="227"/>
-      <c r="R18" s="227"/>
-      <c r="S18" s="227"/>
-      <c r="T18" s="232"/>
+      <c r="M18" s="217"/>
+      <c r="N18" s="235"/>
+      <c r="O18" s="217"/>
+      <c r="P18" s="217"/>
+      <c r="Q18" s="217"/>
+      <c r="R18" s="217"/>
+      <c r="S18" s="217"/>
+      <c r="T18" s="220"/>
       <c r="U18" s="34"/>
     </row>
     <row r="19" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="216"/>
-      <c r="B19" s="225"/>
+      <c r="B19" s="232"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
@@ -3758,19 +3755,19 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="35"/>
-      <c r="M19" s="227"/>
-      <c r="N19" s="229"/>
-      <c r="O19" s="227"/>
-      <c r="P19" s="227"/>
-      <c r="Q19" s="227"/>
-      <c r="R19" s="227"/>
-      <c r="S19" s="227"/>
-      <c r="T19" s="232"/>
+      <c r="M19" s="217"/>
+      <c r="N19" s="235"/>
+      <c r="O19" s="217"/>
+      <c r="P19" s="217"/>
+      <c r="Q19" s="217"/>
+      <c r="R19" s="217"/>
+      <c r="S19" s="217"/>
+      <c r="T19" s="220"/>
       <c r="U19" s="34"/>
     </row>
     <row r="20" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="217"/>
-      <c r="B20" s="226"/>
+      <c r="A20" s="218"/>
+      <c r="B20" s="233"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
@@ -3781,19 +3778,19 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="35"/>
-      <c r="M20" s="217"/>
-      <c r="N20" s="230"/>
-      <c r="O20" s="217"/>
-      <c r="P20" s="217"/>
-      <c r="Q20" s="217"/>
-      <c r="R20" s="217"/>
-      <c r="S20" s="217"/>
-      <c r="T20" s="233"/>
+      <c r="M20" s="218"/>
+      <c r="N20" s="236"/>
+      <c r="O20" s="218"/>
+      <c r="P20" s="218"/>
+      <c r="Q20" s="218"/>
+      <c r="R20" s="218"/>
+      <c r="S20" s="218"/>
+      <c r="T20" s="221"/>
       <c r="U20" s="34"/>
     </row>
     <row r="21" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32"/>
-      <c r="B21" s="224"/>
+      <c r="B21" s="231"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
@@ -3805,18 +3802,18 @@
       <c r="K21" s="29"/>
       <c r="L21" s="35"/>
       <c r="M21" s="216"/>
-      <c r="N21" s="228"/>
+      <c r="N21" s="234"/>
       <c r="O21" s="216"/>
       <c r="P21" s="216"/>
       <c r="Q21" s="216"/>
       <c r="R21" s="216"/>
       <c r="S21" s="216"/>
-      <c r="T21" s="231"/>
+      <c r="T21" s="219"/>
       <c r="U21" s="34"/>
     </row>
     <row r="22" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33"/>
-      <c r="B22" s="225"/>
+      <c r="B22" s="232"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
@@ -3827,19 +3824,19 @@
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="35"/>
-      <c r="M22" s="227"/>
-      <c r="N22" s="229"/>
-      <c r="O22" s="227"/>
-      <c r="P22" s="227"/>
-      <c r="Q22" s="227"/>
-      <c r="R22" s="227"/>
-      <c r="S22" s="227"/>
-      <c r="T22" s="232"/>
+      <c r="M22" s="217"/>
+      <c r="N22" s="235"/>
+      <c r="O22" s="217"/>
+      <c r="P22" s="217"/>
+      <c r="Q22" s="217"/>
+      <c r="R22" s="217"/>
+      <c r="S22" s="217"/>
+      <c r="T22" s="220"/>
       <c r="U22" s="34"/>
     </row>
     <row r="23" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="236"/>
-      <c r="B23" s="225"/>
+      <c r="A23" s="222"/>
+      <c r="B23" s="232"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -3850,19 +3847,19 @@
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="35"/>
-      <c r="M23" s="227"/>
-      <c r="N23" s="229"/>
-      <c r="O23" s="227"/>
-      <c r="P23" s="227"/>
-      <c r="Q23" s="227"/>
-      <c r="R23" s="227"/>
-      <c r="S23" s="227"/>
-      <c r="T23" s="232"/>
+      <c r="M23" s="217"/>
+      <c r="N23" s="235"/>
+      <c r="O23" s="217"/>
+      <c r="P23" s="217"/>
+      <c r="Q23" s="217"/>
+      <c r="R23" s="217"/>
+      <c r="S23" s="217"/>
+      <c r="T23" s="220"/>
       <c r="U23" s="34"/>
     </row>
     <row r="24" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="237"/>
-      <c r="B24" s="226"/>
+      <c r="A24" s="223"/>
+      <c r="B24" s="233"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
@@ -3873,14 +3870,14 @@
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="217"/>
-      <c r="N24" s="230"/>
-      <c r="O24" s="217"/>
-      <c r="P24" s="217"/>
-      <c r="Q24" s="217"/>
-      <c r="R24" s="217"/>
-      <c r="S24" s="217"/>
-      <c r="T24" s="233"/>
+      <c r="M24" s="218"/>
+      <c r="N24" s="236"/>
+      <c r="O24" s="218"/>
+      <c r="P24" s="218"/>
+      <c r="Q24" s="218"/>
+      <c r="R24" s="218"/>
+      <c r="S24" s="218"/>
+      <c r="T24" s="221"/>
       <c r="U24" s="34"/>
     </row>
     <row r="25" spans="1:42" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4069,7 +4066,7 @@
     </row>
     <row r="38" spans="1:37" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="151" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:37" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -4175,40 +4172,40 @@
     </row>
     <row r="40" spans="1:37" ht="69.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="148" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" s="149" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="66"/>
       <c r="E40" s="67"/>
-      <c r="F40" s="238" t="s">
+      <c r="F40" s="224" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="239"/>
-      <c r="H40" s="239"/>
-      <c r="I40" s="240"/>
-      <c r="J40" s="241" t="s">
+      <c r="G40" s="225"/>
+      <c r="H40" s="225"/>
+      <c r="I40" s="226"/>
+      <c r="J40" s="227" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="242"/>
-      <c r="L40" s="242"/>
-      <c r="M40" s="243"/>
+      <c r="K40" s="228"/>
+      <c r="L40" s="228"/>
+      <c r="M40" s="229"/>
       <c r="N40" s="68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O40" s="205" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P40" s="102"/>
-      <c r="Q40" s="244" t="s">
+      <c r="Q40" s="230" t="s">
         <v>116</v>
       </c>
-      <c r="R40" s="244"/>
-      <c r="S40" s="244"/>
-      <c r="T40" s="244"/>
-      <c r="U40" s="244"/>
-      <c r="V40" s="244"/>
+      <c r="R40" s="230"/>
+      <c r="S40" s="230"/>
+      <c r="T40" s="230"/>
+      <c r="U40" s="230"/>
+      <c r="V40" s="230"/>
       <c r="W40" s="39"/>
       <c r="X40" s="39"/>
       <c r="Y40" s="59"/>
@@ -4232,14 +4229,15 @@
       <c r="B41" s="147" t="s">
         <v>108</v>
       </c>
+      <c r="C41" s="27"/>
       <c r="D41" s="112" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E41" s="113" t="s">
         <v>87</v>
       </c>
       <c r="F41" s="113" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G41" s="113" t="s">
         <v>89</v>
@@ -4248,10 +4246,10 @@
         <v>90</v>
       </c>
       <c r="I41" s="112" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J41" s="115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K41" s="115" t="s">
         <v>89</v>
@@ -4260,7 +4258,7 @@
         <v>90</v>
       </c>
       <c r="M41" s="204" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N41" s="206" t="s">
         <v>91</v>
@@ -4321,7 +4319,7 @@
         <v>91</v>
       </c>
       <c r="AJ41" s="160" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AK41" s="16"/>
     </row>
@@ -4329,8 +4327,9 @@
       <c r="A42" s="125">
         <v>1</v>
       </c>
-      <c r="B42" s="125" t="s">
-        <v>124</v>
+      <c r="B42" s="125"/>
+      <c r="C42" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
@@ -4371,9 +4370,8 @@
       <c r="A43" s="125">
         <v>2</v>
       </c>
-      <c r="B43" s="125" t="s">
-        <v>125</v>
-      </c>
+      <c r="B43" s="125"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="119"/>
@@ -4412,6 +4410,7 @@
     <row r="44" spans="1:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="125"/>
       <c r="B44" s="125"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="118"/>
@@ -4450,6 +4449,7 @@
     <row r="45" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="125"/>
       <c r="B45" s="125"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="118"/>
@@ -4488,6 +4488,7 @@
     <row r="46" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="125"/>
       <c r="B46" s="125"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="118"/>
@@ -4526,6 +4527,7 @@
     <row r="47" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="125"/>
       <c r="B47" s="125"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="118"/>
@@ -4564,6 +4566,7 @@
     <row r="48" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="125"/>
       <c r="B48" s="125"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
       <c r="F48" s="118"/>
@@ -4602,6 +4605,7 @@
     <row r="49" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="125"/>
       <c r="B49" s="125"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
       <c r="F49" s="118"/>
@@ -4640,6 +4644,7 @@
     <row r="50" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="125"/>
       <c r="B50" s="125"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
       <c r="F50" s="118"/>
@@ -4678,6 +4683,7 @@
     <row r="51" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="125"/>
       <c r="B51" s="125"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
       <c r="F51" s="118"/>
@@ -4716,6 +4722,7 @@
     <row r="52" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="125"/>
       <c r="B52" s="125"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
       <c r="F52" s="118"/>
@@ -4754,6 +4761,7 @@
     <row r="53" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="125"/>
       <c r="B53" s="125"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
       <c r="F53" s="118"/>
@@ -4792,6 +4800,7 @@
     <row r="54" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="125"/>
       <c r="B54" s="125"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
       <c r="F54" s="118"/>
@@ -4830,6 +4839,7 @@
     <row r="55" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="125"/>
       <c r="B55" s="125"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
       <c r="F55" s="118"/>
@@ -26375,6 +26385,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="T13:T16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q17:Q20"/>
     <mergeCell ref="R17:R20"/>
     <mergeCell ref="S17:S20"/>
     <mergeCell ref="T17:T20"/>
@@ -26391,38 +26433,6 @@
     <mergeCell ref="R21:R24"/>
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="S13:S16"/>
-    <mergeCell ref="T13:T16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="Q9:Q12"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
   </mergeCells>
   <conditionalFormatting sqref="AH1:AH57 AH622:AH1048576">
     <cfRule type="duplicateValues" dxfId="93" priority="47"/>
@@ -26585,8 +26595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV621"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -26635,15 +26645,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="F1" s="218" t="s">
+      <c r="F1" s="239" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="218"/>
-      <c r="H1" s="218"/>
-      <c r="I1" s="218"/>
-      <c r="J1" s="218"/>
-      <c r="K1" s="218"/>
-      <c r="L1" s="218"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
       <c r="U1" s="15" t="s">
         <v>53</v>
       </c>
@@ -26692,22 +26702,22 @@
       <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="219" t="s">
+      <c r="D6" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="220"/>
-      <c r="F6" s="220"/>
-      <c r="G6" s="220"/>
-      <c r="H6" s="221"/>
+      <c r="E6" s="241"/>
+      <c r="F6" s="241"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="242"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
-      <c r="M6" s="219" t="s">
+      <c r="M6" s="240" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="220"/>
-      <c r="O6" s="220"/>
-      <c r="P6" s="220"/>
-      <c r="Q6" s="221"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
     </row>
     <row r="7" spans="1:48" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
@@ -26725,10 +26735,10 @@
       <c r="E7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="222" t="s">
+      <c r="F7" s="243" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="223"/>
+      <c r="G7" s="244"/>
       <c r="H7" s="17" t="s">
         <v>63</v>
       </c>
@@ -26751,10 +26761,10 @@
         <v>69</v>
       </c>
       <c r="O7" s="22"/>
-      <c r="P7" s="222" t="s">
+      <c r="P7" s="243" t="s">
         <v>70</v>
       </c>
-      <c r="Q7" s="223"/>
+      <c r="Q7" s="244"/>
       <c r="R7" s="23" t="s">
         <v>64</v>
       </c>
@@ -26822,7 +26832,7 @@
     </row>
     <row r="9" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="32"/>
-      <c r="B9" s="224"/>
+      <c r="B9" s="231"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
@@ -26834,13 +26844,13 @@
       <c r="K9" s="29"/>
       <c r="L9" s="35"/>
       <c r="M9" s="216"/>
-      <c r="N9" s="228"/>
+      <c r="N9" s="234"/>
       <c r="O9" s="216"/>
       <c r="P9" s="216"/>
       <c r="Q9" s="216"/>
       <c r="R9" s="216"/>
       <c r="S9" s="216"/>
-      <c r="T9" s="231"/>
+      <c r="T9" s="219"/>
       <c r="U9" s="216"/>
       <c r="V9" s="34"/>
       <c r="W9" s="29"/>
@@ -26851,7 +26861,7 @@
     </row>
     <row r="10" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33"/>
-      <c r="B10" s="225"/>
+      <c r="B10" s="232"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
@@ -26862,15 +26872,15 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="35"/>
-      <c r="M10" s="227"/>
-      <c r="N10" s="229"/>
-      <c r="O10" s="227"/>
-      <c r="P10" s="227"/>
-      <c r="Q10" s="227"/>
-      <c r="R10" s="227"/>
-      <c r="S10" s="227"/>
-      <c r="T10" s="232"/>
-      <c r="U10" s="227"/>
+      <c r="M10" s="217"/>
+      <c r="N10" s="235"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="217"/>
+      <c r="Q10" s="217"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="217"/>
+      <c r="T10" s="220"/>
+      <c r="U10" s="217"/>
       <c r="V10" s="34"/>
       <c r="W10" s="29"/>
       <c r="X10" s="29"/>
@@ -26879,7 +26889,7 @@
     </row>
     <row r="11" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="216"/>
-      <c r="B11" s="225"/>
+      <c r="B11" s="232"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
@@ -26890,15 +26900,15 @@
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
       <c r="L11" s="35"/>
-      <c r="M11" s="227"/>
-      <c r="N11" s="229"/>
-      <c r="O11" s="227"/>
-      <c r="P11" s="227"/>
-      <c r="Q11" s="227"/>
-      <c r="R11" s="227"/>
-      <c r="S11" s="227"/>
-      <c r="T11" s="232"/>
-      <c r="U11" s="227"/>
+      <c r="M11" s="217"/>
+      <c r="N11" s="235"/>
+      <c r="O11" s="217"/>
+      <c r="P11" s="217"/>
+      <c r="Q11" s="217"/>
+      <c r="R11" s="217"/>
+      <c r="S11" s="217"/>
+      <c r="T11" s="220"/>
+      <c r="U11" s="217"/>
       <c r="V11" s="34"/>
       <c r="W11" s="29"/>
       <c r="X11" s="29"/>
@@ -26908,8 +26918,8 @@
       <c r="AV11" s="49"/>
     </row>
     <row r="12" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="217"/>
-      <c r="B12" s="226"/>
+      <c r="A12" s="218"/>
+      <c r="B12" s="233"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
@@ -26920,15 +26930,15 @@
       <c r="J12" s="29"/>
       <c r="K12" s="29"/>
       <c r="L12" s="35"/>
-      <c r="M12" s="217"/>
-      <c r="N12" s="230"/>
-      <c r="O12" s="217"/>
-      <c r="P12" s="217"/>
-      <c r="Q12" s="217"/>
-      <c r="R12" s="217"/>
-      <c r="S12" s="217"/>
-      <c r="T12" s="233"/>
-      <c r="U12" s="217"/>
+      <c r="M12" s="218"/>
+      <c r="N12" s="236"/>
+      <c r="O12" s="218"/>
+      <c r="P12" s="218"/>
+      <c r="Q12" s="218"/>
+      <c r="R12" s="218"/>
+      <c r="S12" s="218"/>
+      <c r="T12" s="221"/>
+      <c r="U12" s="218"/>
       <c r="V12" s="34"/>
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
@@ -26937,7 +26947,7 @@
     </row>
     <row r="13" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="36"/>
-      <c r="B13" s="224"/>
+      <c r="B13" s="231"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
@@ -26949,13 +26959,13 @@
       <c r="K13" s="29"/>
       <c r="L13" s="35"/>
       <c r="M13" s="216"/>
-      <c r="N13" s="228"/>
+      <c r="N13" s="234"/>
       <c r="O13" s="216"/>
       <c r="P13" s="216"/>
       <c r="Q13" s="216"/>
       <c r="R13" s="216"/>
       <c r="S13" s="216"/>
-      <c r="T13" s="231"/>
+      <c r="T13" s="219"/>
       <c r="U13" s="216"/>
       <c r="V13" s="34"/>
       <c r="W13" s="29"/>
@@ -26965,7 +26975,7 @@
     </row>
     <row r="14" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="37"/>
-      <c r="B14" s="225"/>
+      <c r="B14" s="232"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
@@ -26976,15 +26986,15 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="227"/>
-      <c r="N14" s="229"/>
-      <c r="O14" s="227"/>
-      <c r="P14" s="227"/>
-      <c r="Q14" s="227"/>
-      <c r="R14" s="227"/>
-      <c r="S14" s="227"/>
-      <c r="T14" s="232"/>
-      <c r="U14" s="227"/>
+      <c r="M14" s="217"/>
+      <c r="N14" s="235"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217"/>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="220"/>
+      <c r="U14" s="217"/>
       <c r="V14" s="34"/>
       <c r="W14" s="29"/>
       <c r="X14" s="29"/>
@@ -26992,8 +27002,8 @@
       <c r="AU14" s="54"/>
     </row>
     <row r="15" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="234"/>
-      <c r="B15" s="225"/>
+      <c r="A15" s="237"/>
+      <c r="B15" s="232"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -27004,15 +27014,15 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="35"/>
-      <c r="M15" s="227"/>
-      <c r="N15" s="229"/>
-      <c r="O15" s="227"/>
-      <c r="P15" s="227"/>
-      <c r="Q15" s="227"/>
-      <c r="R15" s="227"/>
-      <c r="S15" s="227"/>
-      <c r="T15" s="232"/>
-      <c r="U15" s="227"/>
+      <c r="M15" s="217"/>
+      <c r="N15" s="235"/>
+      <c r="O15" s="217"/>
+      <c r="P15" s="217"/>
+      <c r="Q15" s="217"/>
+      <c r="R15" s="217"/>
+      <c r="S15" s="217"/>
+      <c r="T15" s="220"/>
+      <c r="U15" s="217"/>
       <c r="V15" s="34"/>
       <c r="W15" s="29"/>
       <c r="X15" s="29"/>
@@ -27020,8 +27030,8 @@
       <c r="AU15" s="39"/>
     </row>
     <row r="16" spans="1:48" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="235"/>
-      <c r="B16" s="226"/>
+      <c r="A16" s="238"/>
+      <c r="B16" s="233"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
@@ -27032,15 +27042,15 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
       <c r="L16" s="35"/>
-      <c r="M16" s="217"/>
-      <c r="N16" s="230"/>
-      <c r="O16" s="217"/>
-      <c r="P16" s="217"/>
-      <c r="Q16" s="217"/>
-      <c r="R16" s="217"/>
-      <c r="S16" s="217"/>
-      <c r="T16" s="233"/>
-      <c r="U16" s="217"/>
+      <c r="M16" s="218"/>
+      <c r="N16" s="236"/>
+      <c r="O16" s="218"/>
+      <c r="P16" s="218"/>
+      <c r="Q16" s="218"/>
+      <c r="R16" s="218"/>
+      <c r="S16" s="218"/>
+      <c r="T16" s="221"/>
+      <c r="U16" s="218"/>
       <c r="V16" s="34"/>
       <c r="W16" s="29"/>
       <c r="X16" s="29"/>
@@ -27049,7 +27059,7 @@
     </row>
     <row r="17" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32"/>
-      <c r="B17" s="224"/>
+      <c r="B17" s="231"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
@@ -27061,13 +27071,13 @@
       <c r="K17" s="29"/>
       <c r="L17" s="35"/>
       <c r="M17" s="216"/>
-      <c r="N17" s="228"/>
+      <c r="N17" s="234"/>
       <c r="O17" s="216"/>
       <c r="P17" s="216"/>
       <c r="Q17" s="216"/>
       <c r="R17" s="216"/>
       <c r="S17" s="216"/>
-      <c r="T17" s="231"/>
+      <c r="T17" s="219"/>
       <c r="U17" s="216"/>
       <c r="V17" s="34"/>
       <c r="W17" s="29"/>
@@ -27077,7 +27087,7 @@
     </row>
     <row r="18" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33"/>
-      <c r="B18" s="225"/>
+      <c r="B18" s="232"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -27088,22 +27098,22 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="35"/>
-      <c r="M18" s="227"/>
-      <c r="N18" s="229"/>
-      <c r="O18" s="227"/>
-      <c r="P18" s="227"/>
-      <c r="Q18" s="227"/>
-      <c r="R18" s="227"/>
-      <c r="S18" s="227"/>
-      <c r="T18" s="232"/>
-      <c r="U18" s="227"/>
+      <c r="M18" s="217"/>
+      <c r="N18" s="235"/>
+      <c r="O18" s="217"/>
+      <c r="P18" s="217"/>
+      <c r="Q18" s="217"/>
+      <c r="R18" s="217"/>
+      <c r="S18" s="217"/>
+      <c r="T18" s="220"/>
+      <c r="U18" s="217"/>
       <c r="V18" s="34"/>
       <c r="W18" s="29"/>
       <c r="X18" s="29"/>
     </row>
     <row r="19" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="216"/>
-      <c r="B19" s="225"/>
+      <c r="B19" s="232"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
@@ -27114,22 +27124,22 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="35"/>
-      <c r="M19" s="227"/>
-      <c r="N19" s="229"/>
-      <c r="O19" s="227"/>
-      <c r="P19" s="227"/>
-      <c r="Q19" s="227"/>
-      <c r="R19" s="227"/>
-      <c r="S19" s="227"/>
-      <c r="T19" s="232"/>
-      <c r="U19" s="227"/>
+      <c r="M19" s="217"/>
+      <c r="N19" s="235"/>
+      <c r="O19" s="217"/>
+      <c r="P19" s="217"/>
+      <c r="Q19" s="217"/>
+      <c r="R19" s="217"/>
+      <c r="S19" s="217"/>
+      <c r="T19" s="220"/>
+      <c r="U19" s="217"/>
       <c r="V19" s="34"/>
       <c r="W19" s="29"/>
       <c r="X19" s="29"/>
     </row>
     <row r="20" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="217"/>
-      <c r="B20" s="226"/>
+      <c r="A20" s="218"/>
+      <c r="B20" s="233"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
@@ -27140,22 +27150,22 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="35"/>
-      <c r="M20" s="217"/>
-      <c r="N20" s="230"/>
-      <c r="O20" s="217"/>
-      <c r="P20" s="217"/>
-      <c r="Q20" s="217"/>
-      <c r="R20" s="217"/>
-      <c r="S20" s="217"/>
-      <c r="T20" s="233"/>
-      <c r="U20" s="217"/>
+      <c r="M20" s="218"/>
+      <c r="N20" s="236"/>
+      <c r="O20" s="218"/>
+      <c r="P20" s="218"/>
+      <c r="Q20" s="218"/>
+      <c r="R20" s="218"/>
+      <c r="S20" s="218"/>
+      <c r="T20" s="221"/>
+      <c r="U20" s="218"/>
       <c r="V20" s="34"/>
       <c r="W20" s="29"/>
       <c r="X20" s="29"/>
     </row>
     <row r="21" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="32"/>
-      <c r="B21" s="224"/>
+      <c r="B21" s="231"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
@@ -27167,13 +27177,13 @@
       <c r="K21" s="29"/>
       <c r="L21" s="35"/>
       <c r="M21" s="216"/>
-      <c r="N21" s="228"/>
+      <c r="N21" s="234"/>
       <c r="O21" s="216"/>
       <c r="P21" s="216"/>
       <c r="Q21" s="216"/>
       <c r="R21" s="216"/>
       <c r="S21" s="216"/>
-      <c r="T21" s="231"/>
+      <c r="T21" s="219"/>
       <c r="U21" s="216"/>
       <c r="V21" s="34"/>
       <c r="W21" s="29"/>
@@ -27181,7 +27191,7 @@
     </row>
     <row r="22" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33"/>
-      <c r="B22" s="225"/>
+      <c r="B22" s="232"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
@@ -27192,22 +27202,22 @@
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="35"/>
-      <c r="M22" s="227"/>
-      <c r="N22" s="229"/>
-      <c r="O22" s="227"/>
-      <c r="P22" s="227"/>
-      <c r="Q22" s="227"/>
-      <c r="R22" s="227"/>
-      <c r="S22" s="227"/>
-      <c r="T22" s="232"/>
-      <c r="U22" s="227"/>
+      <c r="M22" s="217"/>
+      <c r="N22" s="235"/>
+      <c r="O22" s="217"/>
+      <c r="P22" s="217"/>
+      <c r="Q22" s="217"/>
+      <c r="R22" s="217"/>
+      <c r="S22" s="217"/>
+      <c r="T22" s="220"/>
+      <c r="U22" s="217"/>
       <c r="V22" s="34"/>
       <c r="W22" s="29"/>
       <c r="X22" s="29"/>
     </row>
     <row r="23" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="236"/>
-      <c r="B23" s="225"/>
+      <c r="A23" s="222"/>
+      <c r="B23" s="232"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -27218,22 +27228,22 @@
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="35"/>
-      <c r="M23" s="227"/>
-      <c r="N23" s="229"/>
-      <c r="O23" s="227"/>
-      <c r="P23" s="227"/>
-      <c r="Q23" s="227"/>
-      <c r="R23" s="227"/>
-      <c r="S23" s="227"/>
-      <c r="T23" s="232"/>
-      <c r="U23" s="227"/>
+      <c r="M23" s="217"/>
+      <c r="N23" s="235"/>
+      <c r="O23" s="217"/>
+      <c r="P23" s="217"/>
+      <c r="Q23" s="217"/>
+      <c r="R23" s="217"/>
+      <c r="S23" s="217"/>
+      <c r="T23" s="220"/>
+      <c r="U23" s="217"/>
       <c r="V23" s="34"/>
       <c r="W23" s="29"/>
       <c r="X23" s="29"/>
     </row>
     <row r="24" spans="1:47" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="237"/>
-      <c r="B24" s="226"/>
+      <c r="A24" s="223"/>
+      <c r="B24" s="233"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
@@ -27244,15 +27254,15 @@
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="217"/>
-      <c r="N24" s="230"/>
-      <c r="O24" s="217"/>
-      <c r="P24" s="217"/>
-      <c r="Q24" s="217"/>
-      <c r="R24" s="217"/>
-      <c r="S24" s="217"/>
-      <c r="T24" s="233"/>
-      <c r="U24" s="217"/>
+      <c r="M24" s="218"/>
+      <c r="N24" s="236"/>
+      <c r="O24" s="218"/>
+      <c r="P24" s="218"/>
+      <c r="Q24" s="218"/>
+      <c r="R24" s="218"/>
+      <c r="S24" s="218"/>
+      <c r="T24" s="221"/>
+      <c r="U24" s="218"/>
       <c r="V24" s="34"/>
       <c r="W24" s="29"/>
       <c r="X24" s="29"/>
@@ -27444,7 +27454,7 @@
     </row>
     <row r="38" spans="1:42" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="151" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:42" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -27565,40 +27575,40 @@
     </row>
     <row r="40" spans="1:42" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="148" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" s="149" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="66"/>
       <c r="E40" s="67"/>
-      <c r="F40" s="238" t="s">
+      <c r="F40" s="224" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="239"/>
-      <c r="H40" s="239"/>
-      <c r="I40" s="240"/>
-      <c r="J40" s="241" t="s">
+      <c r="G40" s="225"/>
+      <c r="H40" s="225"/>
+      <c r="I40" s="226"/>
+      <c r="J40" s="227" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="242"/>
-      <c r="L40" s="242"/>
-      <c r="M40" s="243"/>
+      <c r="K40" s="228"/>
+      <c r="L40" s="228"/>
+      <c r="M40" s="229"/>
       <c r="N40" s="68" t="s">
         <v>46</v>
       </c>
       <c r="P40" s="102"/>
-      <c r="Q40" s="244" t="s">
+      <c r="Q40" s="230" t="s">
         <v>116</v>
       </c>
-      <c r="R40" s="244"/>
-      <c r="S40" s="244"/>
-      <c r="T40" s="244"/>
-      <c r="U40" s="244"/>
-      <c r="V40" s="244"/>
-      <c r="W40" s="244"/>
-      <c r="X40" s="244"/>
-      <c r="Y40" s="244"/>
+      <c r="R40" s="230"/>
+      <c r="S40" s="230"/>
+      <c r="T40" s="230"/>
+      <c r="U40" s="230"/>
+      <c r="V40" s="230"/>
+      <c r="W40" s="230"/>
+      <c r="X40" s="230"/>
+      <c r="Y40" s="230"/>
       <c r="Z40" s="39"/>
       <c r="AA40" s="39"/>
       <c r="AB40" s="39"/>
@@ -27727,7 +27737,7 @@
         <v>91</v>
       </c>
       <c r="AO41" s="160" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AP41" s="16"/>
     </row>
@@ -27735,9 +27745,8 @@
       <c r="A42" s="125">
         <v>1</v>
       </c>
-      <c r="B42" s="125" t="s">
-        <v>124</v>
-      </c>
+      <c r="B42" s="125"/>
+      <c r="C42" s="125"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="118"/>
@@ -27782,9 +27791,8 @@
       <c r="A43" s="125">
         <v>2</v>
       </c>
-      <c r="B43" s="125" t="s">
-        <v>125</v>
-      </c>
+      <c r="B43" s="125"/>
+      <c r="C43" s="125"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="119"/>
@@ -27828,6 +27836,7 @@
     <row r="44" spans="1:42" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="125"/>
       <c r="B44" s="125"/>
+      <c r="C44" s="125"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="118"/>
@@ -27871,6 +27880,7 @@
     <row r="45" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="125"/>
       <c r="B45" s="125"/>
+      <c r="C45" s="125"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="118"/>
@@ -27914,6 +27924,7 @@
     <row r="46" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="125"/>
       <c r="B46" s="125"/>
+      <c r="C46" s="125"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="118"/>
@@ -27957,6 +27968,7 @@
     <row r="47" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="125"/>
       <c r="B47" s="125"/>
+      <c r="C47" s="125"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="118"/>
@@ -27999,6 +28011,7 @@
     <row r="48" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="125"/>
       <c r="B48" s="125"/>
+      <c r="C48" s="125"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
       <c r="F48" s="118"/>
@@ -28041,6 +28054,7 @@
     <row r="49" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="125"/>
       <c r="B49" s="125"/>
+      <c r="C49" s="125"/>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
       <c r="F49" s="118"/>
@@ -28083,6 +28097,7 @@
     <row r="50" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="125"/>
       <c r="B50" s="125"/>
+      <c r="C50" s="125"/>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
       <c r="F50" s="118"/>
@@ -28125,6 +28140,7 @@
     <row r="51" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="125"/>
       <c r="B51" s="125"/>
+      <c r="C51" s="125"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
       <c r="F51" s="118"/>
@@ -28167,6 +28183,7 @@
     <row r="52" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="125"/>
       <c r="B52" s="125"/>
+      <c r="C52" s="125"/>
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
       <c r="F52" s="118"/>
@@ -28209,6 +28226,7 @@
     <row r="53" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="125"/>
       <c r="B53" s="125"/>
+      <c r="C53" s="125"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
       <c r="F53" s="118"/>
@@ -28251,6 +28269,7 @@
     <row r="54" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="125"/>
       <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
       <c r="F54" s="118"/>
@@ -28293,6 +28312,7 @@
     <row r="55" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="125"/>
       <c r="B55" s="125"/>
+      <c r="C55" s="125"/>
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
       <c r="F55" s="118"/>
@@ -28335,6 +28355,7 @@
     <row r="56" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="125"/>
       <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
       <c r="D56" s="27"/>
       <c r="E56" s="27"/>
       <c r="F56" s="118"/>
@@ -28377,6 +28398,7 @@
     <row r="57" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="125"/>
       <c r="B57" s="125"/>
+      <c r="C57" s="125"/>
       <c r="D57" s="27"/>
       <c r="E57" s="27"/>
       <c r="F57" s="107"/>
@@ -28419,6 +28441,7 @@
     <row r="58" spans="1:42" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="125"/>
       <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
       <c r="D58" s="27"/>
       <c r="E58" s="27"/>
       <c r="F58" s="118"/>
@@ -28462,6 +28485,7 @@
     <row r="59" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="125"/>
       <c r="B59" s="125"/>
+      <c r="C59" s="125"/>
       <c r="D59" s="27"/>
       <c r="E59" s="27"/>
       <c r="F59" s="118"/>
@@ -28505,6 +28529,7 @@
     <row r="60" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="125"/>
       <c r="B60" s="125"/>
+      <c r="C60" s="125"/>
       <c r="D60" s="27"/>
       <c r="E60" s="27"/>
       <c r="F60" s="118"/>
@@ -28548,6 +28573,7 @@
     <row r="61" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="125"/>
       <c r="B61" s="125"/>
+      <c r="C61" s="125"/>
       <c r="D61" s="27"/>
       <c r="E61" s="27"/>
       <c r="F61" s="118"/>
@@ -28590,6 +28616,7 @@
     <row r="62" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="125"/>
       <c r="B62" s="125"/>
+      <c r="C62" s="125"/>
       <c r="D62" s="27"/>
       <c r="E62" s="27"/>
       <c r="F62" s="118"/>
@@ -28632,6 +28659,7 @@
     <row r="63" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="125"/>
       <c r="B63" s="125"/>
+      <c r="C63" s="125"/>
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
       <c r="F63" s="118"/>
@@ -28674,6 +28702,7 @@
     <row r="64" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="125"/>
       <c r="B64" s="125"/>
+      <c r="C64" s="125"/>
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
       <c r="F64" s="118"/>
@@ -28716,6 +28745,7 @@
     <row r="65" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="125"/>
       <c r="B65" s="125"/>
+      <c r="C65" s="125"/>
       <c r="D65" s="27"/>
       <c r="E65" s="27"/>
       <c r="F65" s="118"/>
@@ -28758,6 +28788,7 @@
     <row r="66" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="125"/>
       <c r="B66" s="125"/>
+      <c r="C66" s="125"/>
       <c r="D66" s="27"/>
       <c r="E66" s="27"/>
       <c r="F66" s="118"/>
@@ -28800,6 +28831,7 @@
     <row r="67" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="125"/>
       <c r="B67" s="125"/>
+      <c r="C67" s="125"/>
       <c r="D67" s="27"/>
       <c r="E67" s="27"/>
       <c r="F67" s="118"/>
@@ -28842,6 +28874,7 @@
     <row r="68" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="125"/>
       <c r="B68" s="125"/>
+      <c r="C68" s="125"/>
       <c r="D68" s="27"/>
       <c r="E68" s="27"/>
       <c r="F68" s="118"/>
@@ -28884,6 +28917,7 @@
     <row r="69" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="125"/>
       <c r="B69" s="125"/>
+      <c r="C69" s="125"/>
       <c r="D69" s="27"/>
       <c r="E69" s="27"/>
       <c r="F69" s="118"/>
@@ -28926,6 +28960,7 @@
     <row r="70" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="125"/>
       <c r="B70" s="125"/>
+      <c r="C70" s="125"/>
       <c r="D70" s="27"/>
       <c r="E70" s="27"/>
       <c r="F70" s="118"/>
@@ -28968,6 +29003,7 @@
     <row r="71" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="125"/>
       <c r="B71" s="125"/>
+      <c r="C71" s="125"/>
       <c r="D71" s="27"/>
       <c r="E71" s="27"/>
       <c r="F71" s="107"/>
@@ -29010,6 +29046,7 @@
     <row r="72" spans="1:42" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="125"/>
       <c r="B72" s="125"/>
+      <c r="C72" s="125"/>
       <c r="D72" s="27"/>
       <c r="E72" s="27"/>
       <c r="F72" s="118"/>
@@ -29053,6 +29090,7 @@
     <row r="73" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="125"/>
       <c r="B73" s="125"/>
+      <c r="C73" s="125"/>
       <c r="D73" s="27"/>
       <c r="E73" s="27"/>
       <c r="F73" s="118"/>
@@ -29096,6 +29134,7 @@
     <row r="74" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="125"/>
       <c r="B74" s="125"/>
+      <c r="C74" s="125"/>
       <c r="D74" s="27"/>
       <c r="E74" s="27"/>
       <c r="F74" s="118"/>
@@ -29139,6 +29178,7 @@
     <row r="75" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="125"/>
       <c r="B75" s="125"/>
+      <c r="C75" s="125"/>
       <c r="D75" s="27"/>
       <c r="E75" s="27"/>
       <c r="F75" s="118"/>
@@ -29181,6 +29221,7 @@
     <row r="76" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="125"/>
       <c r="B76" s="125"/>
+      <c r="C76" s="125"/>
       <c r="D76" s="27"/>
       <c r="E76" s="27"/>
       <c r="F76" s="118"/>
@@ -29223,6 +29264,7 @@
     <row r="77" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="125"/>
       <c r="B77" s="125"/>
+      <c r="C77" s="125"/>
       <c r="D77" s="27"/>
       <c r="E77" s="27"/>
       <c r="F77" s="118"/>
@@ -29265,6 +29307,7 @@
     <row r="78" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="125"/>
       <c r="B78" s="125"/>
+      <c r="C78" s="125"/>
       <c r="D78" s="27"/>
       <c r="E78" s="27"/>
       <c r="F78" s="118"/>
@@ -29307,6 +29350,7 @@
     <row r="79" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="125"/>
       <c r="B79" s="125"/>
+      <c r="C79" s="125"/>
       <c r="D79" s="27"/>
       <c r="E79" s="27"/>
       <c r="F79" s="118"/>
@@ -29349,6 +29393,7 @@
     <row r="80" spans="1:42" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="125"/>
       <c r="B80" s="125"/>
+      <c r="C80" s="125"/>
       <c r="D80" s="27"/>
       <c r="E80" s="27"/>
       <c r="F80" s="118"/>
@@ -52196,6 +52241,44 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="Q9:Q12"/>
+    <mergeCell ref="R9:R12"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="T9:T12"/>
+    <mergeCell ref="U9:U12"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="S13:S16"/>
+    <mergeCell ref="T13:T16"/>
+    <mergeCell ref="U13:U16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="R17:R20"/>
+    <mergeCell ref="S17:S20"/>
+    <mergeCell ref="T17:T20"/>
+    <mergeCell ref="Q17:Q20"/>
+    <mergeCell ref="U17:U20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="M17:M20"/>
+    <mergeCell ref="N17:N20"/>
+    <mergeCell ref="O17:O20"/>
+    <mergeCell ref="P17:P20"/>
     <mergeCell ref="Q40:Y40"/>
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="J40:M40"/>
@@ -52210,44 +52293,6 @@
     <mergeCell ref="R21:R24"/>
     <mergeCell ref="S21:S24"/>
     <mergeCell ref="T21:T24"/>
-    <mergeCell ref="U17:U20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="M17:M20"/>
-    <mergeCell ref="N17:N20"/>
-    <mergeCell ref="O17:O20"/>
-    <mergeCell ref="P17:P20"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="R17:R20"/>
-    <mergeCell ref="S17:S20"/>
-    <mergeCell ref="T17:T20"/>
-    <mergeCell ref="Q17:Q20"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="R9:R12"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="T9:T12"/>
-    <mergeCell ref="U9:U12"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="S13:S16"/>
-    <mergeCell ref="T13:T16"/>
-    <mergeCell ref="U13:U16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="P9:P12"/>
-    <mergeCell ref="Q9:Q12"/>
   </mergeCells>
   <conditionalFormatting sqref="AM1:AM57 AM622:AM1048576">
     <cfRule type="duplicateValues" dxfId="46" priority="47"/>
@@ -52876,10 +52921,10 @@
         <v>45</v>
       </c>
       <c r="F6" s="159" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" s="159" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="159" t="s">
         <v>46</v>
@@ -52890,7 +52935,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="245" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="251" t="s">
         <v>47</v>
@@ -52900,7 +52945,7 @@
       </c>
       <c r="E7" s="192"/>
       <c r="F7" s="192" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G7" s="192"/>
       <c r="H7" s="197"/>
@@ -52915,10 +52960,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="192" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F8" s="192" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="192"/>
       <c r="H8" s="198"/>
@@ -52933,7 +52978,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="192" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F9" s="192">
         <v>75</v>
@@ -52951,10 +52996,10 @@
         <v>51</v>
       </c>
       <c r="E10" s="192" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" s="192" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G10" s="192"/>
       <c r="H10" s="200"/>
@@ -52966,10 +53011,10 @@
       <c r="B11" s="246"/>
       <c r="C11" s="251"/>
       <c r="D11" s="192" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" s="192" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11" s="192"/>
       <c r="G11" s="192"/>
@@ -52981,7 +53026,7 @@
       </c>
       <c r="B12" s="246"/>
       <c r="C12" s="194" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D12" s="192"/>
       <c r="E12" s="192"/>
@@ -52995,13 +53040,13 @@
       </c>
       <c r="B13" s="246"/>
       <c r="C13" s="194" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D13" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E13" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F13" s="192">
         <v>25</v>
@@ -53015,13 +53060,13 @@
       </c>
       <c r="B14" s="246"/>
       <c r="C14" s="194" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D14" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F14" s="192">
         <v>25</v>
@@ -53035,11 +53080,11 @@
       </c>
       <c r="B15" s="246"/>
       <c r="C15" s="194" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D15" s="192"/>
       <c r="E15" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F15" s="192">
         <v>75</v>
@@ -53060,7 +53105,7 @@
       </c>
       <c r="E16" s="192"/>
       <c r="F16" s="201" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G16" s="192"/>
       <c r="H16" s="192"/>
@@ -53072,11 +53117,11 @@
       <c r="B17" s="246"/>
       <c r="C17" s="256"/>
       <c r="D17" s="192" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" s="192"/>
       <c r="F17" s="201" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="192"/>
       <c r="H17" s="192"/>
@@ -53104,10 +53149,10 @@
       <c r="B19" s="246"/>
       <c r="C19" s="256"/>
       <c r="D19" s="192" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E19" s="192" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F19" s="192"/>
       <c r="G19" s="192"/>
@@ -53120,10 +53165,10 @@
       <c r="B20" s="246"/>
       <c r="C20" s="256"/>
       <c r="D20" s="192" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E20" s="192" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" s="192">
         <v>123</v>
@@ -53138,10 +53183,10 @@
       <c r="B21" s="246"/>
       <c r="C21" s="257"/>
       <c r="D21" s="202" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E21" s="192" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F21" s="192">
         <v>1.23</v>
@@ -53155,13 +53200,13 @@
       </c>
       <c r="B22" s="246"/>
       <c r="C22" s="194" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D22" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E22" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F22" s="192">
         <v>75</v>
@@ -53175,14 +53220,14 @@
       </c>
       <c r="B23" s="246"/>
       <c r="C23" s="194" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D23" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="192"/>
       <c r="F23" s="192" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G23" s="192"/>
       <c r="H23" s="192"/>
@@ -53193,14 +53238,14 @@
       </c>
       <c r="B24" s="246"/>
       <c r="C24" s="248" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D24" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="192"/>
       <c r="F24" s="193" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G24" s="192"/>
       <c r="H24" s="192"/>
@@ -53212,11 +53257,11 @@
       <c r="B25" s="246"/>
       <c r="C25" s="249"/>
       <c r="D25" s="192" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="192"/>
       <c r="F25" s="193" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G25" s="192"/>
       <c r="H25" s="192"/>
@@ -53244,10 +53289,10 @@
       <c r="B27" s="246"/>
       <c r="C27" s="249"/>
       <c r="D27" s="192" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E27" s="192" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F27" s="192"/>
       <c r="G27" s="192"/>
@@ -53260,10 +53305,10 @@
       <c r="B28" s="246"/>
       <c r="C28" s="249"/>
       <c r="D28" s="192" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E28" s="192" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F28" s="192">
         <v>123</v>
@@ -53278,10 +53323,10 @@
       <c r="B29" s="246"/>
       <c r="C29" s="250"/>
       <c r="D29" s="202" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E29" s="192" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F29" s="192">
         <v>1.23</v>
@@ -53295,7 +53340,7 @@
       </c>
       <c r="B30" s="246"/>
       <c r="C30" s="194" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D30" s="202"/>
       <c r="E30" s="192"/>
@@ -53309,7 +53354,7 @@
       </c>
       <c r="B31" s="246"/>
       <c r="C31" s="194" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" s="192"/>
       <c r="E31" s="192"/>
@@ -53323,14 +53368,14 @@
       </c>
       <c r="B32" s="246"/>
       <c r="C32" s="252" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D32" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="192"/>
       <c r="F32" s="192" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G32" s="192"/>
       <c r="H32" s="192"/>
@@ -53342,11 +53387,11 @@
       <c r="B33" s="246"/>
       <c r="C33" s="254"/>
       <c r="D33" s="192" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E33" s="192"/>
       <c r="F33" s="201" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G33" s="192"/>
       <c r="H33" s="192"/>
@@ -53374,10 +53419,10 @@
       <c r="B35" s="246"/>
       <c r="C35" s="254"/>
       <c r="D35" s="192" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E35" s="192" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F35" s="192"/>
       <c r="G35" s="192"/>
@@ -53390,10 +53435,10 @@
       <c r="B36" s="246"/>
       <c r="C36" s="254"/>
       <c r="D36" s="192" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E36" s="192" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36" s="192">
         <v>123</v>
@@ -53408,10 +53453,10 @@
       <c r="B37" s="246"/>
       <c r="C37" s="253"/>
       <c r="D37" s="202" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E37" s="192" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F37" s="192">
         <v>1.23</v>
@@ -53425,13 +53470,13 @@
       </c>
       <c r="B38" s="246"/>
       <c r="C38" s="196" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D38" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E38" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F38" s="192">
         <v>25</v>
@@ -53445,7 +53490,7 @@
       </c>
       <c r="B39" s="246"/>
       <c r="C39" s="196" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D39" s="192"/>
       <c r="E39" s="192"/>
@@ -53459,14 +53504,14 @@
       </c>
       <c r="B40" s="246"/>
       <c r="C40" s="252" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E40" s="192"/>
       <c r="F40" s="201" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G40" s="192"/>
       <c r="H40" s="192"/>
@@ -53478,7 +53523,7 @@
       <c r="B41" s="246"/>
       <c r="C41" s="253"/>
       <c r="D41" s="192" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E41" s="192"/>
       <c r="F41" s="192"/>
@@ -53491,13 +53536,13 @@
       </c>
       <c r="B42" s="246"/>
       <c r="C42" s="196" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D42" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E42" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F42" s="192">
         <v>75</v>
@@ -53511,10 +53556,10 @@
       </c>
       <c r="B43" s="246"/>
       <c r="C43" s="196" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D43" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E43" s="192"/>
       <c r="F43" s="192"/>
@@ -53551,7 +53596,7 @@
       </c>
       <c r="B46" s="246"/>
       <c r="C46" s="258" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" s="258"/>
       <c r="E46" s="258"/>
@@ -53565,14 +53610,14 @@
       </c>
       <c r="B47" s="246"/>
       <c r="C47" s="194" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D47" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E47" s="192"/>
       <c r="F47" s="193" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G47" s="192"/>
       <c r="H47" s="192"/>
@@ -53583,13 +53628,13 @@
       </c>
       <c r="B48" s="246"/>
       <c r="C48" s="194" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" s="192" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E48" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F48" s="192">
         <v>15</v>
@@ -53615,7 +53660,7 @@
       </c>
       <c r="B50" s="246"/>
       <c r="C50" s="258" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D50" s="259"/>
       <c r="E50" s="259"/>
@@ -53629,14 +53674,14 @@
       </c>
       <c r="B51" s="246"/>
       <c r="C51" s="194" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D51" s="192" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E51" s="192"/>
       <c r="F51" s="193" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G51" s="203"/>
       <c r="H51" s="192"/>
@@ -53648,11 +53693,11 @@
       <c r="B52" s="246"/>
       <c r="C52" s="194"/>
       <c r="D52" s="192" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E52" s="192"/>
       <c r="F52" s="193" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G52" s="203"/>
       <c r="H52" s="192"/>
@@ -53664,10 +53709,10 @@
       <c r="B53" s="246"/>
       <c r="C53" s="194"/>
       <c r="D53" s="192" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E53" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F53" s="193">
         <v>25</v>
@@ -53682,11 +53727,11 @@
       <c r="B54" s="246"/>
       <c r="C54" s="194"/>
       <c r="D54" s="192" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E54" s="192"/>
       <c r="F54" s="193" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G54" s="203"/>
       <c r="H54" s="192"/>
@@ -53709,7 +53754,7 @@
       </c>
       <c r="B56" s="246"/>
       <c r="C56" s="258" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D56" s="259"/>
       <c r="E56" s="259"/>
@@ -53723,14 +53768,14 @@
       </c>
       <c r="B57" s="246"/>
       <c r="C57" s="248" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D57" s="192" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E57" s="192"/>
       <c r="F57" s="193" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G57" s="192"/>
       <c r="H57" s="192"/>
@@ -53742,11 +53787,11 @@
       <c r="B58" s="246"/>
       <c r="C58" s="249"/>
       <c r="D58" s="192" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E58" s="192"/>
       <c r="F58" s="201" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G58" s="192"/>
       <c r="H58" s="192"/>
@@ -53758,10 +53803,10 @@
       <c r="B59" s="246"/>
       <c r="C59" s="250"/>
       <c r="D59" s="192" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E59" s="193" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F59" s="192">
         <v>25</v>
@@ -53775,14 +53820,14 @@
       </c>
       <c r="B60" s="246"/>
       <c r="C60" s="248" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D60" s="192" t="s">
         <v>48</v>
       </c>
       <c r="E60" s="192"/>
       <c r="F60" s="192" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G60" s="192"/>
       <c r="H60" s="192"/>
@@ -53794,11 +53839,11 @@
       <c r="B61" s="246"/>
       <c r="C61" s="249"/>
       <c r="D61" s="192" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E61" s="192"/>
       <c r="F61" s="192" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G61" s="192"/>
       <c r="H61" s="192"/>
@@ -53826,10 +53871,10 @@
       <c r="B63" s="246"/>
       <c r="C63" s="249"/>
       <c r="D63" s="192" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E63" s="192" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F63" s="192"/>
       <c r="G63" s="192"/>
@@ -53842,10 +53887,10 @@
       <c r="B64" s="246"/>
       <c r="C64" s="249"/>
       <c r="D64" s="192" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E64" s="192" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F64" s="192">
         <v>123</v>
@@ -53860,10 +53905,10 @@
       <c r="B65" s="246"/>
       <c r="C65" s="250"/>
       <c r="D65" s="202" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E65" s="192" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F65" s="192">
         <v>1.23</v>
@@ -53877,14 +53922,14 @@
       </c>
       <c r="B66" s="246"/>
       <c r="C66" s="194" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D66" s="192" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E66" s="192"/>
       <c r="F66" s="201" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G66" s="192"/>
       <c r="H66" s="192"/>
@@ -53907,12 +53952,12 @@
       </c>
       <c r="B68" s="247"/>
       <c r="C68" s="195" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D68" s="192"/>
       <c r="E68" s="192"/>
       <c r="F68" s="192" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G68" s="192"/>
       <c r="H68" s="192"/>
@@ -54000,10 +54045,10 @@
         <v>45</v>
       </c>
       <c r="F6" s="159" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" s="159" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="159" t="s">
         <v>46</v>
@@ -54014,7 +54059,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="245" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="261" t="s">
         <v>47</v>
@@ -54024,7 +54069,7 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="176"/>
@@ -54039,10 +54084,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="177"/>
@@ -54057,7 +54102,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F9" s="178">
         <v>75</v>
@@ -54075,10 +54120,10 @@
         <v>51</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="180"/>
@@ -54090,10 +54135,10 @@
       <c r="B11" s="246"/>
       <c r="C11" s="261"/>
       <c r="D11" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -54105,14 +54150,14 @@
       </c>
       <c r="B12" s="246"/>
       <c r="C12" s="186" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -54123,14 +54168,14 @@
       </c>
       <c r="B13" s="246"/>
       <c r="C13" s="186" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="182"/>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -54142,11 +54187,11 @@
       <c r="B14" s="246"/>
       <c r="C14" s="186"/>
       <c r="D14" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -54157,14 +54202,14 @@
       </c>
       <c r="B15" s="246"/>
       <c r="C15" s="186" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E15" s="182"/>
       <c r="F15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -54175,14 +54220,14 @@
       </c>
       <c r="B16" s="246"/>
       <c r="C16" s="211" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="71" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -54193,14 +54238,14 @@
       </c>
       <c r="B17" s="246"/>
       <c r="C17" s="213" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
@@ -54211,13 +54256,13 @@
       </c>
       <c r="B18" s="246"/>
       <c r="C18" s="212" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F18">
         <v>50</v>
@@ -54231,14 +54276,14 @@
       </c>
       <c r="B19" s="246"/>
       <c r="C19" s="214" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -54249,12 +54294,12 @@
       </c>
       <c r="B20" s="246"/>
       <c r="C20" s="215" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -54564,7 +54609,7 @@
       </c>
       <c r="B46" s="246"/>
       <c r="C46" s="258" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" s="258"/>
       <c r="E46" s="258"/>
@@ -54578,14 +54623,14 @@
       </c>
       <c r="B47" s="246"/>
       <c r="C47" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
@@ -54596,13 +54641,13 @@
       </c>
       <c r="B48" s="246"/>
       <c r="C48" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E48" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F48" s="12">
         <v>15</v>
@@ -54628,7 +54673,7 @@
       </c>
       <c r="B50" s="246"/>
       <c r="C50" s="259" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D50" s="259"/>
       <c r="E50" s="259"/>
@@ -54642,14 +54687,14 @@
       </c>
       <c r="B51" s="246"/>
       <c r="C51" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G51" s="184"/>
       <c r="H51" s="12"/>
@@ -54661,11 +54706,11 @@
       <c r="B52" s="246"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G52" s="184"/>
       <c r="H52" s="12"/>
@@ -54677,10 +54722,10 @@
       <c r="B53" s="246"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E53" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F53" s="1">
         <v>25</v>
@@ -54695,11 +54740,11 @@
       <c r="B54" s="246"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G54" s="184"/>
       <c r="H54" s="12"/>
@@ -54722,7 +54767,7 @@
       </c>
       <c r="B56" s="246"/>
       <c r="C56" s="259" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D56" s="259"/>
       <c r="E56" s="259"/>
@@ -54736,14 +54781,14 @@
       </c>
       <c r="B57" s="246"/>
       <c r="C57" s="248" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -54755,11 +54800,11 @@
       <c r="B58" s="246"/>
       <c r="C58" s="249"/>
       <c r="D58" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
@@ -54771,10 +54816,10 @@
       <c r="B59" s="246"/>
       <c r="C59" s="250"/>
       <c r="D59" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E59" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F59" s="12">
         <v>25</v>
@@ -54788,14 +54833,14 @@
       </c>
       <c r="B60" s="246"/>
       <c r="C60" s="248" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -54807,11 +54852,11 @@
       <c r="B61" s="246"/>
       <c r="C61" s="249"/>
       <c r="D61" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E61" s="12"/>
       <c r="F61" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
@@ -54839,10 +54884,10 @@
       <c r="B63" s="246"/>
       <c r="C63" s="249"/>
       <c r="D63" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
@@ -54855,10 +54900,10 @@
       <c r="B64" s="246"/>
       <c r="C64" s="249"/>
       <c r="D64" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F64" s="12">
         <v>123</v>
@@ -54873,10 +54918,10 @@
       <c r="B65" s="246"/>
       <c r="C65" s="250"/>
       <c r="D65" s="181" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F65" s="12">
         <v>1.23</v>
@@ -54890,14 +54935,14 @@
       </c>
       <c r="B66" s="246"/>
       <c r="C66" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E66" s="12"/>
       <c r="F66" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
@@ -54920,12 +54965,12 @@
       </c>
       <c r="B68" s="247"/>
       <c r="C68" s="185" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
@@ -55012,10 +55057,10 @@
         <v>45</v>
       </c>
       <c r="F6" s="159" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" s="159" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="159" t="s">
         <v>46</v>
@@ -55026,7 +55071,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="245" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="261" t="s">
         <v>47</v>
@@ -55036,7 +55081,7 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="176"/>
@@ -55051,10 +55096,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="177"/>
@@ -55069,7 +55114,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F9" s="178">
         <v>75</v>
@@ -55087,10 +55132,10 @@
         <v>51</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="180"/>
@@ -55102,10 +55147,10 @@
       <c r="B11" s="246"/>
       <c r="C11" s="261"/>
       <c r="D11" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -55117,14 +55162,14 @@
       </c>
       <c r="B12" s="246"/>
       <c r="C12" s="190" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="182"/>
       <c r="F12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -55136,11 +55181,11 @@
       <c r="B13" s="246"/>
       <c r="C13" s="190"/>
       <c r="D13" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E13" s="182"/>
       <c r="F13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -55151,14 +55196,14 @@
       </c>
       <c r="B14" s="246"/>
       <c r="C14" s="190" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -55169,14 +55214,14 @@
       </c>
       <c r="B15" s="246"/>
       <c r="C15" s="187" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -55187,14 +55232,14 @@
       </c>
       <c r="B16" s="246"/>
       <c r="C16" s="268" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -55206,10 +55251,10 @@
       <c r="B17" s="246"/>
       <c r="C17" s="268"/>
       <c r="D17" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F17" s="178">
         <v>15</v>
@@ -55223,13 +55268,13 @@
       </c>
       <c r="B18" s="246"/>
       <c r="C18" s="191" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F18" s="178">
         <v>75</v>
@@ -55243,14 +55288,14 @@
       </c>
       <c r="B19" s="246"/>
       <c r="C19" s="188" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -55560,7 +55605,7 @@
       </c>
       <c r="B45" s="246"/>
       <c r="C45" s="258" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D45" s="258"/>
       <c r="E45" s="258"/>
@@ -55574,14 +55619,14 @@
       </c>
       <c r="B46" s="246"/>
       <c r="C46" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -55592,13 +55637,13 @@
       </c>
       <c r="B47" s="246"/>
       <c r="C47" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E47" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F47" s="12">
         <v>15</v>
@@ -55624,7 +55669,7 @@
       </c>
       <c r="B49" s="246"/>
       <c r="C49" s="259" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D49" s="259"/>
       <c r="E49" s="259"/>
@@ -55638,14 +55683,14 @@
       </c>
       <c r="B50" s="246"/>
       <c r="C50" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G50" s="184"/>
       <c r="H50" s="12"/>
@@ -55657,11 +55702,11 @@
       <c r="B51" s="246"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G51" s="184"/>
       <c r="H51" s="12"/>
@@ -55673,10 +55718,10 @@
       <c r="B52" s="246"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E52" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F52" s="1">
         <v>25</v>
@@ -55691,11 +55736,11 @@
       <c r="B53" s="246"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G53" s="184"/>
       <c r="H53" s="12"/>
@@ -55718,7 +55763,7 @@
       </c>
       <c r="B55" s="246"/>
       <c r="C55" s="259" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D55" s="259"/>
       <c r="E55" s="259"/>
@@ -55732,14 +55777,14 @@
       </c>
       <c r="B56" s="246"/>
       <c r="C56" s="248" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
@@ -55751,11 +55796,11 @@
       <c r="B57" s="246"/>
       <c r="C57" s="249"/>
       <c r="D57" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
@@ -55767,10 +55812,10 @@
       <c r="B58" s="246"/>
       <c r="C58" s="250"/>
       <c r="D58" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E58" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F58" s="12">
         <v>25</v>
@@ -55784,14 +55829,14 @@
       </c>
       <c r="B59" s="246"/>
       <c r="C59" s="248" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
@@ -55803,11 +55848,11 @@
       <c r="B60" s="246"/>
       <c r="C60" s="249"/>
       <c r="D60" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
@@ -55835,10 +55880,10 @@
       <c r="B62" s="246"/>
       <c r="C62" s="249"/>
       <c r="D62" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
@@ -55851,10 +55896,10 @@
       <c r="B63" s="246"/>
       <c r="C63" s="249"/>
       <c r="D63" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F63" s="12">
         <v>123</v>
@@ -55869,10 +55914,10 @@
       <c r="B64" s="246"/>
       <c r="C64" s="250"/>
       <c r="D64" s="181" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F64" s="12">
         <v>1.23</v>
@@ -55886,14 +55931,14 @@
       </c>
       <c r="B65" s="246"/>
       <c r="C65" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E65" s="12"/>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
@@ -55916,12 +55961,12 @@
       </c>
       <c r="B67" s="247"/>
       <c r="C67" s="185" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>

</xml_diff>